<commit_message>
Finished treasure island problem
</commit_message>
<xml_diff>
--- a/LeetCode.xlsx
+++ b/LeetCode.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\EricS\Documents\VSCode Projects\LeetcodeGrind\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{47B2F0A6-7B38-457E-8B3A-6AA6A0CAC0DA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{84771D6C-EFF6-4F4E-B732-15880E80D0AF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="3" xr2:uid="{02D29AA1-7085-42F6-B3D4-4C0365DA5453}"/>
   </bookViews>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="547" uniqueCount="382">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="551" uniqueCount="385">
   <si>
     <t>Roman to Integer:</t>
   </si>
@@ -1187,6 +1187,15 @@
   </si>
   <si>
     <t>just same thing as prev problem but have number to keep track of size, adding 1 if 1 and then adding recursive call on neighbors, 0 if 0</t>
+  </si>
+  <si>
+    <t>just have dictionary going from old to cloned nodes, adding each neighbor using recursion, base cases of returning null or dictionary version</t>
+  </si>
+  <si>
+    <t>fill grid with shortest distance to treasure given walls in certain blocks</t>
+  </si>
+  <si>
+    <t>run dfs on each treasure and update neighbors until smaller value encountered</t>
   </si>
 </sst>
 </file>
@@ -2248,7 +2257,7 @@
   <dimension ref="A1:G967"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B79" zoomScale="90" zoomScaleNormal="122" workbookViewId="0">
-      <selection activeCell="D83" sqref="D83"/>
+      <selection activeCell="D85" sqref="D85"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3569,26 +3578,34 @@
       </c>
       <c r="F82" s="3"/>
     </row>
-    <row r="83" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="B83" s="4" t="s">
         <v>341</v>
       </c>
       <c r="C83" s="4" t="s">
         <v>119</v>
       </c>
-      <c r="D83" s="3"/>
-      <c r="E83" s="3"/>
+      <c r="D83" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="E83" s="3" t="s">
+        <v>382</v>
+      </c>
       <c r="F83" s="3"/>
     </row>
-    <row r="84" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="B84" s="4" t="s">
         <v>342</v>
       </c>
       <c r="C84" s="4" t="s">
         <v>119</v>
       </c>
-      <c r="D84" s="3"/>
-      <c r="E84" s="3"/>
+      <c r="D84" s="3" t="s">
+        <v>383</v>
+      </c>
+      <c r="E84" s="3" t="s">
+        <v>384</v>
+      </c>
       <c r="F84" s="3"/>
     </row>
     <row r="85" spans="1:6" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Finished rotting fruit problem
</commit_message>
<xml_diff>
--- a/LeetCode.xlsx
+++ b/LeetCode.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\EricS\Documents\VSCode Projects\LeetcodeGrind\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{84771D6C-EFF6-4F4E-B732-15880E80D0AF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{92EDFCF6-FEEB-4C27-9B81-065F5FB0E444}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="3" xr2:uid="{02D29AA1-7085-42F6-B3D4-4C0365DA5453}"/>
   </bookViews>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="551" uniqueCount="385">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="963" uniqueCount="387">
   <si>
     <t>Roman to Integer:</t>
   </si>
@@ -1196,6 +1196,12 @@
   </si>
   <si>
     <t>run dfs on each treasure and update neighbors until smaller value encountered</t>
+  </si>
+  <si>
+    <t>rotting oranges infect neighboring oranges, how long does it take for all oranges to be infected, -1 if not possible</t>
+  </si>
+  <si>
+    <t>literally count clean oranges and get all locations of rotten, then go through queue and expand one step out each time, putting all valid back into queue, keep track of time separately as well</t>
   </si>
 </sst>
 </file>
@@ -2257,7 +2263,7 @@
   <dimension ref="A1:G967"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B79" zoomScale="90" zoomScaleNormal="122" workbookViewId="0">
-      <selection activeCell="D85" sqref="D85"/>
+      <selection activeCell="E86" sqref="E86"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3608,15 +3614,19 @@
       </c>
       <c r="F84" s="3"/>
     </row>
-    <row r="85" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:6" ht="45" x14ac:dyDescent="0.25">
       <c r="B85" s="4" t="s">
         <v>343</v>
       </c>
       <c r="C85" s="4" t="s">
         <v>119</v>
       </c>
-      <c r="D85" s="3"/>
-      <c r="E85" s="3"/>
+      <c r="D85" s="3" t="s">
+        <v>385</v>
+      </c>
+      <c r="E85" s="3" t="s">
+        <v>386</v>
+      </c>
       <c r="F85" s="3"/>
     </row>
     <row r="86" spans="1:6" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Finished surround region problem
</commit_message>
<xml_diff>
--- a/LeetCode.xlsx
+++ b/LeetCode.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\EricS\Documents\VSCode Projects\LeetcodeGrind\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{92EDFCF6-FEEB-4C27-9B81-065F5FB0E444}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D759DEA9-F5A9-4994-9C83-2F710D942F94}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="3" xr2:uid="{02D29AA1-7085-42F6-B3D4-4C0365DA5453}"/>
   </bookViews>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="963" uniqueCount="387">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="555" uniqueCount="389">
   <si>
     <t>Roman to Integer:</t>
   </si>
@@ -1202,6 +1202,12 @@
   </si>
   <si>
     <t>literally count clean oranges and get all locations of rotten, then go through queue and expand one step out each time, putting all valid back into queue, keep track of time separately as well</t>
+  </si>
+  <si>
+    <t>go from edges and floodfill to see which are connected to edges, then replace everything with "X" if not connected to edge</t>
+  </si>
+  <si>
+    <t>change all surrounded islands of "O" to "X"</t>
   </si>
 </sst>
 </file>
@@ -2263,7 +2269,7 @@
   <dimension ref="A1:G967"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B79" zoomScale="90" zoomScaleNormal="122" workbookViewId="0">
-      <selection activeCell="E86" sqref="E86"/>
+      <selection activeCell="E87" sqref="E87"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3640,15 +3646,19 @@
       <c r="E86" s="3"/>
       <c r="F86" s="3"/>
     </row>
-    <row r="87" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="B87" s="4" t="s">
         <v>345</v>
       </c>
       <c r="C87" s="4" t="s">
         <v>119</v>
       </c>
-      <c r="D87" s="3"/>
-      <c r="E87" s="3"/>
+      <c r="D87" s="3" t="s">
+        <v>388</v>
+      </c>
+      <c r="E87" s="3" t="s">
+        <v>387</v>
+      </c>
       <c r="F87" s="3"/>
     </row>
     <row r="88" spans="1:6" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Finished course sched problem
</commit_message>
<xml_diff>
--- a/LeetCode.xlsx
+++ b/LeetCode.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\EricS\Documents\VSCode Projects\LeetcodeGrind\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{84614FD7-F28F-4545-868F-D7EB13F927F0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C0B5EC6A-8867-4592-8E03-29F492BB891E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="3120" yWindow="3120" windowWidth="21600" windowHeight="11295" activeTab="3" xr2:uid="{02D29AA1-7085-42F6-B3D4-4C0365DA5453}"/>
   </bookViews>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="557" uniqueCount="391">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="560" uniqueCount="394">
   <si>
     <t>Roman to Integer:</t>
   </si>
@@ -1214,6 +1214,15 @@
   </si>
   <si>
     <t>go from edges and floodfill to see which are connected to edges, then track pacific and atlantic individually, in the end loop through to see which spots reach both</t>
+  </si>
+  <si>
+    <t>given pairs of pre-reqs, figure out if all courses can be taken</t>
+  </si>
+  <si>
+    <t>create graph based on pre reqs, use topological sort to figure out if possible, aka track indegree/# of pre reqs for each course, then start all courses with no pre reqs, make all their children nodes -= 1 indegree and add them to queue if now all their pre-reqs are satisfied, continue until queue is empty and check if # of courses that were satisfied is equal to total num of courses</t>
+  </si>
+  <si>
+    <t>&lt;- Kahn's algorithm</t>
   </si>
 </sst>
 </file>
@@ -2274,8 +2283,8 @@
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:G967"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B80" zoomScale="90" zoomScaleNormal="122" workbookViewId="0">
-      <selection activeCell="D88" sqref="D88"/>
+    <sheetView tabSelected="1" topLeftCell="C85" zoomScale="90" zoomScaleNormal="122" workbookViewId="0">
+      <selection activeCell="F89" sqref="F89"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3671,16 +3680,22 @@
       </c>
       <c r="F87" s="3"/>
     </row>
-    <row r="88" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:6" ht="75" x14ac:dyDescent="0.25">
       <c r="B88" s="4" t="s">
         <v>346</v>
       </c>
       <c r="C88" s="4" t="s">
         <v>119</v>
       </c>
-      <c r="D88" s="3"/>
-      <c r="E88" s="3"/>
-      <c r="F88" s="3"/>
+      <c r="D88" s="3" t="s">
+        <v>391</v>
+      </c>
+      <c r="E88" s="3" t="s">
+        <v>392</v>
+      </c>
+      <c r="F88" s="3" t="s">
+        <v>393</v>
+      </c>
     </row>
     <row r="89" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B89" s="4" t="s">

</xml_diff>

<commit_message>
Finished course schedule 2
</commit_message>
<xml_diff>
--- a/LeetCode.xlsx
+++ b/LeetCode.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\EricS\Documents\VSCode Projects\LeetcodeGrind\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C0B5EC6A-8867-4592-8E03-29F492BB891E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C3C8BD16-9299-468B-A31C-EBA94BF8C0F8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3120" yWindow="3120" windowWidth="21600" windowHeight="11295" activeTab="3" xr2:uid="{02D29AA1-7085-42F6-B3D4-4C0365DA5453}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="3" xr2:uid="{02D29AA1-7085-42F6-B3D4-4C0365DA5453}"/>
   </bookViews>
   <sheets>
     <sheet name="Easy" sheetId="1" r:id="rId1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="560" uniqueCount="394">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="562" uniqueCount="396">
   <si>
     <t>Roman to Integer:</t>
   </si>
@@ -1223,6 +1223,12 @@
   </si>
   <si>
     <t>&lt;- Kahn's algorithm</t>
+  </si>
+  <si>
+    <t>same thing but return a valid order or empty list ^</t>
+  </si>
+  <si>
+    <t>same thing using Kahn's algorithm, instead of adding ret as counter add courses to ret as they are processed with indegree 0</t>
   </si>
 </sst>
 </file>
@@ -2283,8 +2289,8 @@
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:G967"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C85" zoomScale="90" zoomScaleNormal="122" workbookViewId="0">
-      <selection activeCell="F89" sqref="F89"/>
+    <sheetView tabSelected="1" topLeftCell="A85" zoomScale="90" zoomScaleNormal="122" workbookViewId="0">
+      <selection activeCell="D90" sqref="D90"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3697,15 +3703,19 @@
         <v>393</v>
       </c>
     </row>
-    <row r="89" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="B89" s="4" t="s">
         <v>347</v>
       </c>
       <c r="C89" s="4" t="s">
         <v>119</v>
       </c>
-      <c r="D89" s="3"/>
-      <c r="E89" s="3"/>
+      <c r="D89" s="3" t="s">
+        <v>394</v>
+      </c>
+      <c r="E89" s="3" t="s">
+        <v>395</v>
+      </c>
       <c r="F89" s="3"/>
     </row>
     <row r="90" spans="1:6" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Finished word ladder and graph problems
</commit_message>
<xml_diff>
--- a/LeetCode.xlsx
+++ b/LeetCode.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\EricS\Documents\VSCode Projects\LeetcodeGrind\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{80A67E10-B0AF-48CD-BC01-DB97B9FBD625}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AA8D32E7-ADC1-482E-8793-D135AB28975B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="3" xr2:uid="{02D29AA1-7085-42F6-B3D4-4C0365DA5453}"/>
   </bookViews>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="568" uniqueCount="401">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="593" uniqueCount="415">
   <si>
     <t>Roman to Integer:</t>
   </si>
@@ -1244,6 +1244,48 @@
   </si>
   <si>
     <t>union find method, return edge where a and b are the same after calling find since that means they are already connected and there's therefore a loop</t>
+  </si>
+  <si>
+    <t>go from start word to end word only going through words in word list only changing one letter at a time</t>
+  </si>
+  <si>
+    <t>first method is to construct graph using *ord w*rd wo*d wor* and doing BFS, better way is to check every possible other letter in each spot after converting word list into a set and removing when visited, even better is to do that while doing a double ended BFS, going on the end that has a smaller queue</t>
+  </si>
+  <si>
+    <t>2D DP</t>
+  </si>
+  <si>
+    <t>Regular Expression Matching</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Unique Paths   </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Longest Common Subsequence   </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Best Time to Buy And Sell Stock With Cooldown   </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Coin Change II   </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Target Sum   </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Interleaving String   </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Longest Increasing Path In a Matrix   </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Distinct Subsequences   </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Edit Distance   </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Burst Balloons   </t>
   </si>
 </sst>
 </file>
@@ -2304,8 +2346,8 @@
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:G967"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A85" zoomScale="90" zoomScaleNormal="122" workbookViewId="0">
-      <selection activeCell="D93" sqref="D93"/>
+    <sheetView tabSelected="1" topLeftCell="A91" zoomScale="90" zoomScaleNormal="122" workbookViewId="0">
+      <selection activeCell="D115" sqref="D115"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3778,15 +3820,19 @@
       </c>
       <c r="F92" s="3"/>
     </row>
-    <row r="93" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:6" ht="75" x14ac:dyDescent="0.25">
       <c r="B93" s="4" t="s">
         <v>351</v>
       </c>
       <c r="C93" s="4" t="s">
         <v>142</v>
       </c>
-      <c r="D93" s="3"/>
-      <c r="E93" s="3"/>
+      <c r="D93" s="3" t="s">
+        <v>401</v>
+      </c>
+      <c r="E93" s="3" t="s">
+        <v>402</v>
+      </c>
       <c r="F93" s="3"/>
     </row>
     <row r="94" spans="1:6" x14ac:dyDescent="0.25">
@@ -3825,7 +3871,7 @@
       <c r="E96" s="3"/>
       <c r="F96" s="3"/>
     </row>
-    <row r="97" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B97" s="4" t="s">
         <v>356</v>
       </c>
@@ -3836,7 +3882,7 @@
       <c r="E97" s="3"/>
       <c r="F97" s="3"/>
     </row>
-    <row r="98" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B98" s="4" t="s">
         <v>357</v>
       </c>
@@ -3847,7 +3893,7 @@
       <c r="E98" s="3"/>
       <c r="F98" s="3"/>
     </row>
-    <row r="99" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B99" s="4" t="s">
         <v>358</v>
       </c>
@@ -3858,7 +3904,7 @@
       <c r="E99" s="3"/>
       <c r="F99" s="3"/>
     </row>
-    <row r="100" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B100" s="4" t="s">
         <v>359</v>
       </c>
@@ -3869,7 +3915,7 @@
       <c r="E100" s="3"/>
       <c r="F100" s="3"/>
     </row>
-    <row r="101" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B101" s="4" t="s">
         <v>360</v>
       </c>
@@ -3880,7 +3926,7 @@
       <c r="E101" s="3"/>
       <c r="F101" s="3"/>
     </row>
-    <row r="102" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B102" s="4" t="s">
         <v>361</v>
       </c>
@@ -3891,7 +3937,7 @@
       <c r="E102" s="3"/>
       <c r="F102" s="3"/>
     </row>
-    <row r="103" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B103" s="4" t="s">
         <v>362</v>
       </c>
@@ -3902,7 +3948,7 @@
       <c r="E103" s="3"/>
       <c r="F103" s="3"/>
     </row>
-    <row r="104" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B104" s="4" t="s">
         <v>363</v>
       </c>
@@ -3913,7 +3959,7 @@
       <c r="E104" s="3"/>
       <c r="F104" s="3"/>
     </row>
-    <row r="105" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B105" s="4" t="s">
         <v>364</v>
       </c>
@@ -3924,117 +3970,186 @@
       <c r="E105" s="3"/>
       <c r="F105" s="3"/>
     </row>
-    <row r="106" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A106" s="5" t="s">
+        <v>403</v>
+      </c>
+      <c r="B106" s="4" t="s">
+        <v>405</v>
+      </c>
+      <c r="C106" s="4" t="s">
+        <v>119</v>
+      </c>
       <c r="D106" s="3"/>
       <c r="E106" s="3"/>
       <c r="F106" s="3"/>
     </row>
-    <row r="107" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B107" s="4" t="s">
+        <v>406</v>
+      </c>
+      <c r="C107" s="4" t="s">
+        <v>119</v>
+      </c>
       <c r="D107" s="3"/>
       <c r="E107" s="3"/>
       <c r="F107" s="3"/>
     </row>
-    <row r="108" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B108" s="4" t="s">
+        <v>407</v>
+      </c>
+      <c r="C108" s="4" t="s">
+        <v>119</v>
+      </c>
       <c r="D108" s="3"/>
       <c r="E108" s="3"/>
       <c r="F108" s="3"/>
     </row>
-    <row r="109" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="109" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B109" s="4" t="s">
+        <v>408</v>
+      </c>
+      <c r="C109" s="4" t="s">
+        <v>119</v>
+      </c>
       <c r="D109" s="3"/>
       <c r="E109" s="3"/>
       <c r="F109" s="3"/>
     </row>
-    <row r="110" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="110" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B110" s="4" t="s">
+        <v>409</v>
+      </c>
+      <c r="C110" s="4" t="s">
+        <v>119</v>
+      </c>
       <c r="D110" s="3"/>
       <c r="E110" s="3"/>
       <c r="F110" s="3"/>
     </row>
-    <row r="111" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="111" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B111" s="4" t="s">
+        <v>410</v>
+      </c>
+      <c r="C111" s="4" t="s">
+        <v>119</v>
+      </c>
       <c r="D111" s="3"/>
       <c r="E111" s="3"/>
       <c r="F111" s="3"/>
     </row>
-    <row r="112" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="112" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B112" s="4" t="s">
+        <v>411</v>
+      </c>
+      <c r="C112" s="4" t="s">
+        <v>142</v>
+      </c>
       <c r="D112" s="3"/>
       <c r="E112" s="3"/>
       <c r="F112" s="3"/>
     </row>
-    <row r="113" spans="4:6" x14ac:dyDescent="0.25">
+    <row r="113" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B113" s="4" t="s">
+        <v>412</v>
+      </c>
+      <c r="C113" s="4" t="s">
+        <v>142</v>
+      </c>
       <c r="D113" s="3"/>
       <c r="E113" s="3"/>
       <c r="F113" s="3"/>
     </row>
-    <row r="114" spans="4:6" x14ac:dyDescent="0.25">
+    <row r="114" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B114" s="4" t="s">
+        <v>413</v>
+      </c>
+      <c r="C114" s="4" t="s">
+        <v>119</v>
+      </c>
       <c r="D114" s="3"/>
       <c r="E114" s="3"/>
       <c r="F114" s="3"/>
     </row>
-    <row r="115" spans="4:6" x14ac:dyDescent="0.25">
+    <row r="115" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B115" s="4" t="s">
+        <v>414</v>
+      </c>
+      <c r="C115" s="4" t="s">
+        <v>142</v>
+      </c>
       <c r="D115" s="3"/>
       <c r="E115" s="3"/>
       <c r="F115" s="3"/>
     </row>
-    <row r="116" spans="4:6" x14ac:dyDescent="0.25">
+    <row r="116" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B116" s="4" t="s">
+        <v>404</v>
+      </c>
+      <c r="C116" s="4" t="s">
+        <v>142</v>
+      </c>
       <c r="D116" s="3"/>
       <c r="E116" s="3"/>
       <c r="F116" s="3"/>
     </row>
-    <row r="117" spans="4:6" x14ac:dyDescent="0.25">
+    <row r="117" spans="2:6" x14ac:dyDescent="0.25">
       <c r="D117" s="3"/>
       <c r="E117" s="3"/>
       <c r="F117" s="3"/>
     </row>
-    <row r="118" spans="4:6" x14ac:dyDescent="0.25">
+    <row r="118" spans="2:6" x14ac:dyDescent="0.25">
       <c r="D118" s="3"/>
       <c r="E118" s="3"/>
       <c r="F118" s="3"/>
     </row>
-    <row r="119" spans="4:6" x14ac:dyDescent="0.25">
+    <row r="119" spans="2:6" x14ac:dyDescent="0.25">
       <c r="D119" s="3"/>
       <c r="E119" s="3"/>
       <c r="F119" s="3"/>
     </row>
-    <row r="120" spans="4:6" x14ac:dyDescent="0.25">
+    <row r="120" spans="2:6" x14ac:dyDescent="0.25">
       <c r="D120" s="3"/>
       <c r="E120" s="3"/>
       <c r="F120" s="3"/>
     </row>
-    <row r="121" spans="4:6" x14ac:dyDescent="0.25">
+    <row r="121" spans="2:6" x14ac:dyDescent="0.25">
       <c r="D121" s="3"/>
       <c r="E121" s="3"/>
       <c r="F121" s="3"/>
     </row>
-    <row r="122" spans="4:6" x14ac:dyDescent="0.25">
+    <row r="122" spans="2:6" x14ac:dyDescent="0.25">
       <c r="D122" s="3"/>
       <c r="E122" s="3"/>
       <c r="F122" s="3"/>
     </row>
-    <row r="123" spans="4:6" x14ac:dyDescent="0.25">
+    <row r="123" spans="2:6" x14ac:dyDescent="0.25">
       <c r="D123" s="3"/>
       <c r="E123" s="3"/>
       <c r="F123" s="3"/>
     </row>
-    <row r="124" spans="4:6" x14ac:dyDescent="0.25">
+    <row r="124" spans="2:6" x14ac:dyDescent="0.25">
       <c r="D124" s="3"/>
       <c r="E124" s="3"/>
       <c r="F124" s="3"/>
     </row>
-    <row r="125" spans="4:6" x14ac:dyDescent="0.25">
+    <row r="125" spans="2:6" x14ac:dyDescent="0.25">
       <c r="D125" s="3"/>
       <c r="E125" s="3"/>
       <c r="F125" s="3"/>
     </row>
-    <row r="126" spans="4:6" x14ac:dyDescent="0.25">
+    <row r="126" spans="2:6" x14ac:dyDescent="0.25">
       <c r="D126" s="3"/>
       <c r="E126" s="3"/>
       <c r="F126" s="3"/>
     </row>
-    <row r="127" spans="4:6" x14ac:dyDescent="0.25">
+    <row r="127" spans="2:6" x14ac:dyDescent="0.25">
       <c r="D127" s="3"/>
       <c r="E127" s="3"/>
       <c r="F127" s="3"/>
     </row>
-    <row r="128" spans="4:6" x14ac:dyDescent="0.25">
+    <row r="128" spans="2:6" x14ac:dyDescent="0.25">
       <c r="D128" s="3"/>
       <c r="E128" s="3"/>
       <c r="F128" s="3"/>

</xml_diff>

<commit_message>
Finished climbing stairs problem
</commit_message>
<xml_diff>
--- a/LeetCode.xlsx
+++ b/LeetCode.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\EricS\Documents\VSCode Projects\LeetcodeGrind\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AA8D32E7-ADC1-482E-8793-D135AB28975B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E1F2D886-FDA3-4E06-8CDD-0217A9E5E762}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="3" xr2:uid="{02D29AA1-7085-42F6-B3D4-4C0365DA5453}"/>
   </bookViews>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="593" uniqueCount="415">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="595" uniqueCount="417">
   <si>
     <t>Roman to Integer:</t>
   </si>
@@ -1286,6 +1286,12 @@
   </si>
   <si>
     <t xml:space="preserve">Burst Balloons   </t>
+  </si>
+  <si>
+    <t>number of ways to climb n stairs taking steps of size 1 or 2</t>
+  </si>
+  <si>
+    <t>make list len n + 1, make 0 and 1 both have 1 way, then each next step is one step down + 2 steps down, return last one</t>
   </si>
 </sst>
 </file>
@@ -2347,7 +2353,7 @@
   <dimension ref="A1:G967"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A91" zoomScale="90" zoomScaleNormal="122" workbookViewId="0">
-      <selection activeCell="D115" sqref="D115"/>
+      <selection activeCell="D95" sqref="D95"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3835,7 +3841,7 @@
       </c>
       <c r="F93" s="3"/>
     </row>
-    <row r="94" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A94" s="5" t="s">
         <v>352</v>
       </c>
@@ -3845,8 +3851,12 @@
       <c r="C94" s="4" t="s">
         <v>112</v>
       </c>
-      <c r="D94" s="3"/>
-      <c r="E94" s="3"/>
+      <c r="D94" s="3" t="s">
+        <v>415</v>
+      </c>
+      <c r="E94" s="3" t="s">
+        <v>416</v>
+      </c>
       <c r="F94" s="3"/>
     </row>
     <row r="95" spans="1:6" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Finished min cost climbing stairs
</commit_message>
<xml_diff>
--- a/LeetCode.xlsx
+++ b/LeetCode.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\EricS\Documents\VSCode Projects\LeetcodeGrind\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E1F2D886-FDA3-4E06-8CDD-0217A9E5E762}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{84106E4D-F186-4508-905A-4DE2762D51B8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="3" xr2:uid="{02D29AA1-7085-42F6-B3D4-4C0365DA5453}"/>
   </bookViews>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="595" uniqueCount="417">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1051" uniqueCount="419">
   <si>
     <t>Roman to Integer:</t>
   </si>
@@ -1292,6 +1292,12 @@
   </si>
   <si>
     <t>make list len n + 1, make 0 and 1 both have 1 way, then each next step is one step down + 2 steps down, return last one</t>
+  </si>
+  <si>
+    <t>given cost for stepping 1/2 stairs on each level, figure out cheapest way to get to top</t>
+  </si>
+  <si>
+    <t>make list len n + 1, make 0 and 1 have cost 0, check 2 below and 1 below plus their costs and take the minimum to be curr level</t>
   </si>
 </sst>
 </file>
@@ -2353,7 +2359,7 @@
   <dimension ref="A1:G967"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A91" zoomScale="90" zoomScaleNormal="122" workbookViewId="0">
-      <selection activeCell="D95" sqref="D95"/>
+      <selection activeCell="D96" sqref="D96"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3859,15 +3865,19 @@
       </c>
       <c r="F94" s="3"/>
     </row>
-    <row r="95" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="B95" s="4" t="s">
         <v>354</v>
       </c>
       <c r="C95" s="4" t="s">
         <v>112</v>
       </c>
-      <c r="D95" s="3"/>
-      <c r="E95" s="3"/>
+      <c r="D95" s="3" t="s">
+        <v>417</v>
+      </c>
+      <c r="E95" s="3" t="s">
+        <v>418</v>
+      </c>
       <c r="F95" s="3"/>
     </row>
     <row r="96" spans="1:6" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Finished house robber 2
</commit_message>
<xml_diff>
--- a/LeetCode.xlsx
+++ b/LeetCode.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\EricS\Documents\VSCode Projects\LeetcodeGrind\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6A7E7889-8A32-4F0E-96EA-18367852B4CF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C6B8852F-1DD0-4027-BC20-E5D116D877CD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="3" xr2:uid="{02D29AA1-7085-42F6-B3D4-4C0365DA5453}"/>
   </bookViews>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="599" uniqueCount="421">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="601" uniqueCount="423">
   <si>
     <t>Roman to Integer:</t>
   </si>
@@ -1303,7 +1303,13 @@
     <t>each house is given a value, you can't rob adjacent houses, return max profit possible</t>
   </si>
   <si>
-    <t>using given list of values, set second element to max of first element and itself, then future elements are all maximum of 2 houses ago (prev non-adjacent house) plus this house value or the previous house value (don't take every other since it's more profitable to wait extra turn). Remember edge case of list length 1</t>
+    <t>same thing but houses are in circle so first and last are adj</t>
+  </si>
+  <si>
+    <t>literally call house robber function on array without first element and array but without last element to simulate all possibilities, remember len 1 case</t>
+  </si>
+  <si>
+    <t>using given list of values, set second element to max of first element and itself, then future elements are all maximum of 2 houses ago (prev non-adjacent house) plus this house value or the previous house value (don't take every other since it's more profitable to wait extra turn). Remember edge case of list length 1. Also better to just use 2 or 3 variables to track than entire mem arr</t>
   </si>
 </sst>
 </file>
@@ -2365,7 +2371,7 @@
   <dimension ref="A1:G967"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A91" zoomScale="90" zoomScaleNormal="122" workbookViewId="0">
-      <selection activeCell="E97" sqref="E97"/>
+      <selection activeCell="D104" sqref="D104"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3886,7 +3892,7 @@
       </c>
       <c r="F95" s="3"/>
     </row>
-    <row r="96" spans="1:6" ht="75" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:6" ht="75.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B96" s="4" t="s">
         <v>355</v>
       </c>
@@ -3897,19 +3903,23 @@
         <v>419</v>
       </c>
       <c r="E96" s="3" t="s">
-        <v>420</v>
+        <v>422</v>
       </c>
       <c r="F96" s="3"/>
     </row>
-    <row r="97" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="B97" s="4" t="s">
         <v>356</v>
       </c>
       <c r="C97" s="4" t="s">
         <v>119</v>
       </c>
-      <c r="D97" s="3"/>
-      <c r="E97" s="3"/>
+      <c r="D97" s="3" t="s">
+        <v>420</v>
+      </c>
+      <c r="E97" s="3" t="s">
+        <v>421</v>
+      </c>
       <c r="F97" s="3"/>
     </row>
     <row r="98" spans="1:6" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Finished longest palindrome substring
</commit_message>
<xml_diff>
--- a/LeetCode.xlsx
+++ b/LeetCode.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\EricS\Documents\VSCode Projects\LeetcodeGrind\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C6B8852F-1DD0-4027-BC20-E5D116D877CD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6A98CA69-440F-4EC1-95CE-F1F73690B412}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="3" xr2:uid="{02D29AA1-7085-42F6-B3D4-4C0365DA5453}"/>
   </bookViews>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="601" uniqueCount="423">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="603" uniqueCount="425">
   <si>
     <t>Roman to Integer:</t>
   </si>
@@ -1310,6 +1310,12 @@
   </si>
   <si>
     <t>using given list of values, set second element to max of first element and itself, then future elements are all maximum of 2 houses ago (prev non-adjacent house) plus this house value or the previous house value (don't take every other since it's more profitable to wait extra turn). Remember edge case of list length 1. Also better to just use 2 or 3 variables to track than entire mem arr</t>
+  </si>
+  <si>
+    <t>find longest palindromic substring and return</t>
+  </si>
+  <si>
+    <t>keep track of maxlen and ret, loop through all middle indexes and propogate outwards with two pointer, updating maxlen and ret as needed, remember palindromes can be odd and even length so for each middle index you have to do 2 propogations outward</t>
   </si>
 </sst>
 </file>
@@ -2371,7 +2377,7 @@
   <dimension ref="A1:G967"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A91" zoomScale="90" zoomScaleNormal="122" workbookViewId="0">
-      <selection activeCell="D104" sqref="D104"/>
+      <selection activeCell="E99" sqref="E99"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3922,15 +3928,19 @@
       </c>
       <c r="F97" s="3"/>
     </row>
-    <row r="98" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:6" ht="60" x14ac:dyDescent="0.25">
       <c r="B98" s="4" t="s">
         <v>357</v>
       </c>
       <c r="C98" s="4" t="s">
         <v>119</v>
       </c>
-      <c r="D98" s="3"/>
-      <c r="E98" s="3"/>
+      <c r="D98" s="3" t="s">
+        <v>423</v>
+      </c>
+      <c r="E98" s="3" t="s">
+        <v>424</v>
+      </c>
       <c r="F98" s="3"/>
     </row>
     <row r="99" spans="1:6" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Finished max prod subarr
</commit_message>
<xml_diff>
--- a/LeetCode.xlsx
+++ b/LeetCode.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\EricS\Documents\VSCode Projects\LeetcodeGrind\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{469905D6-F23C-479A-BF60-497BF304590A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D37D61B2-E022-401B-A699-17E366035BB2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="3" xr2:uid="{02D29AA1-7085-42F6-B3D4-4C0365DA5453}"/>
   </bookViews>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1075" uniqueCount="431">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="611" uniqueCount="433">
   <si>
     <t>Roman to Integer:</t>
   </si>
@@ -1334,6 +1334,12 @@
   </si>
   <si>
     <t>create dp array initialized to inf, loop through up to amount + 1, inner loop through all coin values, getting I - coin if that's geq 0 and adding 1, taking the min of that and the current value in the array for here</t>
+  </si>
+  <si>
+    <t>return maximum product of a subarray</t>
+  </si>
+  <si>
+    <t>iterate through keeping track of currmax and currmin, updating it each time with all possibilities (currmax * n, currmin * n, n), update ret with currmax</t>
   </si>
 </sst>
 </file>
@@ -2395,7 +2401,7 @@
   <dimension ref="A1:G967"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A93" zoomScale="90" zoomScaleNormal="122" workbookViewId="0">
-      <selection activeCell="D102" sqref="D102"/>
+      <selection activeCell="D103" sqref="D103"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4006,15 +4012,19 @@
       </c>
       <c r="F101" s="3"/>
     </row>
-    <row r="102" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="B102" s="4" t="s">
         <v>361</v>
       </c>
       <c r="C102" s="4" t="s">
         <v>119</v>
       </c>
-      <c r="D102" s="3"/>
-      <c r="E102" s="3"/>
+      <c r="D102" s="3" t="s">
+        <v>431</v>
+      </c>
+      <c r="E102" s="3" t="s">
+        <v>432</v>
+      </c>
       <c r="F102" s="3"/>
     </row>
     <row r="103" spans="1:6" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Finished word break problem
</commit_message>
<xml_diff>
--- a/LeetCode.xlsx
+++ b/LeetCode.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\EricS\Documents\VSCode Projects\LeetcodeGrind\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D37D61B2-E022-401B-A699-17E366035BB2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D9DD8D43-2F2F-4FAC-BE70-6A5FE43F1CF7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="3" xr2:uid="{02D29AA1-7085-42F6-B3D4-4C0365DA5453}"/>
   </bookViews>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="611" uniqueCount="433">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="613" uniqueCount="435">
   <si>
     <t>Roman to Integer:</t>
   </si>
@@ -1340,6 +1340,12 @@
   </si>
   <si>
     <t>iterate through keeping track of currmax and currmin, updating it each time with all possibilities (currmax * n, currmin * n, n), update ret with currmax</t>
+  </si>
+  <si>
+    <t>check if it's possible to make certain string given list of possible substrings</t>
+  </si>
+  <si>
+    <t>basically just use boolean array for dp, marking reacheable spots as True based on substring comparisons, optimal to look backwards rather than propogating forwards though, rmbr to check bounds</t>
   </si>
 </sst>
 </file>
@@ -2401,7 +2407,7 @@
   <dimension ref="A1:G967"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A93" zoomScale="90" zoomScaleNormal="122" workbookViewId="0">
-      <selection activeCell="D103" sqref="D103"/>
+      <selection activeCell="D104" sqref="D104"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4027,15 +4033,19 @@
       </c>
       <c r="F102" s="3"/>
     </row>
-    <row r="103" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:6" ht="45" x14ac:dyDescent="0.25">
       <c r="B103" s="4" t="s">
         <v>362</v>
       </c>
       <c r="C103" s="4" t="s">
         <v>119</v>
       </c>
-      <c r="D103" s="3"/>
-      <c r="E103" s="3"/>
+      <c r="D103" s="3" t="s">
+        <v>433</v>
+      </c>
+      <c r="E103" s="3" t="s">
+        <v>434</v>
+      </c>
       <c r="F103" s="3"/>
     </row>
     <row r="104" spans="1:6" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
finished longest increasing subsequence
</commit_message>
<xml_diff>
--- a/LeetCode.xlsx
+++ b/LeetCode.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\EricS\Documents\VSCode Projects\LeetcodeGrind\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D9DD8D43-2F2F-4FAC-BE70-6A5FE43F1CF7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1BF20DD8-5BD7-4E4A-AE62-CFE30FFF0DE7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="3" xr2:uid="{02D29AA1-7085-42F6-B3D4-4C0365DA5453}"/>
   </bookViews>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="613" uniqueCount="435">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="615" uniqueCount="437">
   <si>
     <t>Roman to Integer:</t>
   </si>
@@ -1346,6 +1346,12 @@
   </si>
   <si>
     <t>basically just use boolean array for dp, marking reacheable spots as True based on substring comparisons, optimal to look backwards rather than propogating forwards though, rmbr to check bounds</t>
+  </si>
+  <si>
+    <t>return length of longest increasing subsequence</t>
+  </si>
+  <si>
+    <t>basically create array of len n + 1 filled w -inf, then you keep tracking the minimum number for each possible length subsequence and update from there, like [0, 0, 1, 2, 3] would mean smallest is 0, second smallest is 1, then 2, and so on, using ret to track the last index in the sorted bunch</t>
   </si>
 </sst>
 </file>
@@ -2406,8 +2412,8 @@
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:G967"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A93" zoomScale="90" zoomScaleNormal="122" workbookViewId="0">
-      <selection activeCell="D104" sqref="D104"/>
+    <sheetView tabSelected="1" topLeftCell="A96" zoomScale="90" zoomScaleNormal="122" workbookViewId="0">
+      <selection activeCell="D105" sqref="D105"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4048,15 +4054,19 @@
       </c>
       <c r="F103" s="3"/>
     </row>
-    <row r="104" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:6" ht="60" x14ac:dyDescent="0.25">
       <c r="B104" s="4" t="s">
         <v>363</v>
       </c>
       <c r="C104" s="4" t="s">
         <v>119</v>
       </c>
-      <c r="D104" s="3"/>
-      <c r="E104" s="3"/>
+      <c r="D104" s="3" t="s">
+        <v>435</v>
+      </c>
+      <c r="E104" s="3" t="s">
+        <v>436</v>
+      </c>
       <c r="F104" s="3"/>
     </row>
     <row r="105" spans="1:6" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Finished partition equal subsets and 1d dp
</commit_message>
<xml_diff>
--- a/LeetCode.xlsx
+++ b/LeetCode.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\EricS\Documents\VSCode Projects\LeetcodeGrind\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1BF20DD8-5BD7-4E4A-AE62-CFE30FFF0DE7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{01E4DFD5-75AD-4B40-9C09-2CC2025B018B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="3" xr2:uid="{02D29AA1-7085-42F6-B3D4-4C0365DA5453}"/>
   </bookViews>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="615" uniqueCount="437">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="618" uniqueCount="440">
   <si>
     <t>Roman to Integer:</t>
   </si>
@@ -1352,6 +1352,15 @@
   </si>
   <si>
     <t>basically create array of len n + 1 filled w -inf, then you keep tracking the minimum number for each possible length subsequence and update from there, like [0, 0, 1, 2, 3] would mean smallest is 0, second smallest is 1, then 2, and so on, using ret to track the last index in the sorted bunch</t>
+  </si>
+  <si>
+    <t>there's a genius bitmap solution</t>
+  </si>
+  <si>
+    <t>return whether an array of integers could be split into 2 equal subsets</t>
+  </si>
+  <si>
+    <t>get sum and return false if odd, target is sum divided by 2, basically check all possible subsets to see if you can get to target (looping through set and all nums over and over and adding the sums if they are less than target)</t>
   </si>
 </sst>
 </file>
@@ -2413,7 +2422,7 @@
   <dimension ref="A1:G967"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A96" zoomScale="90" zoomScaleNormal="122" workbookViewId="0">
-      <selection activeCell="D105" sqref="D105"/>
+      <selection activeCell="D106" sqref="D106"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4069,16 +4078,22 @@
       </c>
       <c r="F104" s="3"/>
     </row>
-    <row r="105" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:6" ht="45" x14ac:dyDescent="0.25">
       <c r="B105" s="4" t="s">
         <v>364</v>
       </c>
       <c r="C105" s="4" t="s">
         <v>119</v>
       </c>
-      <c r="D105" s="3"/>
-      <c r="E105" s="3"/>
-      <c r="F105" s="3"/>
+      <c r="D105" s="3" t="s">
+        <v>438</v>
+      </c>
+      <c r="E105" s="3" t="s">
+        <v>439</v>
+      </c>
+      <c r="F105" s="3" t="s">
+        <v>437</v>
+      </c>
     </row>
     <row r="106" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A106" s="5" t="s">

</xml_diff>

<commit_message>
Finished longest common subseq
</commit_message>
<xml_diff>
--- a/LeetCode.xlsx
+++ b/LeetCode.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\EricS\Documents\VSCode Projects\LeetcodeGrind\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4812E793-91C9-4912-A7C6-04CF24FD64D0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1AB8E172-079D-48F6-9324-FA71E39E88B4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="3" xr2:uid="{02D29AA1-7085-42F6-B3D4-4C0365DA5453}"/>
   </bookViews>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="620" uniqueCount="442">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="622" uniqueCount="444">
   <si>
     <t>Roman to Integer:</t>
   </si>
@@ -1367,6 +1367,12 @@
   </si>
   <si>
     <t>make array of length n all initialized to 1, have nested for loop the first going from 1 to m, second going from 1 to n, insided nested for loop you have arr[i] += arr[i + 1] since going down is the same each time so you just have to add the ones coming from the left, and top row and left column is going to always just be all 1</t>
+  </si>
+  <si>
+    <t>find longest common subsequence in 2 strings</t>
+  </si>
+  <si>
+    <t>create 2d array that is n + 1 x m + 1, at each spot if the character for each of the words is the same, make that spot 1 + track[i - 1][j - 1] the diagonally up left spot since that's the last spot where there could have been a match that would still allow this one to happen, if no match, then current spot's value is the maximum between the spot above and the spot to the left since that's how we propagate the values down and those are the longest common subseq at each point in the string. Remember indexing differences between track and the strings</t>
   </si>
 </sst>
 </file>
@@ -2428,7 +2434,7 @@
   <dimension ref="A1:G967"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A100" zoomScaleNormal="122" workbookViewId="0">
-      <selection activeCell="D107" sqref="D107"/>
+      <selection activeCell="E108" sqref="E108"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4119,15 +4125,19 @@
       </c>
       <c r="F106" s="3"/>
     </row>
-    <row r="107" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:6" ht="120" x14ac:dyDescent="0.25">
       <c r="B107" s="4" t="s">
         <v>406</v>
       </c>
       <c r="C107" s="4" t="s">
         <v>119</v>
       </c>
-      <c r="D107" s="3"/>
-      <c r="E107" s="3"/>
+      <c r="D107" s="3" t="s">
+        <v>442</v>
+      </c>
+      <c r="E107" s="3" t="s">
+        <v>443</v>
+      </c>
       <c r="F107" s="3"/>
     </row>
     <row r="108" spans="1:6" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Finished coin change 2
</commit_message>
<xml_diff>
--- a/LeetCode.xlsx
+++ b/LeetCode.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\EricS\Documents\VSCode Projects\LeetcodeGrind\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1AB8E172-079D-48F6-9324-FA71E39E88B4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{27C8B4D0-5867-471C-A509-926F3F5770AA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="3" xr2:uid="{02D29AA1-7085-42F6-B3D4-4C0365DA5453}"/>
   </bookViews>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="622" uniqueCount="444">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1105" uniqueCount="446">
   <si>
     <t>Roman to Integer:</t>
   </si>
@@ -1373,6 +1373,12 @@
   </si>
   <si>
     <t>create 2d array that is n + 1 x m + 1, at each spot if the character for each of the words is the same, make that spot 1 + track[i - 1][j - 1] the diagonally up left spot since that's the last spot where there could have been a match that would still allow this one to happen, if no match, then current spot's value is the maximum between the spot above and the spot to the left since that's how we propagate the values down and those are the longest common subseq at each point in the string. Remember indexing differences between track and the strings</t>
+  </si>
+  <si>
+    <t>coin change but return total number of combinations of coins that would end up at target value</t>
+  </si>
+  <si>
+    <t>create tracking arr of length n + 1 where n is target amount, initialize arr[0] = 1, for each coin value, loop through and increase each valid index by index minus coin value, return end</t>
   </si>
 </sst>
 </file>
@@ -2433,8 +2439,8 @@
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:G967"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A100" zoomScaleNormal="122" workbookViewId="0">
-      <selection activeCell="E108" sqref="E108"/>
+    <sheetView tabSelected="1" topLeftCell="A104" zoomScaleNormal="122" workbookViewId="0">
+      <selection activeCell="E110" sqref="E110"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4151,15 +4157,19 @@
       <c r="E108" s="3"/>
       <c r="F108" s="3"/>
     </row>
-    <row r="109" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="109" spans="1:6" ht="45" x14ac:dyDescent="0.25">
       <c r="B109" s="4" t="s">
         <v>408</v>
       </c>
       <c r="C109" s="4" t="s">
         <v>119</v>
       </c>
-      <c r="D109" s="3"/>
-      <c r="E109" s="3"/>
+      <c r="D109" s="3" t="s">
+        <v>444</v>
+      </c>
+      <c r="E109" s="3" t="s">
+        <v>445</v>
+      </c>
       <c r="F109" s="3"/>
     </row>
     <row r="110" spans="1:6" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Created files for stocks w cooldown
</commit_message>
<xml_diff>
--- a/LeetCode.xlsx
+++ b/LeetCode.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\EricS\Documents\VSCode Projects\LeetcodeGrind\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{27C8B4D0-5867-471C-A509-926F3F5770AA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CA42FBEB-D313-4406-B4B2-2BEA6375C543}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="3" xr2:uid="{02D29AA1-7085-42F6-B3D4-4C0365DA5453}"/>
   </bookViews>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1105" uniqueCount="446">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="625" uniqueCount="447">
   <si>
     <t>Roman to Integer:</t>
   </si>
@@ -1379,6 +1379,9 @@
   </si>
   <si>
     <t>create tracking arr of length n + 1 where n is target amount, initialize arr[0] = 1, for each coin value, loop through and increase each valid index by index minus coin value, return end</t>
+  </si>
+  <si>
+    <t>cooldown between sell and next buy (gap of 1 day), return optimal profit amount</t>
   </si>
 </sst>
 </file>
@@ -2440,7 +2443,7 @@
   <dimension ref="A1:G967"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A104" zoomScaleNormal="122" workbookViewId="0">
-      <selection activeCell="E110" sqref="E110"/>
+      <selection activeCell="D109" sqref="D109"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4146,14 +4149,16 @@
       </c>
       <c r="F107" s="3"/>
     </row>
-    <row r="108" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="B108" s="4" t="s">
         <v>407</v>
       </c>
       <c r="C108" s="4" t="s">
         <v>119</v>
       </c>
-      <c r="D108" s="3"/>
+      <c r="D108" s="3" t="s">
+        <v>446</v>
+      </c>
       <c r="E108" s="3"/>
       <c r="F108" s="3"/>
     </row>

</xml_diff>

<commit_message>
Finished best time to buy and sell stock w cooldown
</commit_message>
<xml_diff>
--- a/LeetCode.xlsx
+++ b/LeetCode.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\EricS\Documents\VSCode Projects\LeetcodeGrind\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CA42FBEB-D313-4406-B4B2-2BEA6375C543}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{368C5930-BEF3-43A4-B64B-2C0D1E5FAB43}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="3" xr2:uid="{02D29AA1-7085-42F6-B3D4-4C0365DA5453}"/>
   </bookViews>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="625" uniqueCount="447">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="626" uniqueCount="448">
   <si>
     <t>Roman to Integer:</t>
   </si>
@@ -1382,6 +1382,9 @@
   </si>
   <si>
     <t>cooldown between sell and next buy (gap of 1 day), return optimal profit amount</t>
+  </si>
+  <si>
+    <t>basically you have to keep track of optimal profit at each time step ending in a buy + waits or ending in a sell + waits. For buy + wait, the new buy is the max between the previous buy and sell[i - 2] - price (whether it's more worth to buy and hold or sell and buy again), for sell + wait, the new sell is the max between the previous sell and buy and sell (whether's it's more worth to wait or buy again and sell again). Have to initialize buy[1] to -prices[0] to force buy first thing, this allows for the list to propogate properly and it does not act buy first thing necessarily cuz it could be more optimal to sell for 0 at start and buy later which overrides</t>
   </si>
 </sst>
 </file>
@@ -2442,8 +2445,8 @@
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:G967"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A104" zoomScaleNormal="122" workbookViewId="0">
-      <selection activeCell="D109" sqref="D109"/>
+    <sheetView tabSelected="1" topLeftCell="A105" zoomScaleNormal="122" workbookViewId="0">
+      <selection activeCell="D110" sqref="D110"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4149,7 +4152,7 @@
       </c>
       <c r="F107" s="3"/>
     </row>
-    <row r="108" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:6" ht="135" x14ac:dyDescent="0.25">
       <c r="B108" s="4" t="s">
         <v>407</v>
       </c>
@@ -4159,7 +4162,9 @@
       <c r="D108" s="3" t="s">
         <v>446</v>
       </c>
-      <c r="E108" s="3"/>
+      <c r="E108" s="3" t="s">
+        <v>447</v>
+      </c>
       <c r="F108" s="3"/>
     </row>
     <row r="109" spans="1:6" ht="45" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Finished target sum problem, going to try to optimize for space
</commit_message>
<xml_diff>
--- a/LeetCode.xlsx
+++ b/LeetCode.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\EricS\Documents\VSCode Projects\LeetcodeGrind\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{368C5930-BEF3-43A4-B64B-2C0D1E5FAB43}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0395C8DD-15D8-439A-AFF3-84C65DF484EE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="3" xr2:uid="{02D29AA1-7085-42F6-B3D4-4C0365DA5453}"/>
   </bookViews>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="626" uniqueCount="448">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="628" uniqueCount="450">
   <si>
     <t>Roman to Integer:</t>
   </si>
@@ -1385,6 +1385,13 @@
   </si>
   <si>
     <t>basically you have to keep track of optimal profit at each time step ending in a buy + waits or ending in a sell + waits. For buy + wait, the new buy is the max between the previous buy and sell[i - 2] - price (whether it's more worth to buy and hold or sell and buy again), for sell + wait, the new sell is the max between the previous sell and buy and sell (whether's it's more worth to wait or buy again and sell again). Have to initialize buy[1] to -prices[0] to force buy first thing, this allows for the list to propogate properly and it does not act buy first thing necessarily cuz it could be more optimal to sell for 0 at start and buy later which overrides</t>
+  </si>
+  <si>
+    <t>given array of positive ints, figure out number of ways to assign positive and negatives to each to sum to a target sum</t>
+  </si>
+  <si>
+    <t>Problem is basically asking to find all possible subsets splits with positive and negative signs and we want sum(P) - sum(N) = target and we have sum(P) + sum(N) = total. Combining these gives 2 * sum(P) = total + target which becomes 2 * (sum(P) - target) = total - target which has to be even. Therefore, we also just need to get new target of (total - target) / 2 to find all possible subsets since total - target = sum(P) + sum(N) - sum(P) + sum(N) = 2 * sum(N). Now problem statement is just find all subsets that sum to (total - target) / 2
+To solve this, we first find the total and calculate the new target. Then, we do the standard way of checking how many ways to add to a target given an array of numbers, using a 2D matrix that is length of nums x new target + 1. Then we do a nested loop to calculate the number of ways to get to each number given the first i numbers in the sequence choosing to include or not include, similar to combination sum problem but 2D since you care about history.</t>
   </si>
 </sst>
 </file>
@@ -2445,8 +2452,8 @@
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:G967"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A105" zoomScaleNormal="122" workbookViewId="0">
-      <selection activeCell="D110" sqref="D110"/>
+    <sheetView tabSelected="1" topLeftCell="A107" zoomScaleNormal="122" workbookViewId="0">
+      <selection activeCell="E110" sqref="E110"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4182,15 +4189,19 @@
       </c>
       <c r="F109" s="3"/>
     </row>
-    <row r="110" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="110" spans="1:6" ht="240" x14ac:dyDescent="0.25">
       <c r="B110" s="4" t="s">
         <v>409</v>
       </c>
       <c r="C110" s="4" t="s">
         <v>119</v>
       </c>
-      <c r="D110" s="3"/>
-      <c r="E110" s="3"/>
+      <c r="D110" s="3" t="s">
+        <v>448</v>
+      </c>
+      <c r="E110" s="3" t="s">
+        <v>449</v>
+      </c>
       <c r="F110" s="3"/>
     </row>
     <row r="111" spans="1:6" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Added dynamic programming categories to dp section
</commit_message>
<xml_diff>
--- a/LeetCode.xlsx
+++ b/LeetCode.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\EricS\Documents\VSCode Projects\LeetcodeGrind\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0395C8DD-15D8-439A-AFF3-84C65DF484EE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{32C898DB-9BC5-4D95-A8EA-DBCC643C2C7F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="3" xr2:uid="{02D29AA1-7085-42F6-B3D4-4C0365DA5453}"/>
   </bookViews>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="628" uniqueCount="450">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="639" uniqueCount="454">
   <si>
     <t>Roman to Integer:</t>
   </si>
@@ -1392,6 +1392,18 @@
   <si>
     <t>Problem is basically asking to find all possible subsets splits with positive and negative signs and we want sum(P) - sum(N) = target and we have sum(P) + sum(N) = total. Combining these gives 2 * sum(P) = total + target which becomes 2 * (sum(P) - target) = total - target which has to be even. Therefore, we also just need to get new target of (total - target) / 2 to find all possible subsets since total - target = sum(P) + sum(N) - sum(P) + sum(N) = 2 * sum(N). Now problem statement is just find all subsets that sum to (total - target) / 2
 To solve this, we first find the total and calculate the new target. Then, we do the standard way of checking how many ways to add to a target given an array of numbers, using a 2D matrix that is length of nums x new target + 1. Then we do a nested loop to calculate the number of ways to get to each number given the first i numbers in the sequence choosing to include or not include, similar to combination sum problem but 2D since you care about history.</t>
+  </si>
+  <si>
+    <t>Unbounded Knapsack</t>
+  </si>
+  <si>
+    <t>Shortest Path</t>
+  </si>
+  <si>
+    <t>Fibonacci</t>
+  </si>
+  <si>
+    <t>0/1 Knapsack</t>
   </si>
 </sst>
 </file>
@@ -1496,7 +1508,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="19">
+  <cellXfs count="22">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -1508,9 +1520,6 @@
       <alignment horizontal="left" vertical="top" wrapText="1" readingOrder="1"/>
     </xf>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
@@ -1525,9 +1534,6 @@
     <xf numFmtId="49" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="49" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
     <xf numFmtId="49" fontId="7" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
@@ -1536,9 +1542,6 @@
     </xf>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="8" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
     </xf>
     <xf numFmtId="49" fontId="9" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
@@ -1551,6 +1554,24 @@
     </xf>
     <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="49" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="8" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -2450,60 +2471,60 @@
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{55ADB572-3F2B-41BB-A303-53CCEC27F096}">
   <sheetPr codeName="Sheet1"/>
-  <dimension ref="A1:G967"/>
+  <dimension ref="A1:G969"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A107" zoomScaleNormal="122" workbookViewId="0">
-      <selection activeCell="E110" sqref="E110"/>
+    <sheetView tabSelected="1" topLeftCell="A110" zoomScaleNormal="122" workbookViewId="0">
+      <selection activeCell="B124" sqref="B124"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="19.7109375" style="5" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="19.7109375" style="17" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="59.28515625" style="4" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="5.7109375" style="4" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="56.42578125" style="4" customWidth="1"/>
     <col min="5" max="5" width="71.28515625" style="4" customWidth="1"/>
     <col min="6" max="6" width="70.28515625" style="4" customWidth="1"/>
-    <col min="7" max="7" width="91.140625" style="6" customWidth="1"/>
+    <col min="7" max="7" width="91.140625" style="5" customWidth="1"/>
     <col min="8" max="8" width="82.28515625" style="4" customWidth="1"/>
     <col min="9" max="16384" width="9.140625" style="4"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A1" s="18" t="s">
+      <c r="A1" s="15" t="s">
         <v>111</v>
       </c>
-      <c r="B1" s="18"/>
-      <c r="C1" s="18"/>
-      <c r="D1" s="18"/>
-      <c r="E1" s="18"/>
-      <c r="F1" s="18"/>
+      <c r="B1" s="15"/>
+      <c r="C1" s="15"/>
+      <c r="D1" s="15"/>
+      <c r="E1" s="15"/>
+      <c r="F1" s="15"/>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A2" s="9" t="s">
+      <c r="A2" s="16" t="s">
         <v>110</v>
       </c>
-      <c r="B2" s="9" t="s">
+      <c r="B2" s="8" t="s">
         <v>37</v>
       </c>
-      <c r="C2" s="9" t="s">
+      <c r="C2" s="8" t="s">
         <v>160</v>
       </c>
-      <c r="D2" s="9" t="s">
+      <c r="D2" s="8" t="s">
         <v>38</v>
       </c>
-      <c r="E2" s="9" t="s">
+      <c r="E2" s="8" t="s">
         <v>39</v>
       </c>
-      <c r="F2" s="9" t="s">
+      <c r="F2" s="8" t="s">
         <v>41</v>
       </c>
-      <c r="G2" s="9" t="s">
+      <c r="G2" s="8" t="s">
         <v>373</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A3" s="5" t="s">
+      <c r="A3" s="17" t="s">
         <v>109</v>
       </c>
       <c r="B3" s="4" t="s">
@@ -2577,7 +2598,7 @@
       <c r="D7" s="3" t="s">
         <v>127</v>
       </c>
-      <c r="E7" s="6" t="s">
+      <c r="E7" s="5" t="s">
         <v>128</v>
       </c>
       <c r="F7" s="3"/>
@@ -2632,7 +2653,7 @@
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A11" s="5" t="s">
+      <c r="A11" s="17" t="s">
         <v>137</v>
       </c>
       <c r="B11" s="4" t="s">
@@ -2712,7 +2733,7 @@
       <c r="F15" s="3"/>
     </row>
     <row r="16" spans="1:7" ht="30" x14ac:dyDescent="0.25">
-      <c r="A16" s="5" t="s">
+      <c r="A16" s="17" t="s">
         <v>153</v>
       </c>
       <c r="B16" s="4" t="s">
@@ -2826,7 +2847,7 @@
       </c>
     </row>
     <row r="23" spans="1:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="A23" s="5" t="s">
+      <c r="A23" s="17" t="s">
         <v>169</v>
       </c>
       <c r="B23" s="4" t="s">
@@ -2938,7 +2959,7 @@
       </c>
     </row>
     <row r="30" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A30" s="5" t="s">
+      <c r="A30" s="17" t="s">
         <v>168</v>
       </c>
       <c r="B30" s="4" t="s">
@@ -3033,7 +3054,7 @@
       <c r="F35" s="3"/>
     </row>
     <row r="36" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A36" s="5" t="s">
+      <c r="A36" s="17" t="s">
         <v>183</v>
       </c>
       <c r="B36" s="4" t="s">
@@ -3143,16 +3164,16 @@
       <c r="F42" s="3"/>
     </row>
     <row r="43" spans="1:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="B43" s="7" t="s">
+      <c r="B43" s="6" t="s">
         <v>192</v>
       </c>
-      <c r="C43" s="7" t="s">
+      <c r="C43" s="6" t="s">
         <v>119</v>
       </c>
-      <c r="D43" s="8" t="s">
+      <c r="D43" s="7" t="s">
         <v>213</v>
       </c>
-      <c r="E43" s="8" t="s">
+      <c r="E43" s="7" t="s">
         <v>214</v>
       </c>
       <c r="F43" s="3"/>
@@ -3203,7 +3224,7 @@
       <c r="F46" s="3"/>
     </row>
     <row r="47" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A47" s="5" t="s">
+      <c r="A47" s="17" t="s">
         <v>250</v>
       </c>
       <c r="B47" s="4" t="s">
@@ -3420,23 +3441,23 @@
       </c>
     </row>
     <row r="61" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A61" s="10"/>
-      <c r="B61" s="11" t="s">
+      <c r="A61" s="18"/>
+      <c r="B61" s="9" t="s">
         <v>265</v>
       </c>
-      <c r="C61" s="11" t="s">
+      <c r="C61" s="9" t="s">
         <v>142</v>
       </c>
-      <c r="D61" s="12" t="s">
+      <c r="D61" s="10" t="s">
         <v>285</v>
       </c>
-      <c r="E61" s="12" t="s">
+      <c r="E61" s="10" t="s">
         <v>286</v>
       </c>
       <c r="F61" s="3"/>
     </row>
     <row r="62" spans="1:6" ht="105" x14ac:dyDescent="0.25">
-      <c r="A62" s="5" t="s">
+      <c r="A62" s="17" t="s">
         <v>290</v>
       </c>
       <c r="B62" s="4" t="s">
@@ -3488,7 +3509,7 @@
       </c>
     </row>
     <row r="65" spans="1:7" ht="45" x14ac:dyDescent="0.25">
-      <c r="A65" s="5" t="s">
+      <c r="A65" s="17" t="s">
         <v>294</v>
       </c>
       <c r="B65" s="4" t="s">
@@ -3535,7 +3556,7 @@
       <c r="E67" s="3" t="s">
         <v>317</v>
       </c>
-      <c r="F67" s="13"/>
+      <c r="F67" s="11"/>
     </row>
     <row r="68" spans="1:7" ht="75" x14ac:dyDescent="0.25">
       <c r="B68" s="4" t="s">
@@ -3559,7 +3580,7 @@
       <c r="C69" s="4" t="s">
         <v>119</v>
       </c>
-      <c r="D69" s="6" t="s">
+      <c r="D69" s="5" t="s">
         <v>325</v>
       </c>
       <c r="E69" s="3" t="s">
@@ -3628,7 +3649,7 @@
       <c r="F73" s="3"/>
     </row>
     <row r="74" spans="1:7" ht="45" x14ac:dyDescent="0.25">
-      <c r="A74" s="5" t="s">
+      <c r="A74" s="17" t="s">
         <v>330</v>
       </c>
       <c r="B74" s="4" t="s">
@@ -3707,22 +3728,22 @@
       </c>
       <c r="F78" s="3"/>
     </row>
-    <row r="79" spans="1:7" s="15" customFormat="1" ht="30" x14ac:dyDescent="0.25">
-      <c r="A79" s="14"/>
-      <c r="B79" s="15" t="s">
+    <row r="79" spans="1:7" s="12" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+      <c r="A79" s="19"/>
+      <c r="B79" s="12" t="s">
         <v>336</v>
       </c>
-      <c r="C79" s="15" t="s">
+      <c r="C79" s="12" t="s">
         <v>119</v>
       </c>
-      <c r="D79" s="16" t="s">
+      <c r="D79" s="13" t="s">
         <v>371</v>
       </c>
-      <c r="E79" s="16" t="s">
+      <c r="E79" s="13" t="s">
         <v>372</v>
       </c>
-      <c r="F79" s="16"/>
-      <c r="G79" s="17"/>
+      <c r="F79" s="13"/>
+      <c r="G79" s="14"/>
     </row>
     <row r="80" spans="1:7" ht="60" x14ac:dyDescent="0.25">
       <c r="B80" s="4" t="s">
@@ -3740,7 +3761,7 @@
       <c r="F80" s="3"/>
     </row>
     <row r="81" spans="1:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="A81" s="5" t="s">
+      <c r="A81" s="17" t="s">
         <v>338</v>
       </c>
       <c r="B81" s="4" t="s">
@@ -3941,316 +3962,346 @@
       </c>
       <c r="F93" s="3"/>
     </row>
-    <row r="94" spans="1:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="A94" s="5" t="s">
+    <row r="94" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A94" s="17" t="s">
         <v>352</v>
       </c>
-      <c r="B94" s="4" t="s">
+      <c r="D94" s="3"/>
+      <c r="E94" s="3"/>
+      <c r="F94" s="3"/>
+    </row>
+    <row r="95" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A95" s="20" t="s">
+        <v>452</v>
+      </c>
+      <c r="B95" s="4" t="s">
         <v>353</v>
-      </c>
-      <c r="C94" s="4" t="s">
-        <v>112</v>
-      </c>
-      <c r="D94" s="3" t="s">
-        <v>415</v>
-      </c>
-      <c r="E94" s="3" t="s">
-        <v>416</v>
-      </c>
-      <c r="F94" s="3"/>
-    </row>
-    <row r="95" spans="1:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="B95" s="4" t="s">
-        <v>354</v>
       </c>
       <c r="C95" s="4" t="s">
         <v>112</v>
       </c>
       <c r="D95" s="3" t="s">
+        <v>415</v>
+      </c>
+      <c r="E95" s="3" t="s">
+        <v>416</v>
+      </c>
+      <c r="F95" s="3"/>
+    </row>
+    <row r="96" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A96" s="20" t="s">
+        <v>452</v>
+      </c>
+      <c r="B96" s="4" t="s">
+        <v>354</v>
+      </c>
+      <c r="C96" s="4" t="s">
+        <v>112</v>
+      </c>
+      <c r="D96" s="3" t="s">
         <v>417</v>
       </c>
-      <c r="E95" s="3" t="s">
+      <c r="E96" s="3" t="s">
         <v>418</v>
       </c>
-      <c r="F95" s="3"/>
-    </row>
-    <row r="96" spans="1:6" ht="75.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B96" s="4" t="s">
+      <c r="F96" s="3"/>
+    </row>
+    <row r="97" spans="1:6" ht="75.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A97" s="20" t="s">
+        <v>452</v>
+      </c>
+      <c r="B97" s="4" t="s">
         <v>355</v>
-      </c>
-      <c r="C96" s="4" t="s">
-        <v>119</v>
-      </c>
-      <c r="D96" s="3" t="s">
-        <v>419</v>
-      </c>
-      <c r="E96" s="3" t="s">
-        <v>422</v>
-      </c>
-      <c r="F96" s="3"/>
-    </row>
-    <row r="97" spans="1:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="B97" s="4" t="s">
-        <v>356</v>
       </c>
       <c r="C97" s="4" t="s">
         <v>119</v>
       </c>
       <c r="D97" s="3" t="s">
-        <v>420</v>
+        <v>419</v>
       </c>
       <c r="E97" s="3" t="s">
-        <v>421</v>
+        <v>422</v>
       </c>
       <c r="F97" s="3"/>
     </row>
-    <row r="98" spans="1:6" ht="60" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A98" s="20" t="s">
+        <v>452</v>
+      </c>
       <c r="B98" s="4" t="s">
-        <v>357</v>
+        <v>356</v>
       </c>
       <c r="C98" s="4" t="s">
         <v>119</v>
       </c>
       <c r="D98" s="3" t="s">
-        <v>423</v>
+        <v>420</v>
       </c>
       <c r="E98" s="3" t="s">
-        <v>424</v>
+        <v>421</v>
       </c>
       <c r="F98" s="3"/>
     </row>
-    <row r="99" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:6" ht="60" x14ac:dyDescent="0.25">
+      <c r="A99" s="21"/>
       <c r="B99" s="4" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
       <c r="C99" s="4" t="s">
         <v>119</v>
       </c>
       <c r="D99" s="3" t="s">
-        <v>425</v>
+        <v>423</v>
       </c>
       <c r="E99" s="3" t="s">
-        <v>426</v>
+        <v>424</v>
       </c>
       <c r="F99" s="3"/>
     </row>
-    <row r="100" spans="1:6" ht="105" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A100" s="20"/>
       <c r="B100" s="4" t="s">
-        <v>359</v>
+        <v>358</v>
       </c>
       <c r="C100" s="4" t="s">
         <v>119</v>
       </c>
       <c r="D100" s="3" t="s">
-        <v>427</v>
+        <v>425</v>
       </c>
       <c r="E100" s="3" t="s">
-        <v>428</v>
+        <v>426</v>
       </c>
       <c r="F100" s="3"/>
     </row>
-    <row r="101" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:6" ht="105" x14ac:dyDescent="0.25">
+      <c r="A101" s="20" t="s">
+        <v>452</v>
+      </c>
       <c r="B101" s="4" t="s">
-        <v>360</v>
+        <v>359</v>
       </c>
       <c r="C101" s="4" t="s">
         <v>119</v>
       </c>
       <c r="D101" s="3" t="s">
-        <v>429</v>
+        <v>427</v>
       </c>
       <c r="E101" s="3" t="s">
-        <v>430</v>
+        <v>428</v>
       </c>
       <c r="F101" s="3"/>
     </row>
-    <row r="102" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+      <c r="A102" s="20" t="s">
+        <v>450</v>
+      </c>
       <c r="B102" s="4" t="s">
-        <v>361</v>
+        <v>360</v>
       </c>
       <c r="C102" s="4" t="s">
         <v>119</v>
       </c>
       <c r="D102" s="3" t="s">
-        <v>431</v>
+        <v>429</v>
       </c>
       <c r="E102" s="3" t="s">
-        <v>432</v>
+        <v>430</v>
       </c>
       <c r="F102" s="3"/>
     </row>
-    <row r="103" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A103" s="20"/>
       <c r="B103" s="4" t="s">
-        <v>362</v>
+        <v>361</v>
       </c>
       <c r="C103" s="4" t="s">
         <v>119</v>
       </c>
       <c r="D103" s="3" t="s">
-        <v>433</v>
+        <v>431</v>
       </c>
       <c r="E103" s="3" t="s">
-        <v>434</v>
+        <v>432</v>
       </c>
       <c r="F103" s="3"/>
     </row>
-    <row r="104" spans="1:6" ht="60" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+      <c r="A104" s="20"/>
       <c r="B104" s="4" t="s">
-        <v>363</v>
+        <v>362</v>
       </c>
       <c r="C104" s="4" t="s">
         <v>119</v>
       </c>
       <c r="D104" s="3" t="s">
-        <v>435</v>
+        <v>433</v>
       </c>
       <c r="E104" s="3" t="s">
-        <v>436</v>
+        <v>434</v>
       </c>
       <c r="F104" s="3"/>
     </row>
-    <row r="105" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:6" ht="60" x14ac:dyDescent="0.25">
+      <c r="A105" s="20"/>
       <c r="B105" s="4" t="s">
-        <v>364</v>
+        <v>363</v>
       </c>
       <c r="C105" s="4" t="s">
         <v>119</v>
       </c>
       <c r="D105" s="3" t="s">
-        <v>438</v>
+        <v>435</v>
       </c>
       <c r="E105" s="3" t="s">
-        <v>439</v>
-      </c>
-      <c r="F105" s="3" t="s">
-        <v>437</v>
-      </c>
-    </row>
-    <row r="106" spans="1:6" ht="75" x14ac:dyDescent="0.25">
-      <c r="A106" s="5" t="s">
-        <v>403</v>
+        <v>436</v>
+      </c>
+      <c r="F105" s="3"/>
+    </row>
+    <row r="106" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+      <c r="A106" s="20" t="s">
+        <v>453</v>
       </c>
       <c r="B106" s="4" t="s">
-        <v>405</v>
+        <v>364</v>
       </c>
       <c r="C106" s="4" t="s">
         <v>119</v>
       </c>
       <c r="D106" s="3" t="s">
-        <v>440</v>
+        <v>438</v>
       </c>
       <c r="E106" s="3" t="s">
-        <v>441</v>
-      </c>
-      <c r="F106" s="3"/>
-    </row>
-    <row r="107" spans="1:6" ht="120" x14ac:dyDescent="0.25">
-      <c r="B107" s="4" t="s">
-        <v>406</v>
-      </c>
-      <c r="C107" s="4" t="s">
-        <v>119</v>
-      </c>
-      <c r="D107" s="3" t="s">
-        <v>442</v>
-      </c>
-      <c r="E107" s="3" t="s">
-        <v>443</v>
-      </c>
+        <v>439</v>
+      </c>
+      <c r="F106" s="3" t="s">
+        <v>437</v>
+      </c>
+    </row>
+    <row r="107" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A107" s="17" t="s">
+        <v>403</v>
+      </c>
+      <c r="D107" s="3"/>
+      <c r="E107" s="3"/>
       <c r="F107" s="3"/>
     </row>
-    <row r="108" spans="1:6" ht="135" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:6" ht="75" x14ac:dyDescent="0.25">
+      <c r="A108" s="20" t="s">
+        <v>451</v>
+      </c>
       <c r="B108" s="4" t="s">
-        <v>407</v>
+        <v>405</v>
       </c>
       <c r="C108" s="4" t="s">
         <v>119</v>
       </c>
       <c r="D108" s="3" t="s">
-        <v>446</v>
+        <v>440</v>
       </c>
       <c r="E108" s="3" t="s">
-        <v>447</v>
+        <v>441</v>
       </c>
       <c r="F108" s="3"/>
     </row>
-    <row r="109" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+    <row r="109" spans="1:6" ht="120" x14ac:dyDescent="0.25">
+      <c r="A109" s="5" t="s">
+        <v>406</v>
+      </c>
       <c r="B109" s="4" t="s">
-        <v>408</v>
+        <v>406</v>
       </c>
       <c r="C109" s="4" t="s">
         <v>119</v>
       </c>
       <c r="D109" s="3" t="s">
-        <v>444</v>
+        <v>442</v>
       </c>
       <c r="E109" s="3" t="s">
-        <v>445</v>
+        <v>443</v>
       </c>
       <c r="F109" s="3"/>
     </row>
-    <row r="110" spans="1:6" ht="240" x14ac:dyDescent="0.25">
+    <row r="110" spans="1:6" ht="135" x14ac:dyDescent="0.25">
+      <c r="A110" s="20"/>
       <c r="B110" s="4" t="s">
-        <v>409</v>
+        <v>407</v>
       </c>
       <c r="C110" s="4" t="s">
         <v>119</v>
       </c>
       <c r="D110" s="3" t="s">
-        <v>448</v>
+        <v>446</v>
       </c>
       <c r="E110" s="3" t="s">
-        <v>449</v>
+        <v>447</v>
       </c>
       <c r="F110" s="3"/>
     </row>
-    <row r="111" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="111" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+      <c r="A111" s="20" t="s">
+        <v>450</v>
+      </c>
       <c r="B111" s="4" t="s">
-        <v>410</v>
+        <v>408</v>
       </c>
       <c r="C111" s="4" t="s">
         <v>119</v>
       </c>
-      <c r="D111" s="3"/>
-      <c r="E111" s="3"/>
+      <c r="D111" s="3" t="s">
+        <v>444</v>
+      </c>
+      <c r="E111" s="3" t="s">
+        <v>445</v>
+      </c>
       <c r="F111" s="3"/>
     </row>
-    <row r="112" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="112" spans="1:6" ht="240" x14ac:dyDescent="0.25">
+      <c r="A112" s="20" t="s">
+        <v>453</v>
+      </c>
       <c r="B112" s="4" t="s">
-        <v>411</v>
+        <v>409</v>
       </c>
       <c r="C112" s="4" t="s">
-        <v>142</v>
-      </c>
-      <c r="D112" s="3"/>
-      <c r="E112" s="3"/>
+        <v>119</v>
+      </c>
+      <c r="D112" s="3" t="s">
+        <v>448</v>
+      </c>
+      <c r="E112" s="3" t="s">
+        <v>449</v>
+      </c>
       <c r="F112" s="3"/>
     </row>
-    <row r="113" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="113" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A113" s="20"/>
       <c r="B113" s="4" t="s">
-        <v>412</v>
+        <v>410</v>
       </c>
       <c r="C113" s="4" t="s">
-        <v>142</v>
+        <v>119</v>
       </c>
       <c r="D113" s="3"/>
       <c r="E113" s="3"/>
       <c r="F113" s="3"/>
     </row>
-    <row r="114" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="114" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A114" s="20"/>
       <c r="B114" s="4" t="s">
-        <v>413</v>
+        <v>411</v>
       </c>
       <c r="C114" s="4" t="s">
-        <v>119</v>
+        <v>142</v>
       </c>
       <c r="D114" s="3"/>
       <c r="E114" s="3"/>
       <c r="F114" s="3"/>
     </row>
-    <row r="115" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="115" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A115" s="20"/>
       <c r="B115" s="4" t="s">
-        <v>414</v>
+        <v>412</v>
       </c>
       <c r="C115" s="4" t="s">
         <v>142</v>
@@ -4259,73 +4310,88 @@
       <c r="E115" s="3"/>
       <c r="F115" s="3"/>
     </row>
-    <row r="116" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="116" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A116" s="20"/>
       <c r="B116" s="4" t="s">
-        <v>404</v>
+        <v>413</v>
       </c>
       <c r="C116" s="4" t="s">
-        <v>142</v>
+        <v>119</v>
       </c>
       <c r="D116" s="3"/>
       <c r="E116" s="3"/>
       <c r="F116" s="3"/>
     </row>
-    <row r="117" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="117" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A117" s="20"/>
+      <c r="B117" s="4" t="s">
+        <v>414</v>
+      </c>
+      <c r="C117" s="4" t="s">
+        <v>142</v>
+      </c>
       <c r="D117" s="3"/>
       <c r="E117" s="3"/>
       <c r="F117" s="3"/>
     </row>
-    <row r="118" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="118" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A118" s="20"/>
+      <c r="B118" s="4" t="s">
+        <v>404</v>
+      </c>
+      <c r="C118" s="4" t="s">
+        <v>142</v>
+      </c>
       <c r="D118" s="3"/>
       <c r="E118" s="3"/>
       <c r="F118" s="3"/>
     </row>
-    <row r="119" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="119" spans="1:6" x14ac:dyDescent="0.25">
       <c r="D119" s="3"/>
       <c r="E119" s="3"/>
       <c r="F119" s="3"/>
     </row>
-    <row r="120" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="120" spans="1:6" x14ac:dyDescent="0.25">
       <c r="D120" s="3"/>
       <c r="E120" s="3"/>
       <c r="F120" s="3"/>
     </row>
-    <row r="121" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="121" spans="1:6" x14ac:dyDescent="0.25">
       <c r="D121" s="3"/>
       <c r="E121" s="3"/>
       <c r="F121" s="3"/>
     </row>
-    <row r="122" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="122" spans="1:6" x14ac:dyDescent="0.25">
       <c r="D122" s="3"/>
       <c r="E122" s="3"/>
       <c r="F122" s="3"/>
     </row>
-    <row r="123" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="123" spans="1:6" x14ac:dyDescent="0.25">
       <c r="D123" s="3"/>
       <c r="E123" s="3"/>
       <c r="F123" s="3"/>
     </row>
-    <row r="124" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="124" spans="1:6" x14ac:dyDescent="0.25">
       <c r="D124" s="3"/>
       <c r="E124" s="3"/>
       <c r="F124" s="3"/>
     </row>
-    <row r="125" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="125" spans="1:6" x14ac:dyDescent="0.25">
       <c r="D125" s="3"/>
       <c r="E125" s="3"/>
       <c r="F125" s="3"/>
     </row>
-    <row r="126" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="126" spans="1:6" x14ac:dyDescent="0.25">
       <c r="D126" s="3"/>
       <c r="E126" s="3"/>
       <c r="F126" s="3"/>
     </row>
-    <row r="127" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="127" spans="1:6" x14ac:dyDescent="0.25">
       <c r="D127" s="3"/>
       <c r="E127" s="3"/>
       <c r="F127" s="3"/>
     </row>
-    <row r="128" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="128" spans="1:6" x14ac:dyDescent="0.25">
       <c r="D128" s="3"/>
       <c r="E128" s="3"/>
       <c r="F128" s="3"/>
@@ -8524,6 +8590,16 @@
       <c r="D967" s="3"/>
       <c r="E967" s="3"/>
       <c r="F967" s="3"/>
+    </row>
+    <row r="968" spans="4:6" x14ac:dyDescent="0.25">
+      <c r="D968" s="3"/>
+      <c r="E968" s="3"/>
+      <c r="F968" s="3"/>
+    </row>
+    <row r="969" spans="4:6" x14ac:dyDescent="0.25">
+      <c r="D969" s="3"/>
+      <c r="E969" s="3"/>
+      <c r="F969" s="3"/>
     </row>
   </sheetData>
   <mergeCells count="1">

</xml_diff>

<commit_message>
Finished interleaving string problem
</commit_message>
<xml_diff>
--- a/LeetCode.xlsx
+++ b/LeetCode.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\EricS\Documents\VSCode Projects\LeetcodeGrind\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{32C898DB-9BC5-4D95-A8EA-DBCC643C2C7F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{53ADF0A8-4A0D-4E8A-9740-8E64816759EE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="3" xr2:uid="{02D29AA1-7085-42F6-B3D4-4C0365DA5453}"/>
   </bookViews>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="639" uniqueCount="454">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="689" uniqueCount="480">
   <si>
     <t>Roman to Integer:</t>
   </si>
@@ -1404,6 +1404,84 @@
   </si>
   <si>
     <t>0/1 Knapsack</t>
+  </si>
+  <si>
+    <t>Advanced Graphs</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Reconstruct Itinerary   </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Min Cost to Connect All Points   </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Network Delay Time   </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Swim In Rising Water   </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Alien Dictionary   </t>
+  </si>
+  <si>
+    <t>Cheapest Flights Within K Stops</t>
+  </si>
+  <si>
+    <t>REMEMBER TO DO ADVANCED GRAPHS</t>
+  </si>
+  <si>
+    <t>Greedy</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Maximum Subarray   </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Jump Game   </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Jump Game II   </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Gas Station   </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Hand of Straights   </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Merge Triplets to Form Target Triplet   </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Partition Labels   </t>
+  </si>
+  <si>
+    <t>Valid Parenthesis String</t>
+  </si>
+  <si>
+    <t>Intervals</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Insert Interval   </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Merge Intervals   </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Non Overlapping Intervals   </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Meeting Rooms   </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Meeting Rooms II   </t>
+  </si>
+  <si>
+    <t>Minimum Interval to Include Each Query</t>
+  </si>
+  <si>
+    <t>given 2 small strings and a big string, check if you can create big string from interleaving small strings</t>
+  </si>
+  <si>
+    <t>Literally just recursion with memory, if left matches you increment left pointer and recurse, if right matches you do the same, and you use an or on boolean to see what happens, then you save to a vector thingy and see how everything goes</t>
   </si>
 </sst>
 </file>
@@ -1457,7 +1535,6 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
       <sz val="11"/>
       <color theme="0" tint="-0.14999847407452621"/>
       <name val="Calibri"/>
@@ -1466,6 +1543,15 @@
     </font>
     <font>
       <sz val="11"/>
+      <color theme="2"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <u/>
+      <sz val="11"/>
       <color theme="0" tint="-0.14999847407452621"/>
       <name val="Calibri"/>
       <family val="2"/>
@@ -1473,13 +1559,7 @@
     </font>
     <font>
       <b/>
-      <sz val="11"/>
-      <color theme="2"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
+      <u/>
       <sz val="11"/>
       <color theme="2"/>
       <name val="Calibri"/>
@@ -1534,22 +1614,22 @@
     <xf numFmtId="49" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
+    <xf numFmtId="49" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="49" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" shrinkToFit="1"/>
+    </xf>
     <xf numFmtId="49" fontId="7" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
     <xf numFmtId="49" fontId="7" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1" readingOrder="1"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="9" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="49" fontId="9" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="9" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="7" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyAlignment="1">
@@ -1561,17 +1641,17 @@
     <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="8" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="8" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="9" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -2473,8 +2553,8 @@
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:G969"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A110" zoomScaleNormal="122" workbookViewId="0">
-      <selection activeCell="B124" sqref="B124"/>
+    <sheetView tabSelected="1" topLeftCell="A115" zoomScale="81" zoomScaleNormal="122" workbookViewId="0">
+      <selection activeCell="D120" sqref="D120"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2524,7 +2604,7 @@
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A3" s="17" t="s">
+      <c r="A3" s="16" t="s">
         <v>109</v>
       </c>
       <c r="B3" s="4" t="s">
@@ -2542,6 +2622,7 @@
       <c r="F3" s="3"/>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A4" s="16"/>
       <c r="B4" s="4" t="s">
         <v>28</v>
       </c>
@@ -2557,6 +2638,7 @@
       <c r="F4" s="3"/>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A5" s="16"/>
       <c r="B5" s="4" t="s">
         <v>36</v>
       </c>
@@ -2572,6 +2654,7 @@
       <c r="F5" s="3"/>
     </row>
     <row r="6" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="A6" s="16"/>
       <c r="B6" s="4" t="s">
         <v>114</v>
       </c>
@@ -2589,6 +2672,7 @@
       </c>
     </row>
     <row r="7" spans="1:7" ht="75" x14ac:dyDescent="0.25">
+      <c r="A7" s="16"/>
       <c r="B7" s="4" t="s">
         <v>115</v>
       </c>
@@ -2604,6 +2688,7 @@
       <c r="F7" s="3"/>
     </row>
     <row r="8" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="A8" s="16"/>
       <c r="B8" s="4" t="s">
         <v>116</v>
       </c>
@@ -2621,6 +2706,7 @@
       </c>
     </row>
     <row r="9" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="A9" s="16"/>
       <c r="B9" s="4" t="s">
         <v>117</v>
       </c>
@@ -2636,6 +2722,7 @@
       <c r="F9" s="3"/>
     </row>
     <row r="10" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="A10" s="16"/>
       <c r="B10" s="4" t="s">
         <v>118</v>
       </c>
@@ -2653,7 +2740,7 @@
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A11" s="17" t="s">
+      <c r="A11" s="16" t="s">
         <v>137</v>
       </c>
       <c r="B11" s="4" t="s">
@@ -2671,6 +2758,7 @@
       <c r="F11" s="3"/>
     </row>
     <row r="12" spans="1:7" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A12" s="16"/>
       <c r="B12" s="4" t="s">
         <v>138</v>
       </c>
@@ -2688,6 +2776,7 @@
       </c>
     </row>
     <row r="13" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="A13" s="16"/>
       <c r="B13" s="4" t="s">
         <v>139</v>
       </c>
@@ -2703,6 +2792,7 @@
       <c r="F13" s="3"/>
     </row>
     <row r="14" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="A14" s="16"/>
       <c r="B14" s="4" t="s">
         <v>140</v>
       </c>
@@ -2718,6 +2808,7 @@
       <c r="F14" s="3"/>
     </row>
     <row r="15" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+      <c r="A15" s="16"/>
       <c r="B15" s="4" t="s">
         <v>141</v>
       </c>
@@ -2733,7 +2824,7 @@
       <c r="F15" s="3"/>
     </row>
     <row r="16" spans="1:7" ht="30" x14ac:dyDescent="0.25">
-      <c r="A16" s="17" t="s">
+      <c r="A16" s="16" t="s">
         <v>153</v>
       </c>
       <c r="B16" s="4" t="s">
@@ -2751,6 +2842,7 @@
       <c r="F16" s="3"/>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A17" s="16"/>
       <c r="B17" s="4" t="s">
         <v>155</v>
       </c>
@@ -2768,6 +2860,7 @@
       </c>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A18" s="16"/>
       <c r="B18" s="4" t="s">
         <v>156</v>
       </c>
@@ -2783,6 +2876,7 @@
       <c r="F18" s="3"/>
     </row>
     <row r="19" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A19" s="16"/>
       <c r="B19" s="4" t="s">
         <v>157</v>
       </c>
@@ -2798,6 +2892,7 @@
       <c r="F19" s="3"/>
     </row>
     <row r="20" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+      <c r="A20" s="16"/>
       <c r="B20" s="4" t="s">
         <v>158</v>
       </c>
@@ -2813,6 +2908,7 @@
       <c r="F20" s="3"/>
     </row>
     <row r="21" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+      <c r="A21" s="16"/>
       <c r="B21" s="4" t="s">
         <v>159</v>
       </c>
@@ -2830,6 +2926,7 @@
       </c>
     </row>
     <row r="22" spans="1:6" ht="60" x14ac:dyDescent="0.25">
+      <c r="A22" s="16"/>
       <c r="B22" s="4" t="s">
         <v>154</v>
       </c>
@@ -2847,7 +2944,7 @@
       </c>
     </row>
     <row r="23" spans="1:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="A23" s="17" t="s">
+      <c r="A23" s="16" t="s">
         <v>169</v>
       </c>
       <c r="B23" s="4" t="s">
@@ -2865,6 +2962,7 @@
       <c r="F23" s="3"/>
     </row>
     <row r="24" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A24" s="16"/>
       <c r="B24" s="4" t="s">
         <v>171</v>
       </c>
@@ -2880,6 +2978,7 @@
       <c r="F24" s="3"/>
     </row>
     <row r="25" spans="1:6" ht="60" x14ac:dyDescent="0.25">
+      <c r="A25" s="16"/>
       <c r="B25" s="4" t="s">
         <v>172</v>
       </c>
@@ -2895,6 +2994,7 @@
       <c r="F25" s="3"/>
     </row>
     <row r="26" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+      <c r="A26" s="16"/>
       <c r="B26" s="4" t="s">
         <v>173</v>
       </c>
@@ -2910,6 +3010,7 @@
       <c r="F26" s="3"/>
     </row>
     <row r="27" spans="1:6" ht="60" x14ac:dyDescent="0.25">
+      <c r="A27" s="16"/>
       <c r="B27" s="4" t="s">
         <v>174</v>
       </c>
@@ -2925,6 +3026,7 @@
       <c r="F27" s="3"/>
     </row>
     <row r="28" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+      <c r="A28" s="16"/>
       <c r="B28" s="4" t="s">
         <v>175</v>
       </c>
@@ -2942,6 +3044,7 @@
       </c>
     </row>
     <row r="29" spans="1:6" ht="150" x14ac:dyDescent="0.25">
+      <c r="A29" s="16"/>
       <c r="B29" s="4" t="s">
         <v>176</v>
       </c>
@@ -2959,7 +3062,7 @@
       </c>
     </row>
     <row r="30" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A30" s="17" t="s">
+      <c r="A30" s="16" t="s">
         <v>168</v>
       </c>
       <c r="B30" s="4" t="s">
@@ -2977,6 +3080,7 @@
       <c r="F30" s="3"/>
     </row>
     <row r="31" spans="1:6" ht="60" x14ac:dyDescent="0.25">
+      <c r="A31" s="16"/>
       <c r="B31" s="4" t="s">
         <v>178</v>
       </c>
@@ -2992,6 +3096,7 @@
       <c r="F31" s="3"/>
     </row>
     <row r="32" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+      <c r="A32" s="16"/>
       <c r="B32" s="4" t="s">
         <v>179</v>
       </c>
@@ -3009,6 +3114,7 @@
       </c>
     </row>
     <row r="33" spans="1:6" ht="60" x14ac:dyDescent="0.25">
+      <c r="A33" s="16"/>
       <c r="B33" s="4" t="s">
         <v>180</v>
       </c>
@@ -3024,6 +3130,7 @@
       <c r="F33" s="3"/>
     </row>
     <row r="34" spans="1:6" ht="90" x14ac:dyDescent="0.25">
+      <c r="A34" s="16"/>
       <c r="B34" s="4" t="s">
         <v>181</v>
       </c>
@@ -3039,6 +3146,7 @@
       <c r="F34" s="3"/>
     </row>
     <row r="35" spans="1:6" ht="90" x14ac:dyDescent="0.25">
+      <c r="A35" s="16"/>
       <c r="B35" s="4" t="s">
         <v>182</v>
       </c>
@@ -3054,7 +3162,7 @@
       <c r="F35" s="3"/>
     </row>
     <row r="36" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A36" s="17" t="s">
+      <c r="A36" s="16" t="s">
         <v>183</v>
       </c>
       <c r="B36" s="4" t="s">
@@ -3072,6 +3180,7 @@
       <c r="F36" s="3"/>
     </row>
     <row r="37" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A37" s="16"/>
       <c r="B37" s="4" t="s">
         <v>186</v>
       </c>
@@ -3089,6 +3198,7 @@
       </c>
     </row>
     <row r="38" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A38" s="16"/>
       <c r="B38" s="4" t="s">
         <v>187</v>
       </c>
@@ -3104,6 +3214,7 @@
       <c r="F38" s="3"/>
     </row>
     <row r="39" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+      <c r="A39" s="16"/>
       <c r="B39" s="4" t="s">
         <v>188</v>
       </c>
@@ -3119,6 +3230,7 @@
       <c r="F39" s="3"/>
     </row>
     <row r="40" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A40" s="16"/>
       <c r="B40" s="4" t="s">
         <v>189</v>
       </c>
@@ -3134,6 +3246,7 @@
       <c r="F40" s="3"/>
     </row>
     <row r="41" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+      <c r="A41" s="16"/>
       <c r="B41" s="4" t="s">
         <v>190</v>
       </c>
@@ -3149,6 +3262,7 @@
       <c r="F41" s="3"/>
     </row>
     <row r="42" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A42" s="16"/>
       <c r="B42" s="4" t="s">
         <v>191</v>
       </c>
@@ -3164,6 +3278,7 @@
       <c r="F42" s="3"/>
     </row>
     <row r="43" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A43" s="16"/>
       <c r="B43" s="6" t="s">
         <v>192</v>
       </c>
@@ -3179,6 +3294,7 @@
       <c r="F43" s="3"/>
     </row>
     <row r="44" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A44" s="16"/>
       <c r="B44" s="4" t="s">
         <v>193</v>
       </c>
@@ -3194,6 +3310,7 @@
       <c r="F44" s="3"/>
     </row>
     <row r="45" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A45" s="16"/>
       <c r="B45" s="4" t="s">
         <v>194</v>
       </c>
@@ -3209,6 +3326,7 @@
       <c r="F45" s="3"/>
     </row>
     <row r="46" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+      <c r="A46" s="16"/>
       <c r="B46" s="4" t="s">
         <v>184</v>
       </c>
@@ -3224,7 +3342,7 @@
       <c r="F46" s="3"/>
     </row>
     <row r="47" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A47" s="17" t="s">
+      <c r="A47" s="16" t="s">
         <v>250</v>
       </c>
       <c r="B47" s="4" t="s">
@@ -3242,6 +3360,7 @@
       <c r="F47" s="3"/>
     </row>
     <row r="48" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A48" s="16"/>
       <c r="B48" s="4" t="s">
         <v>252</v>
       </c>
@@ -3257,6 +3376,7 @@
       <c r="F48" s="3"/>
     </row>
     <row r="49" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A49" s="16"/>
       <c r="B49" s="4" t="s">
         <v>253</v>
       </c>
@@ -3272,6 +3392,7 @@
       <c r="F49" s="3"/>
     </row>
     <row r="50" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A50" s="16"/>
       <c r="B50" s="4" t="s">
         <v>254</v>
       </c>
@@ -3287,6 +3408,7 @@
       <c r="F50" s="3"/>
     </row>
     <row r="51" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A51" s="16"/>
       <c r="B51" s="4" t="s">
         <v>255</v>
       </c>
@@ -3302,6 +3424,7 @@
       <c r="F51" s="3"/>
     </row>
     <row r="52" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A52" s="16"/>
       <c r="B52" s="4" t="s">
         <v>256</v>
       </c>
@@ -3317,6 +3440,7 @@
       <c r="F52" s="3"/>
     </row>
     <row r="53" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A53" s="16"/>
       <c r="B53" s="4" t="s">
         <v>257</v>
       </c>
@@ -3332,6 +3456,7 @@
       <c r="F53" s="3"/>
     </row>
     <row r="54" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+      <c r="A54" s="16"/>
       <c r="B54" s="4" t="s">
         <v>258</v>
       </c>
@@ -3347,6 +3472,7 @@
       <c r="F54" s="3"/>
     </row>
     <row r="55" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A55" s="16"/>
       <c r="B55" s="4" t="s">
         <v>259</v>
       </c>
@@ -3362,6 +3488,7 @@
       <c r="F55" s="3"/>
     </row>
     <row r="56" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+      <c r="A56" s="16"/>
       <c r="B56" s="4" t="s">
         <v>260</v>
       </c>
@@ -3377,6 +3504,7 @@
       <c r="F56" s="3"/>
     </row>
     <row r="57" spans="1:6" ht="60" x14ac:dyDescent="0.25">
+      <c r="A57" s="16"/>
       <c r="B57" s="4" t="s">
         <v>261</v>
       </c>
@@ -3394,6 +3522,7 @@
       </c>
     </row>
     <row r="58" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+      <c r="A58" s="16"/>
       <c r="B58" s="4" t="s">
         <v>262</v>
       </c>
@@ -3409,6 +3538,7 @@
       <c r="F58" s="3"/>
     </row>
     <row r="59" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+      <c r="A59" s="16"/>
       <c r="B59" s="4" t="s">
         <v>263</v>
       </c>
@@ -3424,6 +3554,7 @@
       <c r="F59" s="3"/>
     </row>
     <row r="60" spans="1:6" ht="60" x14ac:dyDescent="0.25">
+      <c r="A60" s="16"/>
       <c r="B60" s="4" t="s">
         <v>264</v>
       </c>
@@ -3441,7 +3572,7 @@
       </c>
     </row>
     <row r="61" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A61" s="18"/>
+      <c r="A61" s="20"/>
       <c r="B61" s="9" t="s">
         <v>265</v>
       </c>
@@ -3457,7 +3588,7 @@
       <c r="F61" s="3"/>
     </row>
     <row r="62" spans="1:6" ht="105" x14ac:dyDescent="0.25">
-      <c r="A62" s="17" t="s">
+      <c r="A62" s="16" t="s">
         <v>290</v>
       </c>
       <c r="B62" s="4" t="s">
@@ -3477,6 +3608,7 @@
       </c>
     </row>
     <row r="63" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+      <c r="A63" s="16"/>
       <c r="B63" s="4" t="s">
         <v>292</v>
       </c>
@@ -3492,6 +3624,7 @@
       <c r="F63" s="3"/>
     </row>
     <row r="64" spans="1:6" ht="75" x14ac:dyDescent="0.25">
+      <c r="A64" s="16"/>
       <c r="B64" s="4" t="s">
         <v>293</v>
       </c>
@@ -3509,7 +3642,7 @@
       </c>
     </row>
     <row r="65" spans="1:7" ht="45" x14ac:dyDescent="0.25">
-      <c r="A65" s="17" t="s">
+      <c r="A65" s="16" t="s">
         <v>294</v>
       </c>
       <c r="B65" s="4" t="s">
@@ -3527,6 +3660,7 @@
       <c r="F65" s="3"/>
     </row>
     <row r="66" spans="1:7" ht="69" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A66" s="16"/>
       <c r="B66" s="4" t="s">
         <v>296</v>
       </c>
@@ -3544,6 +3678,7 @@
       </c>
     </row>
     <row r="67" spans="1:7" ht="90" x14ac:dyDescent="0.25">
+      <c r="A67" s="16"/>
       <c r="B67" s="4" t="s">
         <v>297</v>
       </c>
@@ -3559,6 +3694,7 @@
       <c r="F67" s="11"/>
     </row>
     <row r="68" spans="1:7" ht="75" x14ac:dyDescent="0.25">
+      <c r="A68" s="16"/>
       <c r="B68" s="4" t="s">
         <v>298</v>
       </c>
@@ -3574,6 +3710,7 @@
       <c r="F68" s="3"/>
     </row>
     <row r="69" spans="1:7" ht="63" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A69" s="16"/>
       <c r="B69" s="4" t="s">
         <v>299</v>
       </c>
@@ -3589,6 +3726,7 @@
       <c r="F69" s="3"/>
     </row>
     <row r="70" spans="1:7" ht="90" x14ac:dyDescent="0.25">
+      <c r="A70" s="16"/>
       <c r="B70" s="4" t="s">
         <v>300</v>
       </c>
@@ -3604,6 +3742,7 @@
       <c r="F70" s="3"/>
     </row>
     <row r="71" spans="1:7" ht="64.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A71" s="16"/>
       <c r="B71" s="4" t="s">
         <v>301</v>
       </c>
@@ -3619,6 +3758,7 @@
       <c r="F71" s="3"/>
     </row>
     <row r="72" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+      <c r="A72" s="16"/>
       <c r="B72" s="4" t="s">
         <v>302</v>
       </c>
@@ -3634,6 +3774,7 @@
       <c r="F72" s="3"/>
     </row>
     <row r="73" spans="1:7" ht="140.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A73" s="16"/>
       <c r="B73" s="4" t="s">
         <v>303</v>
       </c>
@@ -3649,7 +3790,7 @@
       <c r="F73" s="3"/>
     </row>
     <row r="74" spans="1:7" ht="45" x14ac:dyDescent="0.25">
-      <c r="A74" s="17" t="s">
+      <c r="A74" s="16" t="s">
         <v>330</v>
       </c>
       <c r="B74" s="4" t="s">
@@ -3667,6 +3808,7 @@
       <c r="F74" s="3"/>
     </row>
     <row r="75" spans="1:7" ht="60" x14ac:dyDescent="0.25">
+      <c r="A75" s="16"/>
       <c r="B75" s="4" t="s">
         <v>332</v>
       </c>
@@ -3682,6 +3824,7 @@
       <c r="F75" s="3"/>
     </row>
     <row r="76" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="A76" s="16"/>
       <c r="B76" s="4" t="s">
         <v>333</v>
       </c>
@@ -3699,6 +3842,7 @@
       </c>
     </row>
     <row r="77" spans="1:7" ht="82.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A77" s="16"/>
       <c r="B77" s="4" t="s">
         <v>334</v>
       </c>
@@ -3714,6 +3858,7 @@
       <c r="F77" s="3"/>
     </row>
     <row r="78" spans="1:7" ht="75.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A78" s="16"/>
       <c r="B78" s="4" t="s">
         <v>335</v>
       </c>
@@ -3729,7 +3874,7 @@
       <c r="F78" s="3"/>
     </row>
     <row r="79" spans="1:7" s="12" customFormat="1" ht="30" x14ac:dyDescent="0.25">
-      <c r="A79" s="19"/>
+      <c r="A79" s="21"/>
       <c r="B79" s="12" t="s">
         <v>336</v>
       </c>
@@ -3746,6 +3891,7 @@
       <c r="G79" s="14"/>
     </row>
     <row r="80" spans="1:7" ht="60" x14ac:dyDescent="0.25">
+      <c r="A80" s="16"/>
       <c r="B80" s="4" t="s">
         <v>337</v>
       </c>
@@ -3761,7 +3907,7 @@
       <c r="F80" s="3"/>
     </row>
     <row r="81" spans="1:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="A81" s="17" t="s">
+      <c r="A81" s="16" t="s">
         <v>338</v>
       </c>
       <c r="B81" s="4" t="s">
@@ -3781,6 +3927,7 @@
       </c>
     </row>
     <row r="82" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A82" s="16"/>
       <c r="B82" s="4" t="s">
         <v>340</v>
       </c>
@@ -3796,6 +3943,7 @@
       <c r="F82" s="3"/>
     </row>
     <row r="83" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A83" s="16"/>
       <c r="B83" s="4" t="s">
         <v>341</v>
       </c>
@@ -3811,6 +3959,7 @@
       <c r="F83" s="3"/>
     </row>
     <row r="84" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A84" s="16"/>
       <c r="B84" s="4" t="s">
         <v>342</v>
       </c>
@@ -3826,6 +3975,7 @@
       <c r="F84" s="3"/>
     </row>
     <row r="85" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+      <c r="A85" s="16"/>
       <c r="B85" s="4" t="s">
         <v>343</v>
       </c>
@@ -3841,6 +3991,7 @@
       <c r="F85" s="3"/>
     </row>
     <row r="86" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+      <c r="A86" s="16"/>
       <c r="B86" s="4" t="s">
         <v>344</v>
       </c>
@@ -3856,6 +4007,7 @@
       <c r="F86" s="3"/>
     </row>
     <row r="87" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A87" s="16"/>
       <c r="B87" s="4" t="s">
         <v>345</v>
       </c>
@@ -3871,6 +4023,7 @@
       <c r="F87" s="3"/>
     </row>
     <row r="88" spans="1:6" ht="75" x14ac:dyDescent="0.25">
+      <c r="A88" s="16"/>
       <c r="B88" s="4" t="s">
         <v>346</v>
       </c>
@@ -3888,6 +4041,7 @@
       </c>
     </row>
     <row r="89" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A89" s="16"/>
       <c r="B89" s="4" t="s">
         <v>347</v>
       </c>
@@ -3903,6 +4057,7 @@
       <c r="F89" s="3"/>
     </row>
     <row r="90" spans="1:6" ht="60" x14ac:dyDescent="0.25">
+      <c r="A90" s="16"/>
       <c r="B90" s="4" t="s">
         <v>348</v>
       </c>
@@ -3918,6 +4073,7 @@
       <c r="F90" s="3"/>
     </row>
     <row r="91" spans="1:6" ht="75" x14ac:dyDescent="0.25">
+      <c r="A91" s="16"/>
       <c r="B91" s="4" t="s">
         <v>349</v>
       </c>
@@ -3933,6 +4089,7 @@
       <c r="F91" s="3"/>
     </row>
     <row r="92" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A92" s="16"/>
       <c r="B92" s="4" t="s">
         <v>350</v>
       </c>
@@ -3948,6 +4105,7 @@
       <c r="F92" s="3"/>
     </row>
     <row r="93" spans="1:6" ht="75" x14ac:dyDescent="0.25">
+      <c r="A93" s="16"/>
       <c r="B93" s="4" t="s">
         <v>351</v>
       </c>
@@ -3963,515 +4121,643 @@
       <c r="F93" s="3"/>
     </row>
     <row r="94" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A94" s="17" t="s">
+      <c r="A94" s="16" t="s">
+        <v>454</v>
+      </c>
+      <c r="B94" s="4" t="s">
+        <v>455</v>
+      </c>
+      <c r="C94" s="4" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="95" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B95" s="4" t="s">
+        <v>456</v>
+      </c>
+      <c r="C95" s="4" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="96" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B96" s="4" t="s">
+        <v>457</v>
+      </c>
+      <c r="C96" s="4" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="97" spans="1:6" ht="75.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B97" s="4" t="s">
+        <v>458</v>
+      </c>
+      <c r="C97" s="4" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="98" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B98" s="4" t="s">
+        <v>459</v>
+      </c>
+      <c r="C98" s="4" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="99" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B99" s="4" t="s">
+        <v>460</v>
+      </c>
+      <c r="C99" s="4" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="100" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A100" s="16" t="s">
         <v>352</v>
       </c>
-      <c r="D94" s="3"/>
-      <c r="E94" s="3"/>
-      <c r="F94" s="3"/>
-    </row>
-    <row r="95" spans="1:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="A95" s="20" t="s">
+      <c r="D100" s="3"/>
+      <c r="E100" s="3"/>
+      <c r="F100" s="3"/>
+    </row>
+    <row r="101" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A101" s="18" t="s">
         <v>452</v>
       </c>
-      <c r="B95" s="4" t="s">
+      <c r="B101" s="4" t="s">
         <v>353</v>
       </c>
-      <c r="C95" s="4" t="s">
+      <c r="C101" s="4" t="s">
         <v>112</v>
       </c>
-      <c r="D95" s="3" t="s">
+      <c r="D101" s="3" t="s">
         <v>415</v>
       </c>
-      <c r="E95" s="3" t="s">
+      <c r="E101" s="3" t="s">
         <v>416</v>
       </c>
-      <c r="F95" s="3"/>
-    </row>
-    <row r="96" spans="1:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="A96" s="20" t="s">
+      <c r="F101" s="3"/>
+    </row>
+    <row r="102" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A102" s="18" t="s">
         <v>452</v>
       </c>
-      <c r="B96" s="4" t="s">
+      <c r="B102" s="4" t="s">
         <v>354</v>
       </c>
-      <c r="C96" s="4" t="s">
+      <c r="C102" s="4" t="s">
         <v>112</v>
       </c>
-      <c r="D96" s="3" t="s">
+      <c r="D102" s="3" t="s">
         <v>417</v>
       </c>
-      <c r="E96" s="3" t="s">
+      <c r="E102" s="3" t="s">
         <v>418</v>
       </c>
-      <c r="F96" s="3"/>
-    </row>
-    <row r="97" spans="1:6" ht="75.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A97" s="20" t="s">
+      <c r="F102" s="3"/>
+    </row>
+    <row r="103" spans="1:6" ht="90" x14ac:dyDescent="0.25">
+      <c r="A103" s="18" t="s">
         <v>452</v>
       </c>
-      <c r="B97" s="4" t="s">
+      <c r="B103" s="4" t="s">
         <v>355</v>
       </c>
-      <c r="C97" s="4" t="s">
-        <v>119</v>
-      </c>
-      <c r="D97" s="3" t="s">
+      <c r="C103" s="4" t="s">
+        <v>119</v>
+      </c>
+      <c r="D103" s="3" t="s">
         <v>419</v>
       </c>
-      <c r="E97" s="3" t="s">
+      <c r="E103" s="3" t="s">
         <v>422</v>
       </c>
-      <c r="F97" s="3"/>
-    </row>
-    <row r="98" spans="1:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="A98" s="20" t="s">
+      <c r="F103" s="3"/>
+    </row>
+    <row r="104" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A104" s="18" t="s">
         <v>452</v>
       </c>
-      <c r="B98" s="4" t="s">
+      <c r="B104" s="4" t="s">
         <v>356</v>
       </c>
-      <c r="C98" s="4" t="s">
-        <v>119</v>
-      </c>
-      <c r="D98" s="3" t="s">
+      <c r="C104" s="4" t="s">
+        <v>119</v>
+      </c>
+      <c r="D104" s="3" t="s">
         <v>420</v>
       </c>
-      <c r="E98" s="3" t="s">
+      <c r="E104" s="3" t="s">
         <v>421</v>
       </c>
-      <c r="F98" s="3"/>
-    </row>
-    <row r="99" spans="1:6" ht="60" x14ac:dyDescent="0.25">
-      <c r="A99" s="21"/>
-      <c r="B99" s="4" t="s">
+      <c r="F104" s="3"/>
+    </row>
+    <row r="105" spans="1:6" ht="60" x14ac:dyDescent="0.25">
+      <c r="A105" s="19"/>
+      <c r="B105" s="4" t="s">
         <v>357</v>
       </c>
-      <c r="C99" s="4" t="s">
-        <v>119</v>
-      </c>
-      <c r="D99" s="3" t="s">
+      <c r="C105" s="4" t="s">
+        <v>119</v>
+      </c>
+      <c r="D105" s="3" t="s">
         <v>423</v>
       </c>
-      <c r="E99" s="3" t="s">
+      <c r="E105" s="3" t="s">
         <v>424</v>
       </c>
-      <c r="F99" s="3"/>
-    </row>
-    <row r="100" spans="1:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="A100" s="20"/>
-      <c r="B100" s="4" t="s">
+      <c r="F105" s="3"/>
+    </row>
+    <row r="106" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A106" s="18"/>
+      <c r="B106" s="4" t="s">
         <v>358</v>
       </c>
-      <c r="C100" s="4" t="s">
-        <v>119</v>
-      </c>
-      <c r="D100" s="3" t="s">
+      <c r="C106" s="4" t="s">
+        <v>119</v>
+      </c>
+      <c r="D106" s="3" t="s">
         <v>425</v>
       </c>
-      <c r="E100" s="3" t="s">
+      <c r="E106" s="3" t="s">
         <v>426</v>
       </c>
-      <c r="F100" s="3"/>
-    </row>
-    <row r="101" spans="1:6" ht="105" x14ac:dyDescent="0.25">
-      <c r="A101" s="20" t="s">
+      <c r="F106" s="3"/>
+    </row>
+    <row r="107" spans="1:6" ht="105" x14ac:dyDescent="0.25">
+      <c r="A107" s="18" t="s">
         <v>452</v>
       </c>
-      <c r="B101" s="4" t="s">
+      <c r="B107" s="4" t="s">
         <v>359</v>
       </c>
-      <c r="C101" s="4" t="s">
-        <v>119</v>
-      </c>
-      <c r="D101" s="3" t="s">
+      <c r="C107" s="4" t="s">
+        <v>119</v>
+      </c>
+      <c r="D107" s="3" t="s">
         <v>427</v>
       </c>
-      <c r="E101" s="3" t="s">
+      <c r="E107" s="3" t="s">
         <v>428</v>
       </c>
-      <c r="F101" s="3"/>
-    </row>
-    <row r="102" spans="1:6" ht="45" x14ac:dyDescent="0.25">
-      <c r="A102" s="20" t="s">
+      <c r="F107" s="3"/>
+    </row>
+    <row r="108" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+      <c r="A108" s="18" t="s">
         <v>450</v>
       </c>
-      <c r="B102" s="4" t="s">
+      <c r="B108" s="4" t="s">
         <v>360</v>
       </c>
-      <c r="C102" s="4" t="s">
-        <v>119</v>
-      </c>
-      <c r="D102" s="3" t="s">
+      <c r="C108" s="4" t="s">
+        <v>119</v>
+      </c>
+      <c r="D108" s="3" t="s">
         <v>429</v>
       </c>
-      <c r="E102" s="3" t="s">
+      <c r="E108" s="3" t="s">
         <v>430</v>
       </c>
-      <c r="F102" s="3"/>
-    </row>
-    <row r="103" spans="1:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="A103" s="20"/>
-      <c r="B103" s="4" t="s">
+      <c r="F108" s="3"/>
+    </row>
+    <row r="109" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A109" s="18"/>
+      <c r="B109" s="4" t="s">
         <v>361</v>
       </c>
-      <c r="C103" s="4" t="s">
-        <v>119</v>
-      </c>
-      <c r="D103" s="3" t="s">
+      <c r="C109" s="4" t="s">
+        <v>119</v>
+      </c>
+      <c r="D109" s="3" t="s">
         <v>431</v>
       </c>
-      <c r="E103" s="3" t="s">
+      <c r="E109" s="3" t="s">
         <v>432</v>
       </c>
-      <c r="F103" s="3"/>
-    </row>
-    <row r="104" spans="1:6" ht="45" x14ac:dyDescent="0.25">
-      <c r="A104" s="20"/>
-      <c r="B104" s="4" t="s">
+      <c r="F109" s="3"/>
+    </row>
+    <row r="110" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+      <c r="A110" s="18"/>
+      <c r="B110" s="4" t="s">
         <v>362</v>
       </c>
-      <c r="C104" s="4" t="s">
-        <v>119</v>
-      </c>
-      <c r="D104" s="3" t="s">
+      <c r="C110" s="4" t="s">
+        <v>119</v>
+      </c>
+      <c r="D110" s="3" t="s">
         <v>433</v>
       </c>
-      <c r="E104" s="3" t="s">
+      <c r="E110" s="3" t="s">
         <v>434</v>
       </c>
-      <c r="F104" s="3"/>
-    </row>
-    <row r="105" spans="1:6" ht="60" x14ac:dyDescent="0.25">
-      <c r="A105" s="20"/>
-      <c r="B105" s="4" t="s">
+      <c r="F110" s="3"/>
+    </row>
+    <row r="111" spans="1:6" ht="60" x14ac:dyDescent="0.25">
+      <c r="A111" s="18"/>
+      <c r="B111" s="4" t="s">
         <v>363</v>
       </c>
-      <c r="C105" s="4" t="s">
-        <v>119</v>
-      </c>
-      <c r="D105" s="3" t="s">
+      <c r="C111" s="4" t="s">
+        <v>119</v>
+      </c>
+      <c r="D111" s="3" t="s">
         <v>435</v>
       </c>
-      <c r="E105" s="3" t="s">
+      <c r="E111" s="3" t="s">
         <v>436</v>
       </c>
-      <c r="F105" s="3"/>
-    </row>
-    <row r="106" spans="1:6" ht="45" x14ac:dyDescent="0.25">
-      <c r="A106" s="20" t="s">
+      <c r="F111" s="3"/>
+    </row>
+    <row r="112" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+      <c r="A112" s="18" t="s">
         <v>453</v>
       </c>
-      <c r="B106" s="4" t="s">
+      <c r="B112" s="4" t="s">
         <v>364</v>
       </c>
-      <c r="C106" s="4" t="s">
-        <v>119</v>
-      </c>
-      <c r="D106" s="3" t="s">
+      <c r="C112" s="4" t="s">
+        <v>119</v>
+      </c>
+      <c r="D112" s="3" t="s">
         <v>438</v>
       </c>
-      <c r="E106" s="3" t="s">
+      <c r="E112" s="3" t="s">
         <v>439</v>
       </c>
-      <c r="F106" s="3" t="s">
+      <c r="F112" s="3" t="s">
         <v>437</v>
       </c>
     </row>
-    <row r="107" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A107" s="17" t="s">
+    <row r="113" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A113" s="16" t="s">
         <v>403</v>
-      </c>
-      <c r="D107" s="3"/>
-      <c r="E107" s="3"/>
-      <c r="F107" s="3"/>
-    </row>
-    <row r="108" spans="1:6" ht="75" x14ac:dyDescent="0.25">
-      <c r="A108" s="20" t="s">
-        <v>451</v>
-      </c>
-      <c r="B108" s="4" t="s">
-        <v>405</v>
-      </c>
-      <c r="C108" s="4" t="s">
-        <v>119</v>
-      </c>
-      <c r="D108" s="3" t="s">
-        <v>440</v>
-      </c>
-      <c r="E108" s="3" t="s">
-        <v>441</v>
-      </c>
-      <c r="F108" s="3"/>
-    </row>
-    <row r="109" spans="1:6" ht="120" x14ac:dyDescent="0.25">
-      <c r="A109" s="5" t="s">
-        <v>406</v>
-      </c>
-      <c r="B109" s="4" t="s">
-        <v>406</v>
-      </c>
-      <c r="C109" s="4" t="s">
-        <v>119</v>
-      </c>
-      <c r="D109" s="3" t="s">
-        <v>442</v>
-      </c>
-      <c r="E109" s="3" t="s">
-        <v>443</v>
-      </c>
-      <c r="F109" s="3"/>
-    </row>
-    <row r="110" spans="1:6" ht="135" x14ac:dyDescent="0.25">
-      <c r="A110" s="20"/>
-      <c r="B110" s="4" t="s">
-        <v>407</v>
-      </c>
-      <c r="C110" s="4" t="s">
-        <v>119</v>
-      </c>
-      <c r="D110" s="3" t="s">
-        <v>446</v>
-      </c>
-      <c r="E110" s="3" t="s">
-        <v>447</v>
-      </c>
-      <c r="F110" s="3"/>
-    </row>
-    <row r="111" spans="1:6" ht="45" x14ac:dyDescent="0.25">
-      <c r="A111" s="20" t="s">
-        <v>450</v>
-      </c>
-      <c r="B111" s="4" t="s">
-        <v>408</v>
-      </c>
-      <c r="C111" s="4" t="s">
-        <v>119</v>
-      </c>
-      <c r="D111" s="3" t="s">
-        <v>444</v>
-      </c>
-      <c r="E111" s="3" t="s">
-        <v>445</v>
-      </c>
-      <c r="F111" s="3"/>
-    </row>
-    <row r="112" spans="1:6" ht="240" x14ac:dyDescent="0.25">
-      <c r="A112" s="20" t="s">
-        <v>453</v>
-      </c>
-      <c r="B112" s="4" t="s">
-        <v>409</v>
-      </c>
-      <c r="C112" s="4" t="s">
-        <v>119</v>
-      </c>
-      <c r="D112" s="3" t="s">
-        <v>448</v>
-      </c>
-      <c r="E112" s="3" t="s">
-        <v>449</v>
-      </c>
-      <c r="F112" s="3"/>
-    </row>
-    <row r="113" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A113" s="20"/>
-      <c r="B113" s="4" t="s">
-        <v>410</v>
-      </c>
-      <c r="C113" s="4" t="s">
-        <v>119</v>
       </c>
       <c r="D113" s="3"/>
       <c r="E113" s="3"/>
       <c r="F113" s="3"/>
     </row>
-    <row r="114" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A114" s="20"/>
+    <row r="114" spans="1:6" ht="75" x14ac:dyDescent="0.25">
+      <c r="A114" s="18" t="s">
+        <v>451</v>
+      </c>
       <c r="B114" s="4" t="s">
+        <v>405</v>
+      </c>
+      <c r="C114" s="4" t="s">
+        <v>119</v>
+      </c>
+      <c r="D114" s="3" t="s">
+        <v>440</v>
+      </c>
+      <c r="E114" s="3" t="s">
+        <v>441</v>
+      </c>
+      <c r="F114" s="3"/>
+    </row>
+    <row r="115" spans="1:6" ht="120" x14ac:dyDescent="0.25">
+      <c r="A115" s="5" t="s">
+        <v>406</v>
+      </c>
+      <c r="B115" s="4" t="s">
+        <v>406</v>
+      </c>
+      <c r="C115" s="4" t="s">
+        <v>119</v>
+      </c>
+      <c r="D115" s="3" t="s">
+        <v>442</v>
+      </c>
+      <c r="E115" s="3" t="s">
+        <v>443</v>
+      </c>
+      <c r="F115" s="3"/>
+    </row>
+    <row r="116" spans="1:6" ht="135" x14ac:dyDescent="0.25">
+      <c r="A116" s="18"/>
+      <c r="B116" s="4" t="s">
+        <v>407</v>
+      </c>
+      <c r="C116" s="4" t="s">
+        <v>119</v>
+      </c>
+      <c r="D116" s="3" t="s">
+        <v>446</v>
+      </c>
+      <c r="E116" s="3" t="s">
+        <v>447</v>
+      </c>
+      <c r="F116" s="3"/>
+    </row>
+    <row r="117" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+      <c r="A117" s="18" t="s">
+        <v>450</v>
+      </c>
+      <c r="B117" s="4" t="s">
+        <v>408</v>
+      </c>
+      <c r="C117" s="4" t="s">
+        <v>119</v>
+      </c>
+      <c r="D117" s="3" t="s">
+        <v>444</v>
+      </c>
+      <c r="E117" s="3" t="s">
+        <v>445</v>
+      </c>
+      <c r="F117" s="3"/>
+    </row>
+    <row r="118" spans="1:6" ht="240" x14ac:dyDescent="0.25">
+      <c r="A118" s="18" t="s">
+        <v>453</v>
+      </c>
+      <c r="B118" s="4" t="s">
+        <v>409</v>
+      </c>
+      <c r="C118" s="4" t="s">
+        <v>119</v>
+      </c>
+      <c r="D118" s="3" t="s">
+        <v>448</v>
+      </c>
+      <c r="E118" s="3" t="s">
+        <v>449</v>
+      </c>
+      <c r="F118" s="3"/>
+    </row>
+    <row r="119" spans="1:6" ht="60" x14ac:dyDescent="0.25">
+      <c r="A119" s="18"/>
+      <c r="B119" s="4" t="s">
+        <v>410</v>
+      </c>
+      <c r="C119" s="4" t="s">
+        <v>119</v>
+      </c>
+      <c r="D119" s="3" t="s">
+        <v>478</v>
+      </c>
+      <c r="E119" s="3" t="s">
+        <v>479</v>
+      </c>
+      <c r="F119" s="3"/>
+    </row>
+    <row r="120" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A120" s="18"/>
+      <c r="B120" s="4" t="s">
         <v>411</v>
       </c>
-      <c r="C114" s="4" t="s">
+      <c r="C120" s="4" t="s">
         <v>142</v>
       </c>
-      <c r="D114" s="3"/>
-      <c r="E114" s="3"/>
-      <c r="F114" s="3"/>
-    </row>
-    <row r="115" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A115" s="20"/>
-      <c r="B115" s="4" t="s">
-        <v>412</v>
-      </c>
-      <c r="C115" s="4" t="s">
-        <v>142</v>
-      </c>
-      <c r="D115" s="3"/>
-      <c r="E115" s="3"/>
-      <c r="F115" s="3"/>
-    </row>
-    <row r="116" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A116" s="20"/>
-      <c r="B116" s="4" t="s">
-        <v>413</v>
-      </c>
-      <c r="C116" s="4" t="s">
-        <v>119</v>
-      </c>
-      <c r="D116" s="3"/>
-      <c r="E116" s="3"/>
-      <c r="F116" s="3"/>
-    </row>
-    <row r="117" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A117" s="20"/>
-      <c r="B117" s="4" t="s">
-        <v>414</v>
-      </c>
-      <c r="C117" s="4" t="s">
-        <v>142</v>
-      </c>
-      <c r="D117" s="3"/>
-      <c r="E117" s="3"/>
-      <c r="F117" s="3"/>
-    </row>
-    <row r="118" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A118" s="20"/>
-      <c r="B118" s="4" t="s">
-        <v>404</v>
-      </c>
-      <c r="C118" s="4" t="s">
-        <v>142</v>
-      </c>
-      <c r="D118" s="3"/>
-      <c r="E118" s="3"/>
-      <c r="F118" s="3"/>
-    </row>
-    <row r="119" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="D119" s="3"/>
-      <c r="E119" s="3"/>
-      <c r="F119" s="3"/>
-    </row>
-    <row r="120" spans="1:6" x14ac:dyDescent="0.25">
       <c r="D120" s="3"/>
       <c r="E120" s="3"/>
       <c r="F120" s="3"/>
     </row>
     <row r="121" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A121" s="18"/>
+      <c r="B121" s="4" t="s">
+        <v>412</v>
+      </c>
+      <c r="C121" s="4" t="s">
+        <v>142</v>
+      </c>
       <c r="D121" s="3"/>
       <c r="E121" s="3"/>
       <c r="F121" s="3"/>
     </row>
     <row r="122" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A122" s="18"/>
+      <c r="B122" s="4" t="s">
+        <v>413</v>
+      </c>
+      <c r="C122" s="4" t="s">
+        <v>119</v>
+      </c>
       <c r="D122" s="3"/>
       <c r="E122" s="3"/>
       <c r="F122" s="3"/>
     </row>
     <row r="123" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A123" s="18"/>
+      <c r="B123" s="4" t="s">
+        <v>414</v>
+      </c>
+      <c r="C123" s="4" t="s">
+        <v>142</v>
+      </c>
       <c r="D123" s="3"/>
       <c r="E123" s="3"/>
       <c r="F123" s="3"/>
     </row>
     <row r="124" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A124" s="18"/>
+      <c r="B124" s="4" t="s">
+        <v>404</v>
+      </c>
+      <c r="C124" s="4" t="s">
+        <v>142</v>
+      </c>
       <c r="D124" s="3"/>
       <c r="E124" s="3"/>
       <c r="F124" s="3"/>
     </row>
-    <row r="125" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="D125" s="3"/>
-      <c r="E125" s="3"/>
-      <c r="F125" s="3"/>
+    <row r="125" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A125" s="16" t="s">
+        <v>461</v>
+      </c>
+      <c r="B125" s="16" t="s">
+        <v>461</v>
+      </c>
+      <c r="C125" s="16"/>
+      <c r="D125" s="16" t="s">
+        <v>461</v>
+      </c>
+      <c r="E125" s="16" t="s">
+        <v>461</v>
+      </c>
+      <c r="F125" s="16" t="s">
+        <v>461</v>
+      </c>
     </row>
     <row r="126" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A126" s="16" t="s">
+        <v>462</v>
+      </c>
+      <c r="B126" s="4" t="s">
+        <v>463</v>
+      </c>
+      <c r="C126" s="4" t="s">
+        <v>119</v>
+      </c>
       <c r="D126" s="3"/>
       <c r="E126" s="3"/>
       <c r="F126" s="3"/>
     </row>
     <row r="127" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B127" s="4" t="s">
+        <v>464</v>
+      </c>
+      <c r="C127" s="4" t="s">
+        <v>119</v>
+      </c>
       <c r="D127" s="3"/>
       <c r="E127" s="3"/>
       <c r="F127" s="3"/>
     </row>
     <row r="128" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B128" s="4" t="s">
+        <v>465</v>
+      </c>
+      <c r="C128" s="4" t="s">
+        <v>119</v>
+      </c>
       <c r="D128" s="3"/>
       <c r="E128" s="3"/>
       <c r="F128" s="3"/>
     </row>
-    <row r="129" spans="4:6" x14ac:dyDescent="0.25">
+    <row r="129" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B129" s="4" t="s">
+        <v>466</v>
+      </c>
+      <c r="C129" s="4" t="s">
+        <v>119</v>
+      </c>
       <c r="D129" s="3"/>
       <c r="E129" s="3"/>
       <c r="F129" s="3"/>
     </row>
-    <row r="130" spans="4:6" x14ac:dyDescent="0.25">
+    <row r="130" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B130" s="4" t="s">
+        <v>467</v>
+      </c>
+      <c r="C130" s="4" t="s">
+        <v>119</v>
+      </c>
       <c r="D130" s="3"/>
       <c r="E130" s="3"/>
       <c r="F130" s="3"/>
     </row>
-    <row r="131" spans="4:6" x14ac:dyDescent="0.25">
+    <row r="131" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B131" s="4" t="s">
+        <v>468</v>
+      </c>
+      <c r="C131" s="4" t="s">
+        <v>119</v>
+      </c>
       <c r="D131" s="3"/>
       <c r="E131" s="3"/>
       <c r="F131" s="3"/>
     </row>
-    <row r="132" spans="4:6" x14ac:dyDescent="0.25">
+    <row r="132" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B132" s="4" t="s">
+        <v>469</v>
+      </c>
+      <c r="C132" s="4" t="s">
+        <v>119</v>
+      </c>
       <c r="D132" s="3"/>
       <c r="E132" s="3"/>
       <c r="F132" s="3"/>
     </row>
-    <row r="133" spans="4:6" x14ac:dyDescent="0.25">
+    <row r="133" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B133" s="4" t="s">
+        <v>470</v>
+      </c>
+      <c r="C133" s="4" t="s">
+        <v>119</v>
+      </c>
       <c r="D133" s="3"/>
       <c r="E133" s="3"/>
       <c r="F133" s="3"/>
     </row>
-    <row r="134" spans="4:6" x14ac:dyDescent="0.25">
+    <row r="134" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A134" s="16" t="s">
+        <v>471</v>
+      </c>
+      <c r="B134" s="4" t="s">
+        <v>472</v>
+      </c>
+      <c r="C134" s="4" t="s">
+        <v>119</v>
+      </c>
       <c r="D134" s="3"/>
       <c r="E134" s="3"/>
       <c r="F134" s="3"/>
     </row>
-    <row r="135" spans="4:6" x14ac:dyDescent="0.25">
+    <row r="135" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B135" s="4" t="s">
+        <v>473</v>
+      </c>
+      <c r="C135" s="4" t="s">
+        <v>119</v>
+      </c>
       <c r="D135" s="3"/>
       <c r="E135" s="3"/>
       <c r="F135" s="3"/>
     </row>
-    <row r="136" spans="4:6" x14ac:dyDescent="0.25">
+    <row r="136" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B136" s="4" t="s">
+        <v>474</v>
+      </c>
+      <c r="C136" s="4" t="s">
+        <v>119</v>
+      </c>
       <c r="D136" s="3"/>
       <c r="E136" s="3"/>
       <c r="F136" s="3"/>
     </row>
-    <row r="137" spans="4:6" x14ac:dyDescent="0.25">
+    <row r="137" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B137" s="4" t="s">
+        <v>475</v>
+      </c>
+      <c r="C137" s="4" t="s">
+        <v>112</v>
+      </c>
       <c r="D137" s="3"/>
       <c r="E137" s="3"/>
       <c r="F137" s="3"/>
     </row>
-    <row r="138" spans="4:6" x14ac:dyDescent="0.25">
+    <row r="138" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B138" s="4" t="s">
+        <v>476</v>
+      </c>
+      <c r="C138" s="4" t="s">
+        <v>119</v>
+      </c>
       <c r="D138" s="3"/>
       <c r="E138" s="3"/>
       <c r="F138" s="3"/>
     </row>
-    <row r="139" spans="4:6" x14ac:dyDescent="0.25">
+    <row r="139" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B139" s="4" t="s">
+        <v>477</v>
+      </c>
+      <c r="C139" s="4" t="s">
+        <v>142</v>
+      </c>
       <c r="D139" s="3"/>
       <c r="E139" s="3"/>
       <c r="F139" s="3"/>
     </row>
-    <row r="140" spans="4:6" x14ac:dyDescent="0.25">
+    <row r="140" spans="1:6" x14ac:dyDescent="0.25">
       <c r="D140" s="3"/>
       <c r="E140" s="3"/>
       <c r="F140" s="3"/>
     </row>
-    <row r="141" spans="4:6" x14ac:dyDescent="0.25">
+    <row r="141" spans="1:6" x14ac:dyDescent="0.25">
       <c r="D141" s="3"/>
       <c r="E141" s="3"/>
       <c r="F141" s="3"/>
     </row>
-    <row r="142" spans="4:6" x14ac:dyDescent="0.25">
+    <row r="142" spans="1:6" x14ac:dyDescent="0.25">
       <c r="D142" s="3"/>
       <c r="E142" s="3"/>
       <c r="F142" s="3"/>
     </row>
-    <row r="143" spans="4:6" x14ac:dyDescent="0.25">
+    <row r="143" spans="1:6" x14ac:dyDescent="0.25">
       <c r="D143" s="3"/>
       <c r="E143" s="3"/>
       <c r="F143" s="3"/>
     </row>
-    <row r="144" spans="4:6" x14ac:dyDescent="0.25">
+    <row r="144" spans="1:6" x14ac:dyDescent="0.25">
       <c r="D144" s="3"/>
       <c r="E144" s="3"/>
       <c r="F144" s="3"/>
@@ -8606,7 +8892,7 @@
     <mergeCell ref="A1:F1"/>
   </mergeCells>
   <phoneticPr fontId="3" type="noConversion"/>
-  <conditionalFormatting sqref="C1:C1048576">
+  <conditionalFormatting sqref="C1:C124 C126:C1048576">
     <cfRule type="containsText" dxfId="2" priority="1" operator="containsText" text="Hard">
       <formula>NOT(ISERROR(SEARCH("Hard",C1)))</formula>
     </cfRule>

</xml_diff>

<commit_message>
Finished longest increasing path in matrix
</commit_message>
<xml_diff>
--- a/LeetCode.xlsx
+++ b/LeetCode.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\EricS\Documents\VSCode Projects\LeetcodeGrind\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{53ADF0A8-4A0D-4E8A-9740-8E64816759EE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6BC798BB-0E10-4282-BD62-3B6FFBD6EA70}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="3" xr2:uid="{02D29AA1-7085-42F6-B3D4-4C0365DA5453}"/>
   </bookViews>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="689" uniqueCount="480">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="691" uniqueCount="481">
   <si>
     <t>Roman to Integer:</t>
   </si>
@@ -1482,6 +1482,9 @@
   </si>
   <si>
     <t>Literally just recursion with memory, if left matches you increment left pointer and recurse, if right matches you do the same, and you use an or on boolean to see what happens, then you save to a vector thingy and see how everything goes</t>
+  </si>
+  <si>
+    <t>Again it's just recursion with memory, tracking length of increasing path ending in current spot and returning if track matrix is already not -1. In main function call dfs on all non -1 slots since not processed yet and return the maximum of the returns of those. In dfs, initialize starting ret to 1 since each block has length 1, then have 1 + max of the path going each of the 4 directions recursing outwards</t>
   </si>
 </sst>
 </file>
@@ -2553,8 +2556,8 @@
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:G969"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A115" zoomScale="81" zoomScaleNormal="122" workbookViewId="0">
-      <selection activeCell="D120" sqref="D120"/>
+    <sheetView tabSelected="1" topLeftCell="A116" zoomScale="81" zoomScaleNormal="122" workbookViewId="0">
+      <selection activeCell="D121" sqref="D121"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4499,7 +4502,7 @@
       </c>
       <c r="F119" s="3"/>
     </row>
-    <row r="120" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="120" spans="1:6" ht="90" x14ac:dyDescent="0.25">
       <c r="A120" s="18"/>
       <c r="B120" s="4" t="s">
         <v>411</v>
@@ -4507,8 +4510,12 @@
       <c r="C120" s="4" t="s">
         <v>142</v>
       </c>
-      <c r="D120" s="3"/>
-      <c r="E120" s="3"/>
+      <c r="D120" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="E120" s="3" t="s">
+        <v>480</v>
+      </c>
       <c r="F120" s="3"/>
     </row>
     <row r="121" spans="1:6" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Finished distinct subsequences problem
</commit_message>
<xml_diff>
--- a/LeetCode.xlsx
+++ b/LeetCode.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\EricS\Documents\VSCode Projects\LeetcodeGrind\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6BC798BB-0E10-4282-BD62-3B6FFBD6EA70}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B1873549-6F77-4BFC-9B79-7BA1FA540862}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="3" xr2:uid="{02D29AA1-7085-42F6-B3D4-4C0365DA5453}"/>
   </bookViews>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="691" uniqueCount="481">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="693" uniqueCount="483">
   <si>
     <t>Roman to Integer:</t>
   </si>
@@ -1485,6 +1485,12 @@
   </si>
   <si>
     <t>Again it's just recursion with memory, tracking length of increasing path ending in current spot and returning if track matrix is already not -1. In main function call dfs on all non -1 slots since not processed yet and return the maximum of the returns of those. In dfs, initialize starting ret to 1 since each block has length 1, then have 1 + max of the path going each of the 4 directions recursing outwards</t>
+  </si>
+  <si>
+    <t>find # of distinct subseqs in string s that are equal to string t</t>
+  </si>
+  <si>
+    <t>We make track matrix of size n + 1 by m + 1 where track[i][j] is # of ways to make t[:j] from subseqs of s[:i]. First, we initialize all of track[i][0] to 1 since there's always 1 way to make empty string. Then, we do a nested for loop. If there is a character match, we add cell above with cell diagonally top left (track[i + 1][j + 1] = track[i][j + 1] + track[i][j]) since top left is how many subseqs you can make to j w new char and above was how many subseqs there were originally w/o new char. If not match, we just copy above since again that's subseqs originally w/o new char at i.</t>
   </si>
 </sst>
 </file>
@@ -2556,8 +2562,8 @@
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:G969"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A116" zoomScale="81" zoomScaleNormal="122" workbookViewId="0">
-      <selection activeCell="D121" sqref="D121"/>
+    <sheetView tabSelected="1" topLeftCell="A118" zoomScale="81" zoomScaleNormal="122" workbookViewId="0">
+      <selection activeCell="E122" sqref="E122"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4518,7 +4524,7 @@
       </c>
       <c r="F120" s="3"/>
     </row>
-    <row r="121" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="121" spans="1:6" ht="120" x14ac:dyDescent="0.25">
       <c r="A121" s="18"/>
       <c r="B121" s="4" t="s">
         <v>412</v>
@@ -4526,8 +4532,12 @@
       <c r="C121" s="4" t="s">
         <v>142</v>
       </c>
-      <c r="D121" s="3"/>
-      <c r="E121" s="3"/>
+      <c r="D121" s="3" t="s">
+        <v>481</v>
+      </c>
+      <c r="E121" s="3" t="s">
+        <v>482</v>
+      </c>
       <c r="F121" s="3"/>
     </row>
     <row r="122" spans="1:6" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Finally finished edit distance code
</commit_message>
<xml_diff>
--- a/LeetCode.xlsx
+++ b/LeetCode.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27726"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27830"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\EricS\Documents\VSCode Projects\LeetcodeGrind\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B1873549-6F77-4BFC-9B79-7BA1FA540862}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3E5CD070-412E-493D-A07F-332C45AFCBB9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="3" xr2:uid="{02D29AA1-7085-42F6-B3D4-4C0365DA5453}"/>
   </bookViews>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="693" uniqueCount="483">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="696" uniqueCount="486">
   <si>
     <t>Roman to Integer:</t>
   </si>
@@ -1491,6 +1491,15 @@
   </si>
   <si>
     <t>We make track matrix of size n + 1 by m + 1 where track[i][j] is # of ways to make t[:j] from subseqs of s[:i]. First, we initialize all of track[i][0] to 1 since there's always 1 way to make empty string. Then, we do a nested for loop. If there is a character match, we add cell above with cell diagonally top left (track[i + 1][j + 1] = track[i][j + 1] + track[i][j]) since top left is how many subseqs you can make to j w new char and above was how many subseqs there were originally w/o new char. If not match, we just copy above since again that's subseqs originally w/o new char at i.</t>
+  </si>
+  <si>
+    <t>Find number of operations necessary to convert one string to another (ops: insert, remove, change one letter)</t>
+  </si>
+  <si>
+    <t>We make track matrix of size n + 1 by m + 1 where track[i][j] is # of ops required to go from s1[:i] to s2[:j]. We have to initialize the 0th row and column to consecutive counting (0 - n and 0 - m) since that makes sense. Then you traverse through and update based on whether current letters are the same and the top left diagonal, above, and left slot values to determine which operation is optimal here.</t>
+  </si>
+  <si>
+    <t>Can technically fit into 2 n length arrays but pain</t>
   </si>
 </sst>
 </file>
@@ -1597,7 +1606,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="22">
+  <cellXfs count="21">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -1641,16 +1650,10 @@
     <xf numFmtId="49" fontId="7" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
     <xf numFmtId="49" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -1661,6 +1664,9 @@
     </xf>
     <xf numFmtId="49" fontId="9" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -2563,12 +2569,12 @@
   <dimension ref="A1:G969"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A118" zoomScale="81" zoomScaleNormal="122" workbookViewId="0">
-      <selection activeCell="E122" sqref="E122"/>
+      <selection activeCell="D123" sqref="D123"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="19.7109375" style="17" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="19.7109375" style="16" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="59.28515625" style="4" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="5.7109375" style="4" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="56.42578125" style="4" customWidth="1"/>
@@ -2580,17 +2586,17 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A1" s="15" t="s">
+      <c r="A1" s="20" t="s">
         <v>111</v>
       </c>
-      <c r="B1" s="15"/>
-      <c r="C1" s="15"/>
-      <c r="D1" s="15"/>
-      <c r="E1" s="15"/>
-      <c r="F1" s="15"/>
+      <c r="B1" s="20"/>
+      <c r="C1" s="20"/>
+      <c r="D1" s="20"/>
+      <c r="E1" s="20"/>
+      <c r="F1" s="20"/>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A2" s="16" t="s">
+      <c r="A2" s="15" t="s">
         <v>110</v>
       </c>
       <c r="B2" s="8" t="s">
@@ -2613,7 +2619,7 @@
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A3" s="16" t="s">
+      <c r="A3" s="15" t="s">
         <v>109</v>
       </c>
       <c r="B3" s="4" t="s">
@@ -2631,7 +2637,7 @@
       <c r="F3" s="3"/>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A4" s="16"/>
+      <c r="A4" s="15"/>
       <c r="B4" s="4" t="s">
         <v>28</v>
       </c>
@@ -2647,7 +2653,7 @@
       <c r="F4" s="3"/>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A5" s="16"/>
+      <c r="A5" s="15"/>
       <c r="B5" s="4" t="s">
         <v>36</v>
       </c>
@@ -2663,7 +2669,7 @@
       <c r="F5" s="3"/>
     </row>
     <row r="6" spans="1:7" ht="30" x14ac:dyDescent="0.25">
-      <c r="A6" s="16"/>
+      <c r="A6" s="15"/>
       <c r="B6" s="4" t="s">
         <v>114</v>
       </c>
@@ -2681,7 +2687,7 @@
       </c>
     </row>
     <row r="7" spans="1:7" ht="75" x14ac:dyDescent="0.25">
-      <c r="A7" s="16"/>
+      <c r="A7" s="15"/>
       <c r="B7" s="4" t="s">
         <v>115</v>
       </c>
@@ -2697,7 +2703,7 @@
       <c r="F7" s="3"/>
     </row>
     <row r="8" spans="1:7" ht="30" x14ac:dyDescent="0.25">
-      <c r="A8" s="16"/>
+      <c r="A8" s="15"/>
       <c r="B8" s="4" t="s">
         <v>116</v>
       </c>
@@ -2715,7 +2721,7 @@
       </c>
     </row>
     <row r="9" spans="1:7" ht="30" x14ac:dyDescent="0.25">
-      <c r="A9" s="16"/>
+      <c r="A9" s="15"/>
       <c r="B9" s="4" t="s">
         <v>117</v>
       </c>
@@ -2731,7 +2737,7 @@
       <c r="F9" s="3"/>
     </row>
     <row r="10" spans="1:7" ht="30" x14ac:dyDescent="0.25">
-      <c r="A10" s="16"/>
+      <c r="A10" s="15"/>
       <c r="B10" s="4" t="s">
         <v>118</v>
       </c>
@@ -2749,7 +2755,7 @@
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A11" s="16" t="s">
+      <c r="A11" s="15" t="s">
         <v>137</v>
       </c>
       <c r="B11" s="4" t="s">
@@ -2767,7 +2773,7 @@
       <c r="F11" s="3"/>
     </row>
     <row r="12" spans="1:7" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="16"/>
+      <c r="A12" s="15"/>
       <c r="B12" s="4" t="s">
         <v>138</v>
       </c>
@@ -2785,7 +2791,7 @@
       </c>
     </row>
     <row r="13" spans="1:7" ht="30" x14ac:dyDescent="0.25">
-      <c r="A13" s="16"/>
+      <c r="A13" s="15"/>
       <c r="B13" s="4" t="s">
         <v>139</v>
       </c>
@@ -2801,7 +2807,7 @@
       <c r="F13" s="3"/>
     </row>
     <row r="14" spans="1:7" ht="30" x14ac:dyDescent="0.25">
-      <c r="A14" s="16"/>
+      <c r="A14" s="15"/>
       <c r="B14" s="4" t="s">
         <v>140</v>
       </c>
@@ -2817,7 +2823,7 @@
       <c r="F14" s="3"/>
     </row>
     <row r="15" spans="1:7" ht="45" x14ac:dyDescent="0.25">
-      <c r="A15" s="16"/>
+      <c r="A15" s="15"/>
       <c r="B15" s="4" t="s">
         <v>141</v>
       </c>
@@ -2833,7 +2839,7 @@
       <c r="F15" s="3"/>
     </row>
     <row r="16" spans="1:7" ht="30" x14ac:dyDescent="0.25">
-      <c r="A16" s="16" t="s">
+      <c r="A16" s="15" t="s">
         <v>153</v>
       </c>
       <c r="B16" s="4" t="s">
@@ -2851,7 +2857,7 @@
       <c r="F16" s="3"/>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A17" s="16"/>
+      <c r="A17" s="15"/>
       <c r="B17" s="4" t="s">
         <v>155</v>
       </c>
@@ -2869,7 +2875,7 @@
       </c>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A18" s="16"/>
+      <c r="A18" s="15"/>
       <c r="B18" s="4" t="s">
         <v>156</v>
       </c>
@@ -2885,7 +2891,7 @@
       <c r="F18" s="3"/>
     </row>
     <row r="19" spans="1:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="A19" s="16"/>
+      <c r="A19" s="15"/>
       <c r="B19" s="4" t="s">
         <v>157</v>
       </c>
@@ -2901,7 +2907,7 @@
       <c r="F19" s="3"/>
     </row>
     <row r="20" spans="1:6" ht="45" x14ac:dyDescent="0.25">
-      <c r="A20" s="16"/>
+      <c r="A20" s="15"/>
       <c r="B20" s="4" t="s">
         <v>158</v>
       </c>
@@ -2917,7 +2923,7 @@
       <c r="F20" s="3"/>
     </row>
     <row r="21" spans="1:6" ht="45" x14ac:dyDescent="0.25">
-      <c r="A21" s="16"/>
+      <c r="A21" s="15"/>
       <c r="B21" s="4" t="s">
         <v>159</v>
       </c>
@@ -2935,7 +2941,7 @@
       </c>
     </row>
     <row r="22" spans="1:6" ht="60" x14ac:dyDescent="0.25">
-      <c r="A22" s="16"/>
+      <c r="A22" s="15"/>
       <c r="B22" s="4" t="s">
         <v>154</v>
       </c>
@@ -2953,7 +2959,7 @@
       </c>
     </row>
     <row r="23" spans="1:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="A23" s="16" t="s">
+      <c r="A23" s="15" t="s">
         <v>169</v>
       </c>
       <c r="B23" s="4" t="s">
@@ -2971,7 +2977,7 @@
       <c r="F23" s="3"/>
     </row>
     <row r="24" spans="1:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="A24" s="16"/>
+      <c r="A24" s="15"/>
       <c r="B24" s="4" t="s">
         <v>171</v>
       </c>
@@ -2987,7 +2993,7 @@
       <c r="F24" s="3"/>
     </row>
     <row r="25" spans="1:6" ht="60" x14ac:dyDescent="0.25">
-      <c r="A25" s="16"/>
+      <c r="A25" s="15"/>
       <c r="B25" s="4" t="s">
         <v>172</v>
       </c>
@@ -3003,7 +3009,7 @@
       <c r="F25" s="3"/>
     </row>
     <row r="26" spans="1:6" ht="45" x14ac:dyDescent="0.25">
-      <c r="A26" s="16"/>
+      <c r="A26" s="15"/>
       <c r="B26" s="4" t="s">
         <v>173</v>
       </c>
@@ -3019,7 +3025,7 @@
       <c r="F26" s="3"/>
     </row>
     <row r="27" spans="1:6" ht="60" x14ac:dyDescent="0.25">
-      <c r="A27" s="16"/>
+      <c r="A27" s="15"/>
       <c r="B27" s="4" t="s">
         <v>174</v>
       </c>
@@ -3035,7 +3041,7 @@
       <c r="F27" s="3"/>
     </row>
     <row r="28" spans="1:6" ht="45" x14ac:dyDescent="0.25">
-      <c r="A28" s="16"/>
+      <c r="A28" s="15"/>
       <c r="B28" s="4" t="s">
         <v>175</v>
       </c>
@@ -3053,7 +3059,7 @@
       </c>
     </row>
     <row r="29" spans="1:6" ht="150" x14ac:dyDescent="0.25">
-      <c r="A29" s="16"/>
+      <c r="A29" s="15"/>
       <c r="B29" s="4" t="s">
         <v>176</v>
       </c>
@@ -3071,7 +3077,7 @@
       </c>
     </row>
     <row r="30" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A30" s="16" t="s">
+      <c r="A30" s="15" t="s">
         <v>168</v>
       </c>
       <c r="B30" s="4" t="s">
@@ -3089,7 +3095,7 @@
       <c r="F30" s="3"/>
     </row>
     <row r="31" spans="1:6" ht="60" x14ac:dyDescent="0.25">
-      <c r="A31" s="16"/>
+      <c r="A31" s="15"/>
       <c r="B31" s="4" t="s">
         <v>178</v>
       </c>
@@ -3105,7 +3111,7 @@
       <c r="F31" s="3"/>
     </row>
     <row r="32" spans="1:6" ht="45" x14ac:dyDescent="0.25">
-      <c r="A32" s="16"/>
+      <c r="A32" s="15"/>
       <c r="B32" s="4" t="s">
         <v>179</v>
       </c>
@@ -3123,7 +3129,7 @@
       </c>
     </row>
     <row r="33" spans="1:6" ht="60" x14ac:dyDescent="0.25">
-      <c r="A33" s="16"/>
+      <c r="A33" s="15"/>
       <c r="B33" s="4" t="s">
         <v>180</v>
       </c>
@@ -3139,7 +3145,7 @@
       <c r="F33" s="3"/>
     </row>
     <row r="34" spans="1:6" ht="90" x14ac:dyDescent="0.25">
-      <c r="A34" s="16"/>
+      <c r="A34" s="15"/>
       <c r="B34" s="4" t="s">
         <v>181</v>
       </c>
@@ -3155,7 +3161,7 @@
       <c r="F34" s="3"/>
     </row>
     <row r="35" spans="1:6" ht="90" x14ac:dyDescent="0.25">
-      <c r="A35" s="16"/>
+      <c r="A35" s="15"/>
       <c r="B35" s="4" t="s">
         <v>182</v>
       </c>
@@ -3171,7 +3177,7 @@
       <c r="F35" s="3"/>
     </row>
     <row r="36" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A36" s="16" t="s">
+      <c r="A36" s="15" t="s">
         <v>183</v>
       </c>
       <c r="B36" s="4" t="s">
@@ -3189,7 +3195,7 @@
       <c r="F36" s="3"/>
     </row>
     <row r="37" spans="1:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="A37" s="16"/>
+      <c r="A37" s="15"/>
       <c r="B37" s="4" t="s">
         <v>186</v>
       </c>
@@ -3207,7 +3213,7 @@
       </c>
     </row>
     <row r="38" spans="1:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="A38" s="16"/>
+      <c r="A38" s="15"/>
       <c r="B38" s="4" t="s">
         <v>187</v>
       </c>
@@ -3223,7 +3229,7 @@
       <c r="F38" s="3"/>
     </row>
     <row r="39" spans="1:6" ht="45" x14ac:dyDescent="0.25">
-      <c r="A39" s="16"/>
+      <c r="A39" s="15"/>
       <c r="B39" s="4" t="s">
         <v>188</v>
       </c>
@@ -3239,7 +3245,7 @@
       <c r="F39" s="3"/>
     </row>
     <row r="40" spans="1:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="A40" s="16"/>
+      <c r="A40" s="15"/>
       <c r="B40" s="4" t="s">
         <v>189</v>
       </c>
@@ -3255,7 +3261,7 @@
       <c r="F40" s="3"/>
     </row>
     <row r="41" spans="1:6" ht="45" x14ac:dyDescent="0.25">
-      <c r="A41" s="16"/>
+      <c r="A41" s="15"/>
       <c r="B41" s="4" t="s">
         <v>190</v>
       </c>
@@ -3271,7 +3277,7 @@
       <c r="F41" s="3"/>
     </row>
     <row r="42" spans="1:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="A42" s="16"/>
+      <c r="A42" s="15"/>
       <c r="B42" s="4" t="s">
         <v>191</v>
       </c>
@@ -3287,7 +3293,7 @@
       <c r="F42" s="3"/>
     </row>
     <row r="43" spans="1:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="A43" s="16"/>
+      <c r="A43" s="15"/>
       <c r="B43" s="6" t="s">
         <v>192</v>
       </c>
@@ -3303,7 +3309,7 @@
       <c r="F43" s="3"/>
     </row>
     <row r="44" spans="1:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="A44" s="16"/>
+      <c r="A44" s="15"/>
       <c r="B44" s="4" t="s">
         <v>193</v>
       </c>
@@ -3319,7 +3325,7 @@
       <c r="F44" s="3"/>
     </row>
     <row r="45" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A45" s="16"/>
+      <c r="A45" s="15"/>
       <c r="B45" s="4" t="s">
         <v>194</v>
       </c>
@@ -3335,7 +3341,7 @@
       <c r="F45" s="3"/>
     </row>
     <row r="46" spans="1:6" ht="45" x14ac:dyDescent="0.25">
-      <c r="A46" s="16"/>
+      <c r="A46" s="15"/>
       <c r="B46" s="4" t="s">
         <v>184</v>
       </c>
@@ -3351,7 +3357,7 @@
       <c r="F46" s="3"/>
     </row>
     <row r="47" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A47" s="16" t="s">
+      <c r="A47" s="15" t="s">
         <v>250</v>
       </c>
       <c r="B47" s="4" t="s">
@@ -3369,7 +3375,7 @@
       <c r="F47" s="3"/>
     </row>
     <row r="48" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A48" s="16"/>
+      <c r="A48" s="15"/>
       <c r="B48" s="4" t="s">
         <v>252</v>
       </c>
@@ -3385,7 +3391,7 @@
       <c r="F48" s="3"/>
     </row>
     <row r="49" spans="1:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="A49" s="16"/>
+      <c r="A49" s="15"/>
       <c r="B49" s="4" t="s">
         <v>253</v>
       </c>
@@ -3401,7 +3407,7 @@
       <c r="F49" s="3"/>
     </row>
     <row r="50" spans="1:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="A50" s="16"/>
+      <c r="A50" s="15"/>
       <c r="B50" s="4" t="s">
         <v>254</v>
       </c>
@@ -3417,7 +3423,7 @@
       <c r="F50" s="3"/>
     </row>
     <row r="51" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A51" s="16"/>
+      <c r="A51" s="15"/>
       <c r="B51" s="4" t="s">
         <v>255</v>
       </c>
@@ -3433,7 +3439,7 @@
       <c r="F51" s="3"/>
     </row>
     <row r="52" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A52" s="16"/>
+      <c r="A52" s="15"/>
       <c r="B52" s="4" t="s">
         <v>256</v>
       </c>
@@ -3449,7 +3455,7 @@
       <c r="F52" s="3"/>
     </row>
     <row r="53" spans="1:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="A53" s="16"/>
+      <c r="A53" s="15"/>
       <c r="B53" s="4" t="s">
         <v>257</v>
       </c>
@@ -3465,7 +3471,7 @@
       <c r="F53" s="3"/>
     </row>
     <row r="54" spans="1:6" ht="45" x14ac:dyDescent="0.25">
-      <c r="A54" s="16"/>
+      <c r="A54" s="15"/>
       <c r="B54" s="4" t="s">
         <v>258</v>
       </c>
@@ -3481,7 +3487,7 @@
       <c r="F54" s="3"/>
     </row>
     <row r="55" spans="1:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="A55" s="16"/>
+      <c r="A55" s="15"/>
       <c r="B55" s="4" t="s">
         <v>259</v>
       </c>
@@ -3497,7 +3503,7 @@
       <c r="F55" s="3"/>
     </row>
     <row r="56" spans="1:6" ht="45" x14ac:dyDescent="0.25">
-      <c r="A56" s="16"/>
+      <c r="A56" s="15"/>
       <c r="B56" s="4" t="s">
         <v>260</v>
       </c>
@@ -3513,7 +3519,7 @@
       <c r="F56" s="3"/>
     </row>
     <row r="57" spans="1:6" ht="60" x14ac:dyDescent="0.25">
-      <c r="A57" s="16"/>
+      <c r="A57" s="15"/>
       <c r="B57" s="4" t="s">
         <v>261</v>
       </c>
@@ -3531,7 +3537,7 @@
       </c>
     </row>
     <row r="58" spans="1:6" ht="45" x14ac:dyDescent="0.25">
-      <c r="A58" s="16"/>
+      <c r="A58" s="15"/>
       <c r="B58" s="4" t="s">
         <v>262</v>
       </c>
@@ -3547,7 +3553,7 @@
       <c r="F58" s="3"/>
     </row>
     <row r="59" spans="1:6" ht="45" x14ac:dyDescent="0.25">
-      <c r="A59" s="16"/>
+      <c r="A59" s="15"/>
       <c r="B59" s="4" t="s">
         <v>263</v>
       </c>
@@ -3563,7 +3569,7 @@
       <c r="F59" s="3"/>
     </row>
     <row r="60" spans="1:6" ht="60" x14ac:dyDescent="0.25">
-      <c r="A60" s="16"/>
+      <c r="A60" s="15"/>
       <c r="B60" s="4" t="s">
         <v>264</v>
       </c>
@@ -3581,7 +3587,7 @@
       </c>
     </row>
     <row r="61" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A61" s="20"/>
+      <c r="A61" s="18"/>
       <c r="B61" s="9" t="s">
         <v>265</v>
       </c>
@@ -3597,7 +3603,7 @@
       <c r="F61" s="3"/>
     </row>
     <row r="62" spans="1:6" ht="105" x14ac:dyDescent="0.25">
-      <c r="A62" s="16" t="s">
+      <c r="A62" s="15" t="s">
         <v>290</v>
       </c>
       <c r="B62" s="4" t="s">
@@ -3617,7 +3623,7 @@
       </c>
     </row>
     <row r="63" spans="1:6" ht="45" x14ac:dyDescent="0.25">
-      <c r="A63" s="16"/>
+      <c r="A63" s="15"/>
       <c r="B63" s="4" t="s">
         <v>292</v>
       </c>
@@ -3633,7 +3639,7 @@
       <c r="F63" s="3"/>
     </row>
     <row r="64" spans="1:6" ht="75" x14ac:dyDescent="0.25">
-      <c r="A64" s="16"/>
+      <c r="A64" s="15"/>
       <c r="B64" s="4" t="s">
         <v>293</v>
       </c>
@@ -3651,7 +3657,7 @@
       </c>
     </row>
     <row r="65" spans="1:7" ht="45" x14ac:dyDescent="0.25">
-      <c r="A65" s="16" t="s">
+      <c r="A65" s="15" t="s">
         <v>294</v>
       </c>
       <c r="B65" s="4" t="s">
@@ -3669,7 +3675,7 @@
       <c r="F65" s="3"/>
     </row>
     <row r="66" spans="1:7" ht="69" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A66" s="16"/>
+      <c r="A66" s="15"/>
       <c r="B66" s="4" t="s">
         <v>296</v>
       </c>
@@ -3687,7 +3693,7 @@
       </c>
     </row>
     <row r="67" spans="1:7" ht="90" x14ac:dyDescent="0.25">
-      <c r="A67" s="16"/>
+      <c r="A67" s="15"/>
       <c r="B67" s="4" t="s">
         <v>297</v>
       </c>
@@ -3703,7 +3709,7 @@
       <c r="F67" s="11"/>
     </row>
     <row r="68" spans="1:7" ht="75" x14ac:dyDescent="0.25">
-      <c r="A68" s="16"/>
+      <c r="A68" s="15"/>
       <c r="B68" s="4" t="s">
         <v>298</v>
       </c>
@@ -3719,7 +3725,7 @@
       <c r="F68" s="3"/>
     </row>
     <row r="69" spans="1:7" ht="63" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A69" s="16"/>
+      <c r="A69" s="15"/>
       <c r="B69" s="4" t="s">
         <v>299</v>
       </c>
@@ -3735,7 +3741,7 @@
       <c r="F69" s="3"/>
     </row>
     <row r="70" spans="1:7" ht="90" x14ac:dyDescent="0.25">
-      <c r="A70" s="16"/>
+      <c r="A70" s="15"/>
       <c r="B70" s="4" t="s">
         <v>300</v>
       </c>
@@ -3751,7 +3757,7 @@
       <c r="F70" s="3"/>
     </row>
     <row r="71" spans="1:7" ht="64.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A71" s="16"/>
+      <c r="A71" s="15"/>
       <c r="B71" s="4" t="s">
         <v>301</v>
       </c>
@@ -3767,7 +3773,7 @@
       <c r="F71" s="3"/>
     </row>
     <row r="72" spans="1:7" ht="45" x14ac:dyDescent="0.25">
-      <c r="A72" s="16"/>
+      <c r="A72" s="15"/>
       <c r="B72" s="4" t="s">
         <v>302</v>
       </c>
@@ -3783,7 +3789,7 @@
       <c r="F72" s="3"/>
     </row>
     <row r="73" spans="1:7" ht="140.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A73" s="16"/>
+      <c r="A73" s="15"/>
       <c r="B73" s="4" t="s">
         <v>303</v>
       </c>
@@ -3799,7 +3805,7 @@
       <c r="F73" s="3"/>
     </row>
     <row r="74" spans="1:7" ht="45" x14ac:dyDescent="0.25">
-      <c r="A74" s="16" t="s">
+      <c r="A74" s="15" t="s">
         <v>330</v>
       </c>
       <c r="B74" s="4" t="s">
@@ -3817,7 +3823,7 @@
       <c r="F74" s="3"/>
     </row>
     <row r="75" spans="1:7" ht="60" x14ac:dyDescent="0.25">
-      <c r="A75" s="16"/>
+      <c r="A75" s="15"/>
       <c r="B75" s="4" t="s">
         <v>332</v>
       </c>
@@ -3833,7 +3839,7 @@
       <c r="F75" s="3"/>
     </row>
     <row r="76" spans="1:7" ht="30" x14ac:dyDescent="0.25">
-      <c r="A76" s="16"/>
+      <c r="A76" s="15"/>
       <c r="B76" s="4" t="s">
         <v>333</v>
       </c>
@@ -3851,7 +3857,7 @@
       </c>
     </row>
     <row r="77" spans="1:7" ht="82.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A77" s="16"/>
+      <c r="A77" s="15"/>
       <c r="B77" s="4" t="s">
         <v>334</v>
       </c>
@@ -3867,7 +3873,7 @@
       <c r="F77" s="3"/>
     </row>
     <row r="78" spans="1:7" ht="75.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A78" s="16"/>
+      <c r="A78" s="15"/>
       <c r="B78" s="4" t="s">
         <v>335</v>
       </c>
@@ -3883,7 +3889,7 @@
       <c r="F78" s="3"/>
     </row>
     <row r="79" spans="1:7" s="12" customFormat="1" ht="30" x14ac:dyDescent="0.25">
-      <c r="A79" s="21"/>
+      <c r="A79" s="19"/>
       <c r="B79" s="12" t="s">
         <v>336</v>
       </c>
@@ -3900,7 +3906,7 @@
       <c r="G79" s="14"/>
     </row>
     <row r="80" spans="1:7" ht="60" x14ac:dyDescent="0.25">
-      <c r="A80" s="16"/>
+      <c r="A80" s="15"/>
       <c r="B80" s="4" t="s">
         <v>337</v>
       </c>
@@ -3916,7 +3922,7 @@
       <c r="F80" s="3"/>
     </row>
     <row r="81" spans="1:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="A81" s="16" t="s">
+      <c r="A81" s="15" t="s">
         <v>338</v>
       </c>
       <c r="B81" s="4" t="s">
@@ -3936,7 +3942,7 @@
       </c>
     </row>
     <row r="82" spans="1:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="A82" s="16"/>
+      <c r="A82" s="15"/>
       <c r="B82" s="4" t="s">
         <v>340</v>
       </c>
@@ -3952,7 +3958,7 @@
       <c r="F82" s="3"/>
     </row>
     <row r="83" spans="1:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="A83" s="16"/>
+      <c r="A83" s="15"/>
       <c r="B83" s="4" t="s">
         <v>341</v>
       </c>
@@ -3968,7 +3974,7 @@
       <c r="F83" s="3"/>
     </row>
     <row r="84" spans="1:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="A84" s="16"/>
+      <c r="A84" s="15"/>
       <c r="B84" s="4" t="s">
         <v>342</v>
       </c>
@@ -3984,7 +3990,7 @@
       <c r="F84" s="3"/>
     </row>
     <row r="85" spans="1:6" ht="45" x14ac:dyDescent="0.25">
-      <c r="A85" s="16"/>
+      <c r="A85" s="15"/>
       <c r="B85" s="4" t="s">
         <v>343</v>
       </c>
@@ -4000,7 +4006,7 @@
       <c r="F85" s="3"/>
     </row>
     <row r="86" spans="1:6" ht="45" x14ac:dyDescent="0.25">
-      <c r="A86" s="16"/>
+      <c r="A86" s="15"/>
       <c r="B86" s="4" t="s">
         <v>344</v>
       </c>
@@ -4016,7 +4022,7 @@
       <c r="F86" s="3"/>
     </row>
     <row r="87" spans="1:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="A87" s="16"/>
+      <c r="A87" s="15"/>
       <c r="B87" s="4" t="s">
         <v>345</v>
       </c>
@@ -4032,7 +4038,7 @@
       <c r="F87" s="3"/>
     </row>
     <row r="88" spans="1:6" ht="75" x14ac:dyDescent="0.25">
-      <c r="A88" s="16"/>
+      <c r="A88" s="15"/>
       <c r="B88" s="4" t="s">
         <v>346</v>
       </c>
@@ -4050,7 +4056,7 @@
       </c>
     </row>
     <row r="89" spans="1:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="A89" s="16"/>
+      <c r="A89" s="15"/>
       <c r="B89" s="4" t="s">
         <v>347</v>
       </c>
@@ -4066,7 +4072,7 @@
       <c r="F89" s="3"/>
     </row>
     <row r="90" spans="1:6" ht="60" x14ac:dyDescent="0.25">
-      <c r="A90" s="16"/>
+      <c r="A90" s="15"/>
       <c r="B90" s="4" t="s">
         <v>348</v>
       </c>
@@ -4082,7 +4088,7 @@
       <c r="F90" s="3"/>
     </row>
     <row r="91" spans="1:6" ht="75" x14ac:dyDescent="0.25">
-      <c r="A91" s="16"/>
+      <c r="A91" s="15"/>
       <c r="B91" s="4" t="s">
         <v>349</v>
       </c>
@@ -4098,7 +4104,7 @@
       <c r="F91" s="3"/>
     </row>
     <row r="92" spans="1:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="A92" s="16"/>
+      <c r="A92" s="15"/>
       <c r="B92" s="4" t="s">
         <v>350</v>
       </c>
@@ -4114,7 +4120,7 @@
       <c r="F92" s="3"/>
     </row>
     <row r="93" spans="1:6" ht="75" x14ac:dyDescent="0.25">
-      <c r="A93" s="16"/>
+      <c r="A93" s="15"/>
       <c r="B93" s="4" t="s">
         <v>351</v>
       </c>
@@ -4130,7 +4136,7 @@
       <c r="F93" s="3"/>
     </row>
     <row r="94" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A94" s="16" t="s">
+      <c r="A94" s="15" t="s">
         <v>454</v>
       </c>
       <c r="B94" s="4" t="s">
@@ -4181,7 +4187,7 @@
       </c>
     </row>
     <row r="100" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A100" s="16" t="s">
+      <c r="A100" s="15" t="s">
         <v>352</v>
       </c>
       <c r="D100" s="3"/>
@@ -4189,7 +4195,7 @@
       <c r="F100" s="3"/>
     </row>
     <row r="101" spans="1:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="A101" s="18" t="s">
+      <c r="A101" s="5" t="s">
         <v>452</v>
       </c>
       <c r="B101" s="4" t="s">
@@ -4207,7 +4213,7 @@
       <c r="F101" s="3"/>
     </row>
     <row r="102" spans="1:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="A102" s="18" t="s">
+      <c r="A102" s="5" t="s">
         <v>452</v>
       </c>
       <c r="B102" s="4" t="s">
@@ -4225,7 +4231,7 @@
       <c r="F102" s="3"/>
     </row>
     <row r="103" spans="1:6" ht="90" x14ac:dyDescent="0.25">
-      <c r="A103" s="18" t="s">
+      <c r="A103" s="5" t="s">
         <v>452</v>
       </c>
       <c r="B103" s="4" t="s">
@@ -4243,7 +4249,7 @@
       <c r="F103" s="3"/>
     </row>
     <row r="104" spans="1:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="A104" s="18" t="s">
+      <c r="A104" s="5" t="s">
         <v>452</v>
       </c>
       <c r="B104" s="4" t="s">
@@ -4261,7 +4267,7 @@
       <c r="F104" s="3"/>
     </row>
     <row r="105" spans="1:6" ht="60" x14ac:dyDescent="0.25">
-      <c r="A105" s="19"/>
+      <c r="A105" s="17"/>
       <c r="B105" s="4" t="s">
         <v>357</v>
       </c>
@@ -4277,7 +4283,7 @@
       <c r="F105" s="3"/>
     </row>
     <row r="106" spans="1:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="A106" s="18"/>
+      <c r="A106" s="5"/>
       <c r="B106" s="4" t="s">
         <v>358</v>
       </c>
@@ -4293,7 +4299,7 @@
       <c r="F106" s="3"/>
     </row>
     <row r="107" spans="1:6" ht="105" x14ac:dyDescent="0.25">
-      <c r="A107" s="18" t="s">
+      <c r="A107" s="5" t="s">
         <v>452</v>
       </c>
       <c r="B107" s="4" t="s">
@@ -4311,7 +4317,7 @@
       <c r="F107" s="3"/>
     </row>
     <row r="108" spans="1:6" ht="45" x14ac:dyDescent="0.25">
-      <c r="A108" s="18" t="s">
+      <c r="A108" s="5" t="s">
         <v>450</v>
       </c>
       <c r="B108" s="4" t="s">
@@ -4329,7 +4335,7 @@
       <c r="F108" s="3"/>
     </row>
     <row r="109" spans="1:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="A109" s="18"/>
+      <c r="A109" s="5"/>
       <c r="B109" s="4" t="s">
         <v>361</v>
       </c>
@@ -4345,7 +4351,7 @@
       <c r="F109" s="3"/>
     </row>
     <row r="110" spans="1:6" ht="45" x14ac:dyDescent="0.25">
-      <c r="A110" s="18"/>
+      <c r="A110" s="5"/>
       <c r="B110" s="4" t="s">
         <v>362</v>
       </c>
@@ -4361,7 +4367,7 @@
       <c r="F110" s="3"/>
     </row>
     <row r="111" spans="1:6" ht="60" x14ac:dyDescent="0.25">
-      <c r="A111" s="18"/>
+      <c r="A111" s="5"/>
       <c r="B111" s="4" t="s">
         <v>363</v>
       </c>
@@ -4377,7 +4383,7 @@
       <c r="F111" s="3"/>
     </row>
     <row r="112" spans="1:6" ht="45" x14ac:dyDescent="0.25">
-      <c r="A112" s="18" t="s">
+      <c r="A112" s="5" t="s">
         <v>453</v>
       </c>
       <c r="B112" s="4" t="s">
@@ -4397,7 +4403,7 @@
       </c>
     </row>
     <row r="113" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A113" s="16" t="s">
+      <c r="A113" s="15" t="s">
         <v>403</v>
       </c>
       <c r="D113" s="3"/>
@@ -4405,7 +4411,7 @@
       <c r="F113" s="3"/>
     </row>
     <row r="114" spans="1:6" ht="75" x14ac:dyDescent="0.25">
-      <c r="A114" s="18" t="s">
+      <c r="A114" s="5" t="s">
         <v>451</v>
       </c>
       <c r="B114" s="4" t="s">
@@ -4441,7 +4447,7 @@
       <c r="F115" s="3"/>
     </row>
     <row r="116" spans="1:6" ht="135" x14ac:dyDescent="0.25">
-      <c r="A116" s="18"/>
+      <c r="A116" s="5"/>
       <c r="B116" s="4" t="s">
         <v>407</v>
       </c>
@@ -4457,7 +4463,7 @@
       <c r="F116" s="3"/>
     </row>
     <row r="117" spans="1:6" ht="45" x14ac:dyDescent="0.25">
-      <c r="A117" s="18" t="s">
+      <c r="A117" s="5" t="s">
         <v>450</v>
       </c>
       <c r="B117" s="4" t="s">
@@ -4475,7 +4481,7 @@
       <c r="F117" s="3"/>
     </row>
     <row r="118" spans="1:6" ht="240" x14ac:dyDescent="0.25">
-      <c r="A118" s="18" t="s">
+      <c r="A118" s="5" t="s">
         <v>453</v>
       </c>
       <c r="B118" s="4" t="s">
@@ -4493,7 +4499,7 @@
       <c r="F118" s="3"/>
     </row>
     <row r="119" spans="1:6" ht="60" x14ac:dyDescent="0.25">
-      <c r="A119" s="18"/>
+      <c r="A119" s="5"/>
       <c r="B119" s="4" t="s">
         <v>410</v>
       </c>
@@ -4509,7 +4515,7 @@
       <c r="F119" s="3"/>
     </row>
     <row r="120" spans="1:6" ht="90" x14ac:dyDescent="0.25">
-      <c r="A120" s="18"/>
+      <c r="A120" s="5"/>
       <c r="B120" s="4" t="s">
         <v>411</v>
       </c>
@@ -4525,7 +4531,7 @@
       <c r="F120" s="3"/>
     </row>
     <row r="121" spans="1:6" ht="120" x14ac:dyDescent="0.25">
-      <c r="A121" s="18"/>
+      <c r="A121" s="5"/>
       <c r="B121" s="4" t="s">
         <v>412</v>
       </c>
@@ -4540,20 +4546,26 @@
       </c>
       <c r="F121" s="3"/>
     </row>
-    <row r="122" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A122" s="18"/>
+    <row r="122" spans="1:6" ht="90" x14ac:dyDescent="0.25">
+      <c r="A122" s="5"/>
       <c r="B122" s="4" t="s">
         <v>413</v>
       </c>
       <c r="C122" s="4" t="s">
         <v>119</v>
       </c>
-      <c r="D122" s="3"/>
-      <c r="E122" s="3"/>
-      <c r="F122" s="3"/>
+      <c r="D122" s="3" t="s">
+        <v>483</v>
+      </c>
+      <c r="E122" s="3" t="s">
+        <v>484</v>
+      </c>
+      <c r="F122" s="3" t="s">
+        <v>485</v>
+      </c>
     </row>
     <row r="123" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A123" s="18"/>
+      <c r="A123" s="5"/>
       <c r="B123" s="4" t="s">
         <v>414</v>
       </c>
@@ -4565,7 +4577,7 @@
       <c r="F123" s="3"/>
     </row>
     <row r="124" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A124" s="18"/>
+      <c r="A124" s="5"/>
       <c r="B124" s="4" t="s">
         <v>404</v>
       </c>
@@ -4577,25 +4589,25 @@
       <c r="F124" s="3"/>
     </row>
     <row r="125" spans="1:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="A125" s="16" t="s">
+      <c r="A125" s="15" t="s">
         <v>461</v>
       </c>
-      <c r="B125" s="16" t="s">
+      <c r="B125" s="15" t="s">
         <v>461</v>
       </c>
-      <c r="C125" s="16"/>
-      <c r="D125" s="16" t="s">
+      <c r="C125" s="15"/>
+      <c r="D125" s="15" t="s">
         <v>461</v>
       </c>
-      <c r="E125" s="16" t="s">
+      <c r="E125" s="15" t="s">
         <v>461</v>
       </c>
-      <c r="F125" s="16" t="s">
+      <c r="F125" s="15" t="s">
         <v>461</v>
       </c>
     </row>
     <row r="126" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A126" s="16" t="s">
+      <c r="A126" s="15" t="s">
         <v>462</v>
       </c>
       <c r="B126" s="4" t="s">
@@ -4686,7 +4698,7 @@
       <c r="F133" s="3"/>
     </row>
     <row r="134" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A134" s="16" t="s">
+      <c r="A134" s="15" t="s">
         <v>471</v>
       </c>
       <c r="B134" s="4" t="s">

</xml_diff>

<commit_message>
Prepared files for codesignal
</commit_message>
<xml_diff>
--- a/LeetCode.xlsx
+++ b/LeetCode.xlsx
@@ -8,15 +8,16 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\EricS\Documents\VSCode Projects\LeetcodeGrind\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3E5CD070-412E-493D-A07F-332C45AFCBB9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4B45A91C-E703-431B-BC32-464F3E09C376}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="3" xr2:uid="{02D29AA1-7085-42F6-B3D4-4C0365DA5453}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="4" xr2:uid="{02D29AA1-7085-42F6-B3D4-4C0365DA5453}"/>
   </bookViews>
   <sheets>
     <sheet name="Easy" sheetId="1" r:id="rId1"/>
     <sheet name="Medium" sheetId="2" r:id="rId2"/>
     <sheet name="Hard" sheetId="4" r:id="rId3"/>
     <sheet name="Neetcode" sheetId="3" r:id="rId4"/>
+    <sheet name="CodeSignal" sheetId="5" r:id="rId5"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -39,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="696" uniqueCount="486">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="723" uniqueCount="497">
   <si>
     <t>Roman to Integer:</t>
   </si>
@@ -1500,6 +1501,39 @@
   </si>
   <si>
     <t>Can technically fit into 2 n length arrays but pain</t>
+  </si>
+  <si>
+    <t>https://github.com/Leader-board/OA-and-Interviews/blob/main/Online%20Assessments.md#codesignal</t>
+  </si>
+  <si>
+    <t>Q3</t>
+  </si>
+  <si>
+    <t>Spiral Matrix</t>
+  </si>
+  <si>
+    <t>Spiral Matrix 2</t>
+  </si>
+  <si>
+    <t>Rotate Image</t>
+  </si>
+  <si>
+    <t>Diagonal Traverse</t>
+  </si>
+  <si>
+    <t>Reshape Matrix</t>
+  </si>
+  <si>
+    <t>Toeplitz Matrix</t>
+  </si>
+  <si>
+    <t>Image Overlap</t>
+  </si>
+  <si>
+    <t>Transpose Matrix</t>
+  </si>
+  <si>
+    <t>Text Justification</t>
   </si>
 </sst>
 </file>
@@ -1606,7 +1640,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="21">
+  <cellXfs count="24">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -1668,12 +1702,199 @@
     <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="3">
+  <dxfs count="21">
+    <dxf>
+      <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <font>
         <color rgb="FF006100"/>
@@ -2568,8 +2789,8 @@
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:G969"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A118" zoomScale="81" zoomScaleNormal="122" workbookViewId="0">
-      <selection activeCell="D123" sqref="D123"/>
+    <sheetView zoomScale="81" zoomScaleNormal="122" workbookViewId="0">
+      <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -8922,13 +9143,13 @@
   </mergeCells>
   <phoneticPr fontId="3" type="noConversion"/>
   <conditionalFormatting sqref="C1:C124 C126:C1048576">
-    <cfRule type="containsText" dxfId="2" priority="1" operator="containsText" text="Hard">
+    <cfRule type="containsText" dxfId="20" priority="1" operator="containsText" text="Hard">
       <formula>NOT(ISERROR(SEARCH("Hard",C1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="1" priority="2" operator="containsText" text="Med">
+    <cfRule type="containsText" dxfId="19" priority="2" operator="containsText" text="Med">
       <formula>NOT(ISERROR(SEARCH("Med",C1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="0" priority="3" operator="containsText" text="Easy">
+    <cfRule type="containsText" dxfId="18" priority="3" operator="containsText" text="Easy">
       <formula>NOT(ISERROR(SEARCH("Easy",C1)))</formula>
     </cfRule>
   </conditionalFormatting>
@@ -8938,4 +9159,161 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId2"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6933FBFC-44BD-4904-99DA-B0AF53F41F06}">
+  <dimension ref="A1:G11"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F10" sqref="F10"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="16.85546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11.140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="8.42578125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A1" s="22" t="s">
+        <v>486</v>
+      </c>
+      <c r="B1" s="21"/>
+      <c r="C1" s="21"/>
+      <c r="D1" s="21"/>
+      <c r="E1" s="21"/>
+      <c r="F1" s="21"/>
+      <c r="G1" s="21"/>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A2" s="15" t="s">
+        <v>110</v>
+      </c>
+      <c r="B2" s="8" t="s">
+        <v>37</v>
+      </c>
+      <c r="C2" s="8" t="s">
+        <v>160</v>
+      </c>
+      <c r="D2" s="8" t="s">
+        <v>38</v>
+      </c>
+      <c r="E2" s="8" t="s">
+        <v>39</v>
+      </c>
+      <c r="F2" s="8" t="s">
+        <v>41</v>
+      </c>
+      <c r="G2" s="8" t="s">
+        <v>373</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A3" s="23" t="s">
+        <v>487</v>
+      </c>
+      <c r="B3" t="s">
+        <v>488</v>
+      </c>
+      <c r="C3" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B4" t="s">
+        <v>489</v>
+      </c>
+      <c r="C4" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B5" t="s">
+        <v>490</v>
+      </c>
+      <c r="C5" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B6" t="s">
+        <v>491</v>
+      </c>
+      <c r="C6" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B7" t="s">
+        <v>492</v>
+      </c>
+      <c r="C7" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B8" t="s">
+        <v>493</v>
+      </c>
+      <c r="C8" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B9" t="s">
+        <v>494</v>
+      </c>
+      <c r="C9" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B10" t="s">
+        <v>495</v>
+      </c>
+      <c r="C10" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B11" t="s">
+        <v>496</v>
+      </c>
+      <c r="C11" t="s">
+        <v>142</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="A1:G1"/>
+  </mergeCells>
+  <conditionalFormatting sqref="C2">
+    <cfRule type="containsText" dxfId="10" priority="4" operator="containsText" text="Hard">
+      <formula>NOT(ISERROR(SEARCH("Hard",C2)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="9" priority="5" operator="containsText" text="Med">
+      <formula>NOT(ISERROR(SEARCH("Med",C2)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="8" priority="6" operator="containsText" text="Easy">
+      <formula>NOT(ISERROR(SEARCH("Easy",C2)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C1:C1048576">
+    <cfRule type="cellIs" dxfId="0" priority="3" operator="equal">
+      <formula>"Med"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="1" priority="2" operator="equal">
+      <formula>"Easy"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="2" priority="1" operator="equal">
+      <formula>"Hard"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <hyperlinks>
+    <hyperlink ref="A1" r:id="rId1" location="codesignal" xr:uid="{FDD3F645-9AE9-4B2C-9C20-391FDBD2E2E2}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Finished spiral matrix 2
</commit_message>
<xml_diff>
--- a/LeetCode.xlsx
+++ b/LeetCode.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\EricS\Documents\VSCode Projects\LeetcodeGrind\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{56AD4A33-2907-427C-AC46-BA681999A9D4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C7415BA7-5812-4D99-801A-4E83B7F87D8B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="4" xr2:uid="{02D29AA1-7085-42F6-B3D4-4C0365DA5453}"/>
   </bookViews>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="725" uniqueCount="499">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="727" uniqueCount="501">
   <si>
     <t>Roman to Integer:</t>
   </si>
@@ -1540,6 +1540,12 @@
   </si>
   <si>
     <t>Track the 4 sides boundaries with 4 integers and do 4 loops going across top, down on the right, across bottom, up on the left, incrementing the bounds as necessary and making loops based on the bounds</t>
+  </si>
+  <si>
+    <t>Fill in square matrix using a spiral pattern going from 1 to n^2</t>
+  </si>
+  <si>
+    <t>Same thing as spiral matrix but filling in instead of adding to list</t>
   </si>
 </sst>
 </file>
@@ -9178,7 +9184,7 @@
   <dimension ref="A1:G11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D4" sqref="D4"/>
+      <selection activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -9246,6 +9252,12 @@
       </c>
       <c r="C4" t="s">
         <v>119</v>
+      </c>
+      <c r="D4" s="25" t="s">
+        <v>499</v>
+      </c>
+      <c r="E4" s="25" t="s">
+        <v>500</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Finished diagonal traverse and text justification
</commit_message>
<xml_diff>
--- a/LeetCode.xlsx
+++ b/LeetCode.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\EricS\Documents\VSCode Projects\LeetcodeGrind\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{68963FB0-2101-427B-B758-F2858EF025FA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3E49B8FF-9853-4073-BF9E-52E5E5A4D22C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="4" xr2:uid="{02D29AA1-7085-42F6-B3D4-4C0365DA5453}"/>
   </bookViews>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="730" uniqueCount="504">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="749" uniqueCount="516">
   <si>
     <t>Roman to Integer:</t>
   </si>
@@ -1555,13 +1555,49 @@
   </si>
   <si>
     <t>Keep track of ring and offset, loop through rings 0 to n // 2 and offset from 0 to n - 2 * r - 1, use a temp variable and figure out how to get the 4 correct slots based on ring and offset and shift the 4 around</t>
+  </si>
+  <si>
+    <t>Traverse matrix in alternating diagonals</t>
+  </si>
+  <si>
+    <t>Have things to track location and direction, change direction when you reach certain edges where you only increment one pointer, then you just keep traversing diagonal and adding to ret</t>
+  </si>
+  <si>
+    <t>Q4</t>
+  </si>
+  <si>
+    <t>Longest Consecutive Sequence</t>
+  </si>
+  <si>
+    <t>Pairs Divisible 60</t>
+  </si>
+  <si>
+    <t>Longest Palindrome Concat</t>
+  </si>
+  <si>
+    <t>Doubled Pair Arr</t>
+  </si>
+  <si>
+    <t>3Sum Multiplicity</t>
+  </si>
+  <si>
+    <t>Count Nice Subarrays</t>
+  </si>
+  <si>
+    <t>K-Diff Pairs in Array</t>
+  </si>
+  <si>
+    <t>Special adding spaces to make text stick to edges</t>
+  </si>
+  <si>
+    <t>Lots of math to figure out how to calculate spaces between each word and figuring out where to stop words</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="10" x14ac:knownFonts="1">
+  <fonts count="12" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1639,6 +1675,20 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <u/>
+      <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -1661,7 +1711,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="26">
+  <cellXfs count="31">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -1735,6 +1785,17 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="11" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -9190,15 +9251,15 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6933FBFC-44BD-4904-99DA-B0AF53F41F06}">
-  <dimension ref="A1:G11"/>
+  <dimension ref="A1:G18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E5" sqref="E5"/>
+      <selection activeCell="D12" sqref="D12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="16.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="28.85546875" style="28" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="65" style="25" customWidth="1"/>
     <col min="5" max="5" width="109.28515625" style="25" customWidth="1"/>
     <col min="6" max="6" width="45.28515625" style="25" customWidth="1"/>
@@ -9208,7 +9269,7 @@
       <c r="A1" s="22" t="s">
         <v>486</v>
       </c>
-      <c r="B1" s="21"/>
+      <c r="B1" s="29"/>
       <c r="C1" s="21"/>
       <c r="D1" s="21"/>
       <c r="E1" s="21"/>
@@ -9219,7 +9280,7 @@
       <c r="A2" s="15" t="s">
         <v>110</v>
       </c>
-      <c r="B2" s="8" t="s">
+      <c r="B2" s="30" t="s">
         <v>37</v>
       </c>
       <c r="C2" s="8" t="s">
@@ -9242,7 +9303,7 @@
       <c r="A3" s="23" t="s">
         <v>487</v>
       </c>
-      <c r="B3" t="s">
+      <c r="B3" s="28" t="s">
         <v>488</v>
       </c>
       <c r="C3" t="s">
@@ -9256,7 +9317,7 @@
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B4" t="s">
+      <c r="B4" s="28" t="s">
         <v>489</v>
       </c>
       <c r="C4" t="s">
@@ -9270,7 +9331,7 @@
       </c>
     </row>
     <row r="5" spans="1:7" ht="30" x14ac:dyDescent="0.25">
-      <c r="B5" t="s">
+      <c r="B5" s="28" t="s">
         <v>490</v>
       </c>
       <c r="C5" t="s">
@@ -9286,52 +9347,127 @@
         <v>501</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B6" t="s">
+    <row r="6" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="B6" s="28" t="s">
         <v>491</v>
       </c>
       <c r="C6" t="s">
         <v>119</v>
       </c>
+      <c r="D6" s="25" t="s">
+        <v>504</v>
+      </c>
+      <c r="E6" s="25" t="s">
+        <v>505</v>
+      </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B7" t="s">
+      <c r="B7" s="26" t="s">
         <v>492</v>
       </c>
-      <c r="C7" t="s">
+      <c r="C7" s="26" t="s">
         <v>112</v>
       </c>
+      <c r="D7" s="27"/>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B8" t="s">
+      <c r="B8" s="26" t="s">
         <v>493</v>
       </c>
-      <c r="C8" t="s">
+      <c r="C8" s="26" t="s">
         <v>112</v>
       </c>
+      <c r="D8" s="27"/>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B9" t="s">
+      <c r="B9" s="26" t="s">
         <v>494</v>
       </c>
-      <c r="C9" t="s">
-        <v>119</v>
-      </c>
+      <c r="C9" s="26" t="s">
+        <v>119</v>
+      </c>
+      <c r="D9" s="27"/>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B10" t="s">
+      <c r="B10" s="26" t="s">
         <v>495</v>
       </c>
-      <c r="C10" t="s">
+      <c r="C10" s="26" t="s">
         <v>112</v>
       </c>
+      <c r="D10" s="27"/>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B11" t="s">
+      <c r="B11" s="28" t="s">
         <v>496</v>
       </c>
       <c r="C11" t="s">
         <v>142</v>
+      </c>
+      <c r="D11" s="25" t="s">
+        <v>514</v>
+      </c>
+      <c r="E11" s="25" t="s">
+        <v>515</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A12" s="23" t="s">
+        <v>506</v>
+      </c>
+      <c r="B12" s="28" t="s">
+        <v>507</v>
+      </c>
+      <c r="C12" s="26" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B13" s="28" t="s">
+        <v>508</v>
+      </c>
+      <c r="C13" s="26" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B14" s="28" t="s">
+        <v>509</v>
+      </c>
+      <c r="C14" s="26" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B15" s="28" t="s">
+        <v>510</v>
+      </c>
+      <c r="C15" s="26" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B16" s="28" t="s">
+        <v>511</v>
+      </c>
+      <c r="C16" s="26" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="17" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B17" s="28" t="s">
+        <v>512</v>
+      </c>
+      <c r="C17" s="26" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="18" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B18" s="28" t="s">
+        <v>513</v>
+      </c>
+      <c r="C18" s="26" t="s">
+        <v>119</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Finished longest consec seq
</commit_message>
<xml_diff>
--- a/LeetCode.xlsx
+++ b/LeetCode.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\EricS\Documents\VSCode Projects\LeetcodeGrind\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3E49B8FF-9853-4073-BF9E-52E5E5A4D22C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{59323049-A69C-41F3-8E71-04FA161B5D0F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="4" xr2:uid="{02D29AA1-7085-42F6-B3D4-4C0365DA5453}"/>
   </bookViews>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="749" uniqueCount="516">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="751" uniqueCount="518">
   <si>
     <t>Roman to Integer:</t>
   </si>
@@ -1591,6 +1591,12 @@
   </si>
   <si>
     <t>Lots of math to figure out how to calculate spaces between each word and figuring out where to stop words</t>
+  </si>
+  <si>
+    <t>find len of longest consecutive sequence possible created from array</t>
+  </si>
+  <si>
+    <t>sort and count or convert to set and check n - 1 over and over and keep track of max</t>
   </si>
 </sst>
 </file>
@@ -2877,8 +2883,8 @@
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:G969"/>
   <sheetViews>
-    <sheetView zoomScale="81" zoomScaleNormal="122" workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+    <sheetView topLeftCell="A120" zoomScale="81" zoomScaleNormal="122" workbookViewId="0">
+      <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -9254,7 +9260,7 @@
   <dimension ref="A1:G18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D12" sqref="D12"/>
+      <selection activeCell="D13" sqref="D13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -9420,6 +9426,12 @@
       </c>
       <c r="C12" s="26" t="s">
         <v>119</v>
+      </c>
+      <c r="D12" s="25" t="s">
+        <v>516</v>
+      </c>
+      <c r="E12" s="25" t="s">
+        <v>517</v>
       </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Finished pairs divis 60
</commit_message>
<xml_diff>
--- a/LeetCode.xlsx
+++ b/LeetCode.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\EricS\Documents\VSCode Projects\LeetcodeGrind\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{59323049-A69C-41F3-8E71-04FA161B5D0F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1A994C12-0555-4A61-A7D9-1827B957F2B9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="4" xr2:uid="{02D29AA1-7085-42F6-B3D4-4C0365DA5453}"/>
   </bookViews>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="751" uniqueCount="518">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="753" uniqueCount="520">
   <si>
     <t>Roman to Integer:</t>
   </si>
@@ -1597,6 +1597,12 @@
   </si>
   <si>
     <t>sort and count or convert to set and check n - 1 over and over and keep track of max</t>
+  </si>
+  <si>
+    <t>count pairs that sum to number divisible by 60</t>
+  </si>
+  <si>
+    <t>get modulos and loop through counts</t>
   </si>
 </sst>
 </file>
@@ -9260,7 +9266,7 @@
   <dimension ref="A1:G18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D13" sqref="D13"/>
+      <selection activeCell="E14" sqref="E14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -9440,6 +9446,12 @@
       </c>
       <c r="C13" s="26" t="s">
         <v>119</v>
+      </c>
+      <c r="D13" s="25" t="s">
+        <v>518</v>
+      </c>
+      <c r="E13" s="25" t="s">
+        <v>519</v>
       </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Finished longest palindrome w 2 letter words and doubled pair array
</commit_message>
<xml_diff>
--- a/LeetCode.xlsx
+++ b/LeetCode.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\EricS\Documents\VSCode Projects\LeetcodeGrind\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1A994C12-0555-4A61-A7D9-1827B957F2B9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FD2AE0DB-C3A0-4EF6-81D3-18C00DF97E59}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="4" xr2:uid="{02D29AA1-7085-42F6-B3D4-4C0365DA5453}"/>
   </bookViews>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="753" uniqueCount="520">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="757" uniqueCount="524">
   <si>
     <t>Roman to Integer:</t>
   </si>
@@ -1593,16 +1593,28 @@
     <t>Lots of math to figure out how to calculate spaces between each word and figuring out where to stop words</t>
   </si>
   <si>
-    <t>find len of longest consecutive sequence possible created from array</t>
-  </si>
-  <si>
-    <t>sort and count or convert to set and check n - 1 over and over and keep track of max</t>
-  </si>
-  <si>
-    <t>count pairs that sum to number divisible by 60</t>
-  </si>
-  <si>
-    <t>get modulos and loop through counts</t>
+    <t>Find len of longest palindrome you can form from list of 2 letter words</t>
+  </si>
+  <si>
+    <t>Count pairs that sum to number divisible by 60</t>
+  </si>
+  <si>
+    <t>Find len of longest consecutive sequence possible created from array</t>
+  </si>
+  <si>
+    <t>Sort and count or convert to set and check n - 1 over and over and keep track of max</t>
+  </si>
+  <si>
+    <t>Get modulos and loop through counts</t>
+  </si>
+  <si>
+    <t>Count the occurrence of each word, then loop through and check reverses (only check first half), if both letters are the same mid is a boolean to track if there's an odd one out, otherwise you floor division by 2 to get how many you can insert on each side, at the end you check if mid then you add 2 more to ret</t>
+  </si>
+  <si>
+    <t>Check if it's possible to pair all elements in array with its double/half</t>
+  </si>
+  <si>
+    <t>Use unordered_map, count all unique elements, sort elements by absolute value, traverse and subtract each one from it's double, return false if double doesn't exist or doesn't have enough, can stop early after processing half of the numbers (only count the small half)</t>
   </si>
 </sst>
 </file>
@@ -1867,6 +1879,16 @@
     </dxf>
     <dxf>
       <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
         <color rgb="FF006100"/>
       </font>
       <fill>
@@ -1917,26 +1939,6 @@
     </dxf>
     <dxf>
       <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C5700"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
         <color rgb="FF006100"/>
       </font>
       <fill>
@@ -1962,6 +1964,16 @@
       <fill>
         <patternFill>
           <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
         </patternFill>
       </fill>
     </dxf>
@@ -9243,13 +9255,13 @@
   </mergeCells>
   <phoneticPr fontId="3" type="noConversion"/>
   <conditionalFormatting sqref="C1:C124 C126:C1048576">
-    <cfRule type="containsText" dxfId="20" priority="1" operator="containsText" text="Hard">
+    <cfRule type="containsText" dxfId="8" priority="1" operator="containsText" text="Hard">
       <formula>NOT(ISERROR(SEARCH("Hard",C1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="19" priority="2" operator="containsText" text="Med">
+    <cfRule type="containsText" dxfId="7" priority="2" operator="containsText" text="Med">
       <formula>NOT(ISERROR(SEARCH("Med",C1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="18" priority="3" operator="containsText" text="Easy">
+    <cfRule type="containsText" dxfId="6" priority="3" operator="containsText" text="Easy">
       <formula>NOT(ISERROR(SEARCH("Easy",C1)))</formula>
     </cfRule>
   </conditionalFormatting>
@@ -9266,7 +9278,7 @@
   <dimension ref="A1:G18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E14" sqref="E14"/>
+      <selection activeCell="D16" sqref="D16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -9434,10 +9446,10 @@
         <v>119</v>
       </c>
       <c r="D12" s="25" t="s">
-        <v>516</v>
+        <v>518</v>
       </c>
       <c r="E12" s="25" t="s">
-        <v>517</v>
+        <v>519</v>
       </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.25">
@@ -9448,26 +9460,38 @@
         <v>119</v>
       </c>
       <c r="D13" s="25" t="s">
-        <v>518</v>
+        <v>517</v>
       </c>
       <c r="E13" s="25" t="s">
-        <v>519</v>
-      </c>
-    </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+        <v>520</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" ht="45" x14ac:dyDescent="0.25">
       <c r="B14" s="28" t="s">
         <v>509</v>
       </c>
       <c r="C14" s="26" t="s">
         <v>119</v>
       </c>
-    </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="D14" s="25" t="s">
+        <v>516</v>
+      </c>
+      <c r="E14" s="25" t="s">
+        <v>521</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" ht="45" x14ac:dyDescent="0.25">
       <c r="B15" s="28" t="s">
         <v>510</v>
       </c>
       <c r="C15" s="26" t="s">
         <v>119</v>
+      </c>
+      <c r="D15" s="25" t="s">
+        <v>522</v>
+      </c>
+      <c r="E15" s="25" t="s">
+        <v>523</v>
       </c>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.25">
@@ -9499,25 +9523,25 @@
     <mergeCell ref="A1:G1"/>
   </mergeCells>
   <conditionalFormatting sqref="C2">
-    <cfRule type="containsText" dxfId="10" priority="4" operator="containsText" text="Hard">
+    <cfRule type="containsText" dxfId="5" priority="4" operator="containsText" text="Hard">
       <formula>NOT(ISERROR(SEARCH("Hard",C2)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="9" priority="5" operator="containsText" text="Med">
+    <cfRule type="containsText" dxfId="4" priority="5" operator="containsText" text="Med">
       <formula>NOT(ISERROR(SEARCH("Med",C2)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="8" priority="6" operator="containsText" text="Easy">
+    <cfRule type="containsText" dxfId="3" priority="6" operator="containsText" text="Easy">
       <formula>NOT(ISERROR(SEARCH("Easy",C2)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C1:C1048576">
-    <cfRule type="cellIs" dxfId="0" priority="3" operator="equal">
-      <formula>"Med"</formula>
+    <cfRule type="cellIs" dxfId="2" priority="1" operator="equal">
+      <formula>"Hard"</formula>
     </cfRule>
     <cfRule type="cellIs" dxfId="1" priority="2" operator="equal">
       <formula>"Easy"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="2" priority="1" operator="equal">
-      <formula>"Hard"</formula>
+    <cfRule type="cellIs" dxfId="0" priority="3" operator="equal">
+      <formula>"Med"</formula>
     </cfRule>
   </conditionalFormatting>
   <hyperlinks>

</xml_diff>

<commit_message>
Finished 3sum w multiplicity
</commit_message>
<xml_diff>
--- a/LeetCode.xlsx
+++ b/LeetCode.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\EricS\Documents\VSCode Projects\LeetcodeGrind\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FD2AE0DB-C3A0-4EF6-81D3-18C00DF97E59}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6918BCA4-33D8-4D56-B196-9CBF7387B18B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="4" xr2:uid="{02D29AA1-7085-42F6-B3D4-4C0365DA5453}"/>
   </bookViews>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="757" uniqueCount="524">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="759" uniqueCount="526">
   <si>
     <t>Roman to Integer:</t>
   </si>
@@ -1615,6 +1615,12 @@
   </si>
   <si>
     <t>Use unordered_map, count all unique elements, sort elements by absolute value, traverse and subtract each one from it's double, return false if double doesn't exist or doesn't have enough, can stop early after processing half of the numbers (only count the small half)</t>
+  </si>
+  <si>
+    <t>3 sum but numbers are repeated</t>
+  </si>
+  <si>
+    <t>Use unordered map to do counting, loop through all unique values and check 3 scenarios with value1, value2, value3 = target - value1 - value2. First, if value3 no exist, continue. 3 scenarios are v1 == v2 == v3 in which case we have the same element thrice, we just need to do track[v1] * (track[v1] - 1]) * (track[v1] - 2) / 6 to account for duplicates and still consider all possibilities. Scenario 2 is v1 == v2 != v3, where we would have track[v1] * (track[v1] - 1) / 2 * track[v3] for same reasons. Final scenario is v1 &lt; v2 &lt; v3, we need this specific condition to avoid double counting, then we increment ret as needed and do modulos and long to int conversion as necessary</t>
   </si>
 </sst>
 </file>
@@ -9278,7 +9284,7 @@
   <dimension ref="A1:G18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D16" sqref="D16"/>
+      <selection activeCell="D17" sqref="D17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -9494,12 +9500,18 @@
         <v>523</v>
       </c>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:7" ht="90" x14ac:dyDescent="0.25">
       <c r="B16" s="28" t="s">
         <v>511</v>
       </c>
       <c r="C16" s="26" t="s">
         <v>119</v>
+      </c>
+      <c r="D16" s="25" t="s">
+        <v>524</v>
+      </c>
+      <c r="E16" s="25" t="s">
+        <v>525</v>
       </c>
     </row>
     <row r="17" spans="2:3" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Finished count nice subarrs
</commit_message>
<xml_diff>
--- a/LeetCode.xlsx
+++ b/LeetCode.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\EricS\Documents\VSCode Projects\LeetcodeGrind\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6918BCA4-33D8-4D56-B196-9CBF7387B18B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A04BA46A-DEF1-48F3-A307-77246A10A92C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="4" xr2:uid="{02D29AA1-7085-42F6-B3D4-4C0365DA5453}"/>
   </bookViews>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="759" uniqueCount="526">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="761" uniqueCount="528">
   <si>
     <t>Roman to Integer:</t>
   </si>
@@ -1621,6 +1621,12 @@
   </si>
   <si>
     <t>Use unordered map to do counting, loop through all unique values and check 3 scenarios with value1, value2, value3 = target - value1 - value2. First, if value3 no exist, continue. 3 scenarios are v1 == v2 == v3 in which case we have the same element thrice, we just need to do track[v1] * (track[v1] - 1]) * (track[v1] - 2) / 6 to account for duplicates and still consider all possibilities. Scenario 2 is v1 == v2 != v3, where we would have track[v1] * (track[v1] - 1) / 2 * track[v3] for same reasons. Final scenario is v1 &lt; v2 &lt; v3, we need this specific condition to avoid double counting, then we increment ret as needed and do modulos and long to int conversion as necessary</t>
+  </si>
+  <si>
+    <t>Given array of nums, count number of subarrays where there are exactly k odds</t>
+  </si>
+  <si>
+    <t>Loop through to get all indices of odds, then traverse using window and look at left buffer and right buffer and calculate accordingly. Another solution is to use prefix sum like method of tracking how many ways there are to create subarrays of each number of odd numbers, then figure out how many ways you can add and remove front portions to create exactly k (read comments in github code since hard to explain prefix sum solution)</t>
   </si>
 </sst>
 </file>
@@ -9284,7 +9290,7 @@
   <dimension ref="A1:G18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D17" sqref="D17"/>
+      <selection activeCell="E18" sqref="E18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -9514,15 +9520,21 @@
         <v>525</v>
       </c>
     </row>
-    <row r="17" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="17" spans="2:5" ht="60" x14ac:dyDescent="0.25">
       <c r="B17" s="28" t="s">
         <v>512</v>
       </c>
       <c r="C17" s="26" t="s">
         <v>119</v>
       </c>
-    </row>
-    <row r="18" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="D17" s="25" t="s">
+        <v>526</v>
+      </c>
+      <c r="E17" s="25" t="s">
+        <v>527</v>
+      </c>
+    </row>
+    <row r="18" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B18" s="28" t="s">
         <v>513</v>
       </c>

</xml_diff>

<commit_message>
Finally finished burst balloon problem
</commit_message>
<xml_diff>
--- a/LeetCode.xlsx
+++ b/LeetCode.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\EricS\Documents\VSCode Projects\LeetcodeGrind\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2571E47F-9708-404D-8D20-9A2E97179E4D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A7526594-000F-458C-B115-4C47710E06D5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="4" xr2:uid="{02D29AA1-7085-42F6-B3D4-4C0365DA5453}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="3" xr2:uid="{02D29AA1-7085-42F6-B3D4-4C0365DA5453}"/>
   </bookViews>
   <sheets>
     <sheet name="Easy" sheetId="1" r:id="rId1"/>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="763" uniqueCount="530">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="765" uniqueCount="532">
   <si>
     <t>Roman to Integer:</t>
   </si>
@@ -1633,6 +1633,12 @@
   </si>
   <si>
     <t>Same thing as longest consecutive sequence except check -k, unless target difference is 0 then you have to count numbers that occur more than once. Alternate solution is to sort and then use sliding window</t>
+  </si>
+  <si>
+    <t>Given array of balloon values and that popping a balloon gives you left neighbor * balloon * right neighbor points, determine max amount of points you can get, neighbors are = 1 if neighbors don't exist</t>
+  </si>
+  <si>
+    <t>The essence is you realize the subproblem is actually which balloon you pop last, since popping last you know what the left and right neighbors would be. This allows us to get an O(N^3) solution. To be smart, we realize we can use table dp if we do each subarray of each possible length increasingly, so all subarrays of length 1 first, then 2, and so on. This way, when we take the last pop and try to see the left and right side, we know those are shorter and are already in the table before. Then, given offset/length, we loop through all possible left starting indices and calculate right index from these 2. Then, we loop between left and right and try all possible last pop balloons, setting dp value to be the best.</t>
   </si>
 </sst>
 </file>
@@ -1753,7 +1759,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="31">
+  <cellXfs count="30">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -1812,149 +1818,36 @@
     <xf numFmtId="49" fontId="9" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="49" fontId="11" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
     <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="49" fontId="11" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="21">
-    <dxf>
-      <font>
-        <color rgb="FF9C5700"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C5700"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C5700"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C5700"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="9">
     <dxf>
       <font>
         <color rgb="FF006100"/>
@@ -2002,16 +1895,6 @@
       <fill>
         <patternFill>
           <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C5700"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
         </patternFill>
       </fill>
     </dxf>
@@ -2919,8 +2802,8 @@
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:G969"/>
   <sheetViews>
-    <sheetView topLeftCell="A120" zoomScale="81" zoomScaleNormal="122" workbookViewId="0">
-      <selection activeCell="B10" sqref="B10"/>
+    <sheetView tabSelected="1" topLeftCell="A119" zoomScale="81" zoomScaleNormal="122" workbookViewId="0">
+      <selection activeCell="D124" sqref="D124"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2937,14 +2820,14 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A1" s="20" t="s">
+      <c r="A1" s="26" t="s">
         <v>111</v>
       </c>
-      <c r="B1" s="20"/>
-      <c r="C1" s="20"/>
-      <c r="D1" s="20"/>
-      <c r="E1" s="20"/>
-      <c r="F1" s="20"/>
+      <c r="B1" s="26"/>
+      <c r="C1" s="26"/>
+      <c r="D1" s="26"/>
+      <c r="E1" s="26"/>
+      <c r="F1" s="26"/>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" s="15" t="s">
@@ -4915,7 +4798,7 @@
         <v>485</v>
       </c>
     </row>
-    <row r="123" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="123" spans="1:6" ht="90" x14ac:dyDescent="0.25">
       <c r="A123" s="5"/>
       <c r="B123" s="4" t="s">
         <v>414</v>
@@ -4923,8 +4806,12 @@
       <c r="C123" s="4" t="s">
         <v>142</v>
       </c>
-      <c r="D123" s="3"/>
-      <c r="E123" s="3"/>
+      <c r="D123" s="3" t="s">
+        <v>530</v>
+      </c>
+      <c r="E123" s="3" t="s">
+        <v>531</v>
+      </c>
       <c r="F123" s="3"/>
     </row>
     <row r="124" spans="1:6" x14ac:dyDescent="0.25">
@@ -9295,46 +9182,46 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6933FBFC-44BD-4904-99DA-B0AF53F41F06}">
   <dimension ref="A1:G18"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView topLeftCell="A15" workbookViewId="0">
       <selection activeCell="E18" sqref="E18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="28.85546875" style="28" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="65" style="25" customWidth="1"/>
-    <col min="5" max="5" width="109.28515625" style="25" customWidth="1"/>
-    <col min="6" max="6" width="45.28515625" style="25" customWidth="1"/>
+    <col min="2" max="2" width="28.85546875" style="24" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="65" style="17" customWidth="1"/>
+    <col min="5" max="5" width="109.28515625" style="17" customWidth="1"/>
+    <col min="6" max="6" width="45.28515625" style="17" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A1" s="22" t="s">
+      <c r="A1" s="27" t="s">
         <v>486</v>
       </c>
-      <c r="B1" s="29"/>
-      <c r="C1" s="21"/>
-      <c r="D1" s="21"/>
-      <c r="E1" s="21"/>
-      <c r="F1" s="21"/>
-      <c r="G1" s="21"/>
+      <c r="B1" s="28"/>
+      <c r="C1" s="29"/>
+      <c r="D1" s="29"/>
+      <c r="E1" s="29"/>
+      <c r="F1" s="29"/>
+      <c r="G1" s="29"/>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" s="15" t="s">
         <v>110</v>
       </c>
-      <c r="B2" s="30" t="s">
+      <c r="B2" s="25" t="s">
         <v>37</v>
       </c>
       <c r="C2" s="8" t="s">
         <v>160</v>
       </c>
-      <c r="D2" s="24" t="s">
+      <c r="D2" s="21" t="s">
         <v>38</v>
       </c>
-      <c r="E2" s="24" t="s">
+      <c r="E2" s="21" t="s">
         <v>39</v>
       </c>
-      <c r="F2" s="24" t="s">
+      <c r="F2" s="21" t="s">
         <v>41</v>
       </c>
       <c r="G2" s="8" t="s">
@@ -9342,215 +9229,215 @@
       </c>
     </row>
     <row r="3" spans="1:7" ht="30" x14ac:dyDescent="0.25">
-      <c r="A3" s="23" t="s">
+      <c r="A3" s="20" t="s">
         <v>487</v>
       </c>
-      <c r="B3" s="28" t="s">
+      <c r="B3" s="24" t="s">
         <v>488</v>
       </c>
       <c r="C3" t="s">
         <v>119</v>
       </c>
-      <c r="D3" s="25" t="s">
+      <c r="D3" s="17" t="s">
         <v>497</v>
       </c>
-      <c r="E3" s="25" t="s">
+      <c r="E3" s="17" t="s">
         <v>498</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B4" s="28" t="s">
+      <c r="B4" s="24" t="s">
         <v>489</v>
       </c>
       <c r="C4" t="s">
         <v>119</v>
       </c>
-      <c r="D4" s="25" t="s">
+      <c r="D4" s="17" t="s">
         <v>499</v>
       </c>
-      <c r="E4" s="25" t="s">
+      <c r="E4" s="17" t="s">
         <v>500</v>
       </c>
     </row>
     <row r="5" spans="1:7" ht="30" x14ac:dyDescent="0.25">
-      <c r="B5" s="28" t="s">
+      <c r="B5" s="24" t="s">
         <v>490</v>
       </c>
       <c r="C5" t="s">
         <v>119</v>
       </c>
-      <c r="D5" s="25" t="s">
+      <c r="D5" s="17" t="s">
         <v>502</v>
       </c>
-      <c r="E5" s="25" t="s">
+      <c r="E5" s="17" t="s">
         <v>503</v>
       </c>
-      <c r="F5" s="25" t="s">
+      <c r="F5" s="17" t="s">
         <v>501</v>
       </c>
     </row>
     <row r="6" spans="1:7" ht="30" x14ac:dyDescent="0.25">
-      <c r="B6" s="28" t="s">
+      <c r="B6" s="24" t="s">
         <v>491</v>
       </c>
       <c r="C6" t="s">
         <v>119</v>
       </c>
-      <c r="D6" s="25" t="s">
+      <c r="D6" s="17" t="s">
         <v>504</v>
       </c>
-      <c r="E6" s="25" t="s">
+      <c r="E6" s="17" t="s">
         <v>505</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B7" s="26" t="s">
+      <c r="B7" s="22" t="s">
         <v>492</v>
       </c>
-      <c r="C7" s="26" t="s">
+      <c r="C7" s="22" t="s">
         <v>112</v>
       </c>
-      <c r="D7" s="27"/>
+      <c r="D7" s="23"/>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B8" s="26" t="s">
+      <c r="B8" s="22" t="s">
         <v>493</v>
       </c>
-      <c r="C8" s="26" t="s">
+      <c r="C8" s="22" t="s">
         <v>112</v>
       </c>
-      <c r="D8" s="27"/>
+      <c r="D8" s="23"/>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B9" s="26" t="s">
+      <c r="B9" s="22" t="s">
         <v>494</v>
       </c>
-      <c r="C9" s="26" t="s">
-        <v>119</v>
-      </c>
-      <c r="D9" s="27"/>
+      <c r="C9" s="22" t="s">
+        <v>119</v>
+      </c>
+      <c r="D9" s="23"/>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B10" s="26" t="s">
+      <c r="B10" s="22" t="s">
         <v>495</v>
       </c>
-      <c r="C10" s="26" t="s">
+      <c r="C10" s="22" t="s">
         <v>112</v>
       </c>
-      <c r="D10" s="27"/>
+      <c r="D10" s="23"/>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B11" s="28" t="s">
+      <c r="B11" s="24" t="s">
         <v>496</v>
       </c>
       <c r="C11" t="s">
         <v>142</v>
       </c>
-      <c r="D11" s="25" t="s">
+      <c r="D11" s="17" t="s">
         <v>514</v>
       </c>
-      <c r="E11" s="25" t="s">
+      <c r="E11" s="17" t="s">
         <v>515</v>
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A12" s="23" t="s">
+      <c r="A12" s="20" t="s">
         <v>506</v>
       </c>
-      <c r="B12" s="28" t="s">
+      <c r="B12" s="24" t="s">
         <v>507</v>
       </c>
-      <c r="C12" s="26" t="s">
-        <v>119</v>
-      </c>
-      <c r="D12" s="25" t="s">
+      <c r="C12" s="22" t="s">
+        <v>119</v>
+      </c>
+      <c r="D12" s="17" t="s">
         <v>518</v>
       </c>
-      <c r="E12" s="25" t="s">
+      <c r="E12" s="17" t="s">
         <v>519</v>
       </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B13" s="28" t="s">
+      <c r="B13" s="24" t="s">
         <v>508</v>
       </c>
-      <c r="C13" s="26" t="s">
-        <v>119</v>
-      </c>
-      <c r="D13" s="25" t="s">
+      <c r="C13" s="22" t="s">
+        <v>119</v>
+      </c>
+      <c r="D13" s="17" t="s">
         <v>517</v>
       </c>
-      <c r="E13" s="25" t="s">
+      <c r="E13" s="17" t="s">
         <v>520</v>
       </c>
     </row>
     <row r="14" spans="1:7" ht="45" x14ac:dyDescent="0.25">
-      <c r="B14" s="28" t="s">
+      <c r="B14" s="24" t="s">
         <v>509</v>
       </c>
-      <c r="C14" s="26" t="s">
-        <v>119</v>
-      </c>
-      <c r="D14" s="25" t="s">
+      <c r="C14" s="22" t="s">
+        <v>119</v>
+      </c>
+      <c r="D14" s="17" t="s">
         <v>516</v>
       </c>
-      <c r="E14" s="25" t="s">
+      <c r="E14" s="17" t="s">
         <v>521</v>
       </c>
     </row>
     <row r="15" spans="1:7" ht="45" x14ac:dyDescent="0.25">
-      <c r="B15" s="28" t="s">
+      <c r="B15" s="24" t="s">
         <v>510</v>
       </c>
-      <c r="C15" s="26" t="s">
-        <v>119</v>
-      </c>
-      <c r="D15" s="25" t="s">
+      <c r="C15" s="22" t="s">
+        <v>119</v>
+      </c>
+      <c r="D15" s="17" t="s">
         <v>522</v>
       </c>
-      <c r="E15" s="25" t="s">
+      <c r="E15" s="17" t="s">
         <v>523</v>
       </c>
     </row>
     <row r="16" spans="1:7" ht="90" x14ac:dyDescent="0.25">
-      <c r="B16" s="28" t="s">
+      <c r="B16" s="24" t="s">
         <v>511</v>
       </c>
-      <c r="C16" s="26" t="s">
-        <v>119</v>
-      </c>
-      <c r="D16" s="25" t="s">
+      <c r="C16" s="22" t="s">
+        <v>119</v>
+      </c>
+      <c r="D16" s="17" t="s">
         <v>524</v>
       </c>
-      <c r="E16" s="25" t="s">
+      <c r="E16" s="17" t="s">
         <v>525</v>
       </c>
     </row>
     <row r="17" spans="2:5" ht="60" x14ac:dyDescent="0.25">
-      <c r="B17" s="28" t="s">
+      <c r="B17" s="24" t="s">
         <v>512</v>
       </c>
-      <c r="C17" s="26" t="s">
-        <v>119</v>
-      </c>
-      <c r="D17" s="25" t="s">
+      <c r="C17" s="22" t="s">
+        <v>119</v>
+      </c>
+      <c r="D17" s="17" t="s">
         <v>526</v>
       </c>
-      <c r="E17" s="25" t="s">
+      <c r="E17" s="17" t="s">
         <v>527</v>
       </c>
     </row>
     <row r="18" spans="2:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="B18" s="28" t="s">
+      <c r="B18" s="24" t="s">
         <v>513</v>
       </c>
-      <c r="C18" s="26" t="s">
-        <v>119</v>
-      </c>
-      <c r="D18" s="25" t="s">
+      <c r="C18" s="22" t="s">
+        <v>119</v>
+      </c>
+      <c r="D18" s="17" t="s">
         <v>528</v>
       </c>
-      <c r="E18" s="25" t="s">
+      <c r="E18" s="17" t="s">
         <v>529</v>
       </c>
     </row>
@@ -9558,26 +9445,26 @@
   <mergeCells count="1">
     <mergeCell ref="A1:G1"/>
   </mergeCells>
+  <conditionalFormatting sqref="C1:C1048576">
+    <cfRule type="cellIs" dxfId="5" priority="1" operator="equal">
+      <formula>"Hard"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="4" priority="2" operator="equal">
+      <formula>"Easy"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="3" priority="3" operator="equal">
+      <formula>"Med"</formula>
+    </cfRule>
+  </conditionalFormatting>
   <conditionalFormatting sqref="C2">
-    <cfRule type="containsText" dxfId="5" priority="4" operator="containsText" text="Hard">
+    <cfRule type="containsText" dxfId="2" priority="4" operator="containsText" text="Hard">
       <formula>NOT(ISERROR(SEARCH("Hard",C2)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="4" priority="5" operator="containsText" text="Med">
+    <cfRule type="containsText" dxfId="1" priority="5" operator="containsText" text="Med">
       <formula>NOT(ISERROR(SEARCH("Med",C2)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="3" priority="6" operator="containsText" text="Easy">
+    <cfRule type="containsText" dxfId="0" priority="6" operator="containsText" text="Easy">
       <formula>NOT(ISERROR(SEARCH("Easy",C2)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C1:C1048576">
-    <cfRule type="cellIs" dxfId="2" priority="1" operator="equal">
-      <formula>"Hard"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="1" priority="2" operator="equal">
-      <formula>"Easy"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="0" priority="3" operator="equal">
-      <formula>"Med"</formula>
     </cfRule>
   </conditionalFormatting>
   <hyperlinks>

</xml_diff>

<commit_message>
Finished regex matching and 2D DP
</commit_message>
<xml_diff>
--- a/LeetCode.xlsx
+++ b/LeetCode.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\EricS\Documents\VSCode Projects\LeetcodeGrind\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A7526594-000F-458C-B115-4C47710E06D5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C9BBC743-AC5C-4BF7-966C-2291DC84D759}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="3" xr2:uid="{02D29AA1-7085-42F6-B3D4-4C0365DA5453}"/>
   </bookViews>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="765" uniqueCount="532">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="767" uniqueCount="534">
   <si>
     <t>Roman to Integer:</t>
   </si>
@@ -1639,6 +1639,12 @@
   </si>
   <si>
     <t>The essence is you realize the subproblem is actually which balloon you pop last, since popping last you know what the left and right neighbors would be. This allows us to get an O(N^3) solution. To be smart, we realize we can use table dp if we do each subarray of each possible length increasingly, so all subarrays of length 1 first, then 2, and so on. This way, when we take the last pop and try to see the left and right side, we know those are shorter and are already in the table before. Then, given offset/length, we loop through all possible left starting indices and calculate right index from these 2. Then, we loop between left and right and try all possible last pop balloons, setting dp value to be the best.</t>
+  </si>
+  <si>
+    <t>Match pattern strings with . wildcard and * for one or more repeat of previous char as well as standard alphabet, return boolean if string and pattern match</t>
+  </si>
+  <si>
+    <t>Same thing as edit distance basically, do casework looking at . vs * vs same character and check the 2 dimensional track array accordingly for each one, with track[i][j] meaning p[:j] matches s[:i]. Will need loop at the start to populate first row, could also do other way of including that in the actual program but that's more painful</t>
   </si>
 </sst>
 </file>
@@ -2803,7 +2809,7 @@
   <dimension ref="A1:G969"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A119" zoomScale="81" zoomScaleNormal="122" workbookViewId="0">
-      <selection activeCell="D124" sqref="D124"/>
+      <selection activeCell="E125" sqref="E125"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4814,7 +4820,7 @@
       </c>
       <c r="F123" s="3"/>
     </row>
-    <row r="124" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="124" spans="1:6" ht="45" x14ac:dyDescent="0.25">
       <c r="A124" s="5"/>
       <c r="B124" s="4" t="s">
         <v>404</v>
@@ -4822,8 +4828,12 @@
       <c r="C124" s="4" t="s">
         <v>142</v>
       </c>
-      <c r="D124" s="3"/>
-      <c r="E124" s="3"/>
+      <c r="D124" s="3" t="s">
+        <v>532</v>
+      </c>
+      <c r="E124" s="3" t="s">
+        <v>533</v>
+      </c>
       <c r="F124" s="3"/>
     </row>
     <row r="125" spans="1:6" ht="30" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Finished reconstruct flight itinerary
</commit_message>
<xml_diff>
--- a/LeetCode.xlsx
+++ b/LeetCode.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\EricS\Documents\VSCode Projects\LeetcodeGrind\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C9BBC743-AC5C-4BF7-966C-2291DC84D759}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D8173D4F-337C-4485-B14D-32D64396B6FA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="3" xr2:uid="{02D29AA1-7085-42F6-B3D4-4C0365DA5453}"/>
   </bookViews>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="767" uniqueCount="534">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="765" uniqueCount="536">
   <si>
     <t>Roman to Integer:</t>
   </si>
@@ -1428,9 +1428,6 @@
     <t>Cheapest Flights Within K Stops</t>
   </si>
   <si>
-    <t>REMEMBER TO DO ADVANCED GRAPHS</t>
-  </si>
-  <si>
     <t>Greedy</t>
   </si>
   <si>
@@ -1645,6 +1642,15 @@
   </si>
   <si>
     <t>Same thing as edit distance basically, do casework looking at . vs * vs same character and check the 2 dimensional track array accordingly for each one, with track[i][j] meaning p[:j] matches s[:i]. Will need loop at the start to populate first row, could also do other way of including that in the actual program but that's more painful</t>
+  </si>
+  <si>
+    <t>Given list of departure and arrival tuples, determine the lexicographically smallest possible path given starting at JFK and every flight is used and valid path exists</t>
+  </si>
+  <si>
+    <t>first create hashmap to track all possible travel places using priority queue to keep them sorted, then you want to continue down every possible path until you reach end where you add to list, as this ensures the first thing added is the last place you can end up and then the second last and so on. Then reverse and return</t>
+  </si>
+  <si>
+    <t>DFS/backtracking works but too slow</t>
   </si>
 </sst>
 </file>
@@ -2806,10 +2812,10 @@
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{55ADB572-3F2B-41BB-A303-53CCEC27F096}">
   <sheetPr codeName="Sheet1"/>
-  <dimension ref="A1:G969"/>
+  <dimension ref="A1:G968"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A119" zoomScale="81" zoomScaleNormal="122" workbookViewId="0">
-      <selection activeCell="E125" sqref="E125"/>
+    <sheetView tabSelected="1" topLeftCell="A88" zoomScale="81" zoomScaleNormal="122" workbookViewId="0">
+      <selection activeCell="F95" sqref="F95"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2817,8 +2823,8 @@
     <col min="1" max="1" width="19.7109375" style="16" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="59.28515625" style="4" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="5.7109375" style="4" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="56.42578125" style="4" customWidth="1"/>
-    <col min="5" max="5" width="111.42578125" style="4" customWidth="1"/>
+    <col min="4" max="4" width="56.42578125" style="5" customWidth="1"/>
+    <col min="5" max="5" width="111.42578125" style="5" customWidth="1"/>
     <col min="6" max="6" width="43.42578125" style="4" customWidth="1"/>
     <col min="7" max="7" width="91.140625" style="5" customWidth="1"/>
     <col min="8" max="8" width="82.28515625" style="4" customWidth="1"/>
@@ -2845,10 +2851,10 @@
       <c r="C2" s="8" t="s">
         <v>160</v>
       </c>
-      <c r="D2" s="8" t="s">
+      <c r="D2" s="15" t="s">
         <v>38</v>
       </c>
-      <c r="E2" s="8" t="s">
+      <c r="E2" s="15" t="s">
         <v>39</v>
       </c>
       <c r="F2" s="8" t="s">
@@ -2926,7 +2932,7 @@
         <v>126</v>
       </c>
     </row>
-    <row r="7" spans="1:7" ht="75" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:7" ht="45" x14ac:dyDescent="0.25">
       <c r="A7" s="15"/>
       <c r="B7" s="4" t="s">
         <v>115</v>
@@ -3030,7 +3036,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="13" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A13" s="15"/>
       <c r="B13" s="4" t="s">
         <v>139</v>
@@ -3062,7 +3068,7 @@
       </c>
       <c r="F14" s="3"/>
     </row>
-    <row r="15" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A15" s="15"/>
       <c r="B15" s="4" t="s">
         <v>141</v>
@@ -3078,7 +3084,7 @@
       </c>
       <c r="F15" s="3"/>
     </row>
-    <row r="16" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A16" s="15" t="s">
         <v>153</v>
       </c>
@@ -3096,7 +3102,7 @@
       </c>
       <c r="F16" s="3"/>
     </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A17" s="15"/>
       <c r="B17" s="4" t="s">
         <v>155</v>
@@ -3180,7 +3186,7 @@
         <v>199</v>
       </c>
     </row>
-    <row r="22" spans="1:6" ht="60" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:6" ht="45" x14ac:dyDescent="0.25">
       <c r="A22" s="15"/>
       <c r="B22" s="4" t="s">
         <v>154</v>
@@ -3216,7 +3222,7 @@
       </c>
       <c r="F23" s="3"/>
     </row>
-    <row r="24" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A24" s="15"/>
       <c r="B24" s="4" t="s">
         <v>171</v>
@@ -3248,7 +3254,7 @@
       </c>
       <c r="F25" s="3"/>
     </row>
-    <row r="26" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A26" s="15"/>
       <c r="B26" s="4" t="s">
         <v>173</v>
@@ -3264,7 +3270,7 @@
       </c>
       <c r="F26" s="3"/>
     </row>
-    <row r="27" spans="1:6" ht="60" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:6" ht="45" x14ac:dyDescent="0.25">
       <c r="A27" s="15"/>
       <c r="B27" s="4" t="s">
         <v>174</v>
@@ -3298,7 +3304,7 @@
         <v>230</v>
       </c>
     </row>
-    <row r="29" spans="1:6" ht="150" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:6" ht="90" x14ac:dyDescent="0.25">
       <c r="A29" s="15"/>
       <c r="B29" s="4" t="s">
         <v>176</v>
@@ -3334,7 +3340,7 @@
       </c>
       <c r="F30" s="3"/>
     </row>
-    <row r="31" spans="1:6" ht="60" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:6" ht="45" x14ac:dyDescent="0.25">
       <c r="A31" s="15"/>
       <c r="B31" s="4" t="s">
         <v>178</v>
@@ -3350,7 +3356,7 @@
       </c>
       <c r="F31" s="3"/>
     </row>
-    <row r="32" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:6" ht="60" x14ac:dyDescent="0.25">
       <c r="A32" s="15"/>
       <c r="B32" s="4" t="s">
         <v>179</v>
@@ -3368,7 +3374,7 @@
         <v>245</v>
       </c>
     </row>
-    <row r="33" spans="1:6" ht="60" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A33" s="15"/>
       <c r="B33" s="4" t="s">
         <v>180</v>
@@ -3384,7 +3390,7 @@
       </c>
       <c r="F33" s="3"/>
     </row>
-    <row r="34" spans="1:6" ht="90" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:6" ht="60" x14ac:dyDescent="0.25">
       <c r="A34" s="15"/>
       <c r="B34" s="4" t="s">
         <v>181</v>
@@ -3400,7 +3406,7 @@
       </c>
       <c r="F34" s="3"/>
     </row>
-    <row r="35" spans="1:6" ht="90" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:6" ht="60" x14ac:dyDescent="0.25">
       <c r="A35" s="15"/>
       <c r="B35" s="4" t="s">
         <v>182</v>
@@ -3468,7 +3474,7 @@
       </c>
       <c r="F38" s="3"/>
     </row>
-    <row r="39" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A39" s="15"/>
       <c r="B39" s="4" t="s">
         <v>188</v>
@@ -3516,7 +3522,7 @@
       </c>
       <c r="F41" s="3"/>
     </row>
-    <row r="42" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A42" s="15"/>
       <c r="B42" s="4" t="s">
         <v>191</v>
@@ -3580,7 +3586,7 @@
       </c>
       <c r="F45" s="3"/>
     </row>
-    <row r="46" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A46" s="15"/>
       <c r="B46" s="4" t="s">
         <v>184</v>
@@ -3710,7 +3716,7 @@
       </c>
       <c r="F53" s="3"/>
     </row>
-    <row r="54" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A54" s="15"/>
       <c r="B54" s="4" t="s">
         <v>258</v>
@@ -3742,7 +3748,7 @@
       </c>
       <c r="F55" s="3"/>
     </row>
-    <row r="56" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A56" s="15"/>
       <c r="B56" s="4" t="s">
         <v>260</v>
@@ -3758,7 +3764,7 @@
       </c>
       <c r="F56" s="3"/>
     </row>
-    <row r="57" spans="1:6" ht="60" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:6" ht="45" x14ac:dyDescent="0.25">
       <c r="A57" s="15"/>
       <c r="B57" s="4" t="s">
         <v>261</v>
@@ -3776,7 +3782,7 @@
         <v>281</v>
       </c>
     </row>
-    <row r="58" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A58" s="15"/>
       <c r="B58" s="4" t="s">
         <v>262</v>
@@ -3792,7 +3798,7 @@
       </c>
       <c r="F58" s="3"/>
     </row>
-    <row r="59" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A59" s="15"/>
       <c r="B59" s="4" t="s">
         <v>263</v>
@@ -3808,7 +3814,7 @@
       </c>
       <c r="F59" s="3"/>
     </row>
-    <row r="60" spans="1:6" ht="60" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:6" ht="45" x14ac:dyDescent="0.25">
       <c r="A60" s="15"/>
       <c r="B60" s="4" t="s">
         <v>264</v>
@@ -3842,7 +3848,7 @@
       </c>
       <c r="F61" s="3"/>
     </row>
-    <row r="62" spans="1:6" ht="105" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:6" ht="75" x14ac:dyDescent="0.25">
       <c r="A62" s="15" t="s">
         <v>290</v>
       </c>
@@ -3862,7 +3868,7 @@
         <v>306</v>
       </c>
     </row>
-    <row r="63" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A63" s="15"/>
       <c r="B63" s="4" t="s">
         <v>292</v>
@@ -3878,7 +3884,7 @@
       </c>
       <c r="F63" s="3"/>
     </row>
-    <row r="64" spans="1:6" ht="75" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:6" ht="60" x14ac:dyDescent="0.25">
       <c r="A64" s="15"/>
       <c r="B64" s="4" t="s">
         <v>293</v>
@@ -3896,7 +3902,7 @@
         <v>312</v>
       </c>
     </row>
-    <row r="65" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A65" s="15" t="s">
         <v>294</v>
       </c>
@@ -3922,7 +3928,7 @@
       <c r="C66" s="4" t="s">
         <v>119</v>
       </c>
-      <c r="D66" s="4" t="s">
+      <c r="D66" s="5" t="s">
         <v>313</v>
       </c>
       <c r="E66" s="3" t="s">
@@ -3932,7 +3938,7 @@
         <v>315</v>
       </c>
     </row>
-    <row r="67" spans="1:7" ht="90" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:7" ht="75" x14ac:dyDescent="0.25">
       <c r="A67" s="15"/>
       <c r="B67" s="4" t="s">
         <v>297</v>
@@ -3948,7 +3954,7 @@
       </c>
       <c r="F67" s="11"/>
     </row>
-    <row r="68" spans="1:7" ht="75" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:7" ht="45" x14ac:dyDescent="0.25">
       <c r="A68" s="15"/>
       <c r="B68" s="4" t="s">
         <v>298</v>
@@ -3980,7 +3986,7 @@
       </c>
       <c r="F69" s="3"/>
     </row>
-    <row r="70" spans="1:7" ht="90" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:7" ht="60" x14ac:dyDescent="0.25">
       <c r="A70" s="15"/>
       <c r="B70" s="4" t="s">
         <v>300</v>
@@ -4012,7 +4018,7 @@
       </c>
       <c r="F71" s="3"/>
     </row>
-    <row r="72" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A72" s="15"/>
       <c r="B72" s="4" t="s">
         <v>302</v>
@@ -4044,7 +4050,7 @@
       </c>
       <c r="F73" s="3"/>
     </row>
-    <row r="74" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A74" s="15" t="s">
         <v>330</v>
       </c>
@@ -4145,7 +4151,7 @@
       <c r="F79" s="13"/>
       <c r="G79" s="14"/>
     </row>
-    <row r="80" spans="1:7" ht="60" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:7" ht="45" x14ac:dyDescent="0.25">
       <c r="A80" s="15"/>
       <c r="B80" s="4" t="s">
         <v>337</v>
@@ -4229,7 +4235,7 @@
       </c>
       <c r="F84" s="3"/>
     </row>
-    <row r="85" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A85" s="15"/>
       <c r="B85" s="4" t="s">
         <v>343</v>
@@ -4277,7 +4283,7 @@
       </c>
       <c r="F87" s="3"/>
     </row>
-    <row r="88" spans="1:6" ht="75" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:6" ht="60" x14ac:dyDescent="0.25">
       <c r="A88" s="15"/>
       <c r="B88" s="4" t="s">
         <v>346</v>
@@ -4311,7 +4317,7 @@
       </c>
       <c r="F89" s="3"/>
     </row>
-    <row r="90" spans="1:6" ht="60" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:6" ht="45" x14ac:dyDescent="0.25">
       <c r="A90" s="15"/>
       <c r="B90" s="4" t="s">
         <v>348</v>
@@ -4327,7 +4333,7 @@
       </c>
       <c r="F90" s="3"/>
     </row>
-    <row r="91" spans="1:6" ht="75" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:6" ht="45" x14ac:dyDescent="0.25">
       <c r="A91" s="15"/>
       <c r="B91" s="4" t="s">
         <v>349</v>
@@ -4359,7 +4365,7 @@
       </c>
       <c r="F92" s="3"/>
     </row>
-    <row r="93" spans="1:6" ht="75" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:6" ht="45" x14ac:dyDescent="0.25">
       <c r="A93" s="15"/>
       <c r="B93" s="4" t="s">
         <v>351</v>
@@ -4375,7 +4381,7 @@
       </c>
       <c r="F93" s="3"/>
     </row>
-    <row r="94" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:6" ht="45" x14ac:dyDescent="0.25">
       <c r="A94" s="15" t="s">
         <v>454</v>
       </c>
@@ -4384,6 +4390,15 @@
       </c>
       <c r="C94" s="4" t="s">
         <v>142</v>
+      </c>
+      <c r="D94" s="5" t="s">
+        <v>533</v>
+      </c>
+      <c r="E94" s="5" t="s">
+        <v>534</v>
+      </c>
+      <c r="F94" s="4" t="s">
+        <v>535</v>
       </c>
     </row>
     <row r="95" spans="1:6" x14ac:dyDescent="0.25">
@@ -4434,7 +4449,7 @@
       <c r="E100" s="3"/>
       <c r="F100" s="3"/>
     </row>
-    <row r="101" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A101" s="5" t="s">
         <v>452</v>
       </c>
@@ -4470,7 +4485,7 @@
       </c>
       <c r="F102" s="3"/>
     </row>
-    <row r="103" spans="1:6" ht="90" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:6" ht="60" x14ac:dyDescent="0.25">
       <c r="A103" s="5" t="s">
         <v>452</v>
       </c>
@@ -4506,7 +4521,7 @@
       </c>
       <c r="F104" s="3"/>
     </row>
-    <row r="105" spans="1:6" ht="60" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:6" ht="45" x14ac:dyDescent="0.25">
       <c r="A105" s="17"/>
       <c r="B105" s="4" t="s">
         <v>357</v>
@@ -4538,7 +4553,7 @@
       </c>
       <c r="F106" s="3"/>
     </row>
-    <row r="107" spans="1:6" ht="105" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:6" ht="75" x14ac:dyDescent="0.25">
       <c r="A107" s="5" t="s">
         <v>452</v>
       </c>
@@ -4556,7 +4571,7 @@
       </c>
       <c r="F107" s="3"/>
     </row>
-    <row r="108" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A108" s="5" t="s">
         <v>450</v>
       </c>
@@ -4590,7 +4605,7 @@
       </c>
       <c r="F109" s="3"/>
     </row>
-    <row r="110" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+    <row r="110" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A110" s="5"/>
       <c r="B110" s="4" t="s">
         <v>362</v>
@@ -4606,7 +4621,7 @@
       </c>
       <c r="F110" s="3"/>
     </row>
-    <row r="111" spans="1:6" ht="60" x14ac:dyDescent="0.25">
+    <row r="111" spans="1:6" ht="45" x14ac:dyDescent="0.25">
       <c r="A111" s="5"/>
       <c r="B111" s="4" t="s">
         <v>363</v>
@@ -4622,7 +4637,7 @@
       </c>
       <c r="F111" s="3"/>
     </row>
-    <row r="112" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+    <row r="112" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A112" s="5" t="s">
         <v>453</v>
       </c>
@@ -4650,7 +4665,7 @@
       <c r="E113" s="3"/>
       <c r="F113" s="3"/>
     </row>
-    <row r="114" spans="1:6" ht="75" x14ac:dyDescent="0.25">
+    <row r="114" spans="1:6" ht="45" x14ac:dyDescent="0.25">
       <c r="A114" s="5" t="s">
         <v>451</v>
       </c>
@@ -4668,7 +4683,7 @@
       </c>
       <c r="F114" s="3"/>
     </row>
-    <row r="115" spans="1:6" ht="120" x14ac:dyDescent="0.25">
+    <row r="115" spans="1:6" ht="75" x14ac:dyDescent="0.25">
       <c r="A115" s="5" t="s">
         <v>406</v>
       </c>
@@ -4686,7 +4701,7 @@
       </c>
       <c r="F115" s="3"/>
     </row>
-    <row r="116" spans="1:6" ht="135" x14ac:dyDescent="0.25">
+    <row r="116" spans="1:6" ht="90" x14ac:dyDescent="0.25">
       <c r="A116" s="5"/>
       <c r="B116" s="4" t="s">
         <v>407</v>
@@ -4702,7 +4717,7 @@
       </c>
       <c r="F116" s="3"/>
     </row>
-    <row r="117" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+    <row r="117" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A117" s="5" t="s">
         <v>450</v>
       </c>
@@ -4720,7 +4735,7 @@
       </c>
       <c r="F117" s="3"/>
     </row>
-    <row r="118" spans="1:6" ht="240" x14ac:dyDescent="0.25">
+    <row r="118" spans="1:6" ht="150" x14ac:dyDescent="0.25">
       <c r="A118" s="5" t="s">
         <v>453</v>
       </c>
@@ -4738,7 +4753,7 @@
       </c>
       <c r="F118" s="3"/>
     </row>
-    <row r="119" spans="1:6" ht="60" x14ac:dyDescent="0.25">
+    <row r="119" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A119" s="5"/>
       <c r="B119" s="4" t="s">
         <v>410</v>
@@ -4747,14 +4762,14 @@
         <v>119</v>
       </c>
       <c r="D119" s="3" t="s">
+        <v>477</v>
+      </c>
+      <c r="E119" s="3" t="s">
         <v>478</v>
       </c>
-      <c r="E119" s="3" t="s">
-        <v>479</v>
-      </c>
       <c r="F119" s="3"/>
     </row>
-    <row r="120" spans="1:6" ht="90" x14ac:dyDescent="0.25">
+    <row r="120" spans="1:6" ht="60" x14ac:dyDescent="0.25">
       <c r="A120" s="5"/>
       <c r="B120" s="4" t="s">
         <v>411</v>
@@ -4766,11 +4781,11 @@
         <v>45</v>
       </c>
       <c r="E120" s="3" t="s">
-        <v>480</v>
+        <v>479</v>
       </c>
       <c r="F120" s="3"/>
     </row>
-    <row r="121" spans="1:6" ht="120" x14ac:dyDescent="0.25">
+    <row r="121" spans="1:6" ht="75" x14ac:dyDescent="0.25">
       <c r="A121" s="5"/>
       <c r="B121" s="4" t="s">
         <v>412</v>
@@ -4779,14 +4794,14 @@
         <v>142</v>
       </c>
       <c r="D121" s="3" t="s">
+        <v>480</v>
+      </c>
+      <c r="E121" s="3" t="s">
         <v>481</v>
       </c>
-      <c r="E121" s="3" t="s">
-        <v>482</v>
-      </c>
       <c r="F121" s="3"/>
     </row>
-    <row r="122" spans="1:6" ht="90" x14ac:dyDescent="0.25">
+    <row r="122" spans="1:6" ht="60" x14ac:dyDescent="0.25">
       <c r="A122" s="5"/>
       <c r="B122" s="4" t="s">
         <v>413</v>
@@ -4795,13 +4810,13 @@
         <v>119</v>
       </c>
       <c r="D122" s="3" t="s">
+        <v>482</v>
+      </c>
+      <c r="E122" s="3" t="s">
         <v>483</v>
       </c>
-      <c r="E122" s="3" t="s">
+      <c r="F122" s="3" t="s">
         <v>484</v>
-      </c>
-      <c r="F122" s="3" t="s">
-        <v>485</v>
       </c>
     </row>
     <row r="123" spans="1:6" ht="90" x14ac:dyDescent="0.25">
@@ -4813,10 +4828,10 @@
         <v>142</v>
       </c>
       <c r="D123" s="3" t="s">
+        <v>529</v>
+      </c>
+      <c r="E123" s="3" t="s">
         <v>530</v>
-      </c>
-      <c r="E123" s="3" t="s">
-        <v>531</v>
       </c>
       <c r="F123" s="3"/>
     </row>
@@ -4829,35 +4844,28 @@
         <v>142</v>
       </c>
       <c r="D124" s="3" t="s">
+        <v>531</v>
+      </c>
+      <c r="E124" s="3" t="s">
         <v>532</v>
       </c>
-      <c r="E124" s="3" t="s">
-        <v>533</v>
-      </c>
       <c r="F124" s="3"/>
     </row>
-    <row r="125" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="125" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A125" s="15" t="s">
         <v>461</v>
       </c>
-      <c r="B125" s="15" t="s">
-        <v>461</v>
-      </c>
-      <c r="C125" s="15"/>
-      <c r="D125" s="15" t="s">
-        <v>461</v>
-      </c>
-      <c r="E125" s="15" t="s">
-        <v>461</v>
-      </c>
-      <c r="F125" s="15" t="s">
-        <v>461</v>
-      </c>
+      <c r="B125" s="4" t="s">
+        <v>462</v>
+      </c>
+      <c r="C125" s="4" t="s">
+        <v>119</v>
+      </c>
+      <c r="D125" s="3"/>
+      <c r="E125" s="3"/>
+      <c r="F125" s="3"/>
     </row>
     <row r="126" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A126" s="15" t="s">
-        <v>462</v>
-      </c>
       <c r="B126" s="4" t="s">
         <v>463</v>
       </c>
@@ -4935,8 +4943,11 @@
       <c r="F132" s="3"/>
     </row>
     <row r="133" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A133" s="15" t="s">
+        <v>470</v>
+      </c>
       <c r="B133" s="4" t="s">
-        <v>470</v>
+        <v>471</v>
       </c>
       <c r="C133" s="4" t="s">
         <v>119</v>
@@ -4946,9 +4957,6 @@
       <c r="F133" s="3"/>
     </row>
     <row r="134" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A134" s="15" t="s">
-        <v>471</v>
-      </c>
       <c r="B134" s="4" t="s">
         <v>472</v>
       </c>
@@ -4975,7 +4983,7 @@
         <v>474</v>
       </c>
       <c r="C136" s="4" t="s">
-        <v>119</v>
+        <v>112</v>
       </c>
       <c r="D136" s="3"/>
       <c r="E136" s="3"/>
@@ -4986,7 +4994,7 @@
         <v>475</v>
       </c>
       <c r="C137" s="4" t="s">
-        <v>112</v>
+        <v>119</v>
       </c>
       <c r="D137" s="3"/>
       <c r="E137" s="3"/>
@@ -4997,19 +5005,13 @@
         <v>476</v>
       </c>
       <c r="C138" s="4" t="s">
-        <v>119</v>
+        <v>142</v>
       </c>
       <c r="D138" s="3"/>
       <c r="E138" s="3"/>
       <c r="F138" s="3"/>
     </row>
     <row r="139" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B139" s="4" t="s">
-        <v>477</v>
-      </c>
-      <c r="C139" s="4" t="s">
-        <v>142</v>
-      </c>
       <c r="D139" s="3"/>
       <c r="E139" s="3"/>
       <c r="F139" s="3"/>
@@ -9158,18 +9160,13 @@
       <c r="D968" s="3"/>
       <c r="E968" s="3"/>
       <c r="F968" s="3"/>
-    </row>
-    <row r="969" spans="4:6" x14ac:dyDescent="0.25">
-      <c r="D969" s="3"/>
-      <c r="E969" s="3"/>
-      <c r="F969" s="3"/>
     </row>
   </sheetData>
   <mergeCells count="1">
     <mergeCell ref="A1:F1"/>
   </mergeCells>
   <phoneticPr fontId="3" type="noConversion"/>
-  <conditionalFormatting sqref="C1:C124 C126:C1048576">
+  <conditionalFormatting sqref="C1:C1048576">
     <cfRule type="containsText" dxfId="8" priority="1" operator="containsText" text="Hard">
       <formula>NOT(ISERROR(SEARCH("Hard",C1)))</formula>
     </cfRule>
@@ -9206,7 +9203,7 @@
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" s="27" t="s">
-        <v>486</v>
+        <v>485</v>
       </c>
       <c r="B1" s="28"/>
       <c r="C1" s="29"/>
@@ -9240,69 +9237,69 @@
     </row>
     <row r="3" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A3" s="20" t="s">
+        <v>486</v>
+      </c>
+      <c r="B3" s="24" t="s">
         <v>487</v>
       </c>
-      <c r="B3" s="24" t="s">
-        <v>488</v>
-      </c>
       <c r="C3" t="s">
         <v>119</v>
       </c>
       <c r="D3" s="17" t="s">
+        <v>496</v>
+      </c>
+      <c r="E3" s="17" t="s">
         <v>497</v>
-      </c>
-      <c r="E3" s="17" t="s">
-        <v>498</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B4" s="24" t="s">
-        <v>489</v>
+        <v>488</v>
       </c>
       <c r="C4" t="s">
         <v>119</v>
       </c>
       <c r="D4" s="17" t="s">
+        <v>498</v>
+      </c>
+      <c r="E4" s="17" t="s">
         <v>499</v>
-      </c>
-      <c r="E4" s="17" t="s">
-        <v>500</v>
       </c>
     </row>
     <row r="5" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="B5" s="24" t="s">
-        <v>490</v>
+        <v>489</v>
       </c>
       <c r="C5" t="s">
         <v>119</v>
       </c>
       <c r="D5" s="17" t="s">
+        <v>501</v>
+      </c>
+      <c r="E5" s="17" t="s">
         <v>502</v>
       </c>
-      <c r="E5" s="17" t="s">
-        <v>503</v>
-      </c>
       <c r="F5" s="17" t="s">
-        <v>501</v>
+        <v>500</v>
       </c>
     </row>
     <row r="6" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="B6" s="24" t="s">
-        <v>491</v>
+        <v>490</v>
       </c>
       <c r="C6" t="s">
         <v>119</v>
       </c>
       <c r="D6" s="17" t="s">
+        <v>503</v>
+      </c>
+      <c r="E6" s="17" t="s">
         <v>504</v>
-      </c>
-      <c r="E6" s="17" t="s">
-        <v>505</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B7" s="22" t="s">
-        <v>492</v>
+        <v>491</v>
       </c>
       <c r="C7" s="22" t="s">
         <v>112</v>
@@ -9311,7 +9308,7 @@
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B8" s="22" t="s">
-        <v>493</v>
+        <v>492</v>
       </c>
       <c r="C8" s="22" t="s">
         <v>112</v>
@@ -9320,7 +9317,7 @@
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B9" s="22" t="s">
-        <v>494</v>
+        <v>493</v>
       </c>
       <c r="C9" s="22" t="s">
         <v>119</v>
@@ -9329,7 +9326,7 @@
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B10" s="22" t="s">
-        <v>495</v>
+        <v>494</v>
       </c>
       <c r="C10" s="22" t="s">
         <v>112</v>
@@ -9338,117 +9335,117 @@
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B11" s="24" t="s">
-        <v>496</v>
+        <v>495</v>
       </c>
       <c r="C11" t="s">
         <v>142</v>
       </c>
       <c r="D11" s="17" t="s">
+        <v>513</v>
+      </c>
+      <c r="E11" s="17" t="s">
         <v>514</v>
-      </c>
-      <c r="E11" s="17" t="s">
-        <v>515</v>
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A12" s="20" t="s">
+        <v>505</v>
+      </c>
+      <c r="B12" s="24" t="s">
         <v>506</v>
       </c>
-      <c r="B12" s="24" t="s">
-        <v>507</v>
-      </c>
       <c r="C12" s="22" t="s">
         <v>119</v>
       </c>
       <c r="D12" s="17" t="s">
+        <v>517</v>
+      </c>
+      <c r="E12" s="17" t="s">
         <v>518</v>
-      </c>
-      <c r="E12" s="17" t="s">
-        <v>519</v>
       </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B13" s="24" t="s">
-        <v>508</v>
+        <v>507</v>
       </c>
       <c r="C13" s="22" t="s">
         <v>119</v>
       </c>
       <c r="D13" s="17" t="s">
-        <v>517</v>
+        <v>516</v>
       </c>
       <c r="E13" s="17" t="s">
-        <v>520</v>
+        <v>519</v>
       </c>
     </row>
     <row r="14" spans="1:7" ht="45" x14ac:dyDescent="0.25">
       <c r="B14" s="24" t="s">
-        <v>509</v>
+        <v>508</v>
       </c>
       <c r="C14" s="22" t="s">
         <v>119</v>
       </c>
       <c r="D14" s="17" t="s">
-        <v>516</v>
+        <v>515</v>
       </c>
       <c r="E14" s="17" t="s">
-        <v>521</v>
+        <v>520</v>
       </c>
     </row>
     <row r="15" spans="1:7" ht="45" x14ac:dyDescent="0.25">
       <c r="B15" s="24" t="s">
-        <v>510</v>
+        <v>509</v>
       </c>
       <c r="C15" s="22" t="s">
         <v>119</v>
       </c>
       <c r="D15" s="17" t="s">
+        <v>521</v>
+      </c>
+      <c r="E15" s="17" t="s">
         <v>522</v>
-      </c>
-      <c r="E15" s="17" t="s">
-        <v>523</v>
       </c>
     </row>
     <row r="16" spans="1:7" ht="90" x14ac:dyDescent="0.25">
       <c r="B16" s="24" t="s">
-        <v>511</v>
+        <v>510</v>
       </c>
       <c r="C16" s="22" t="s">
         <v>119</v>
       </c>
       <c r="D16" s="17" t="s">
+        <v>523</v>
+      </c>
+      <c r="E16" s="17" t="s">
         <v>524</v>
-      </c>
-      <c r="E16" s="17" t="s">
-        <v>525</v>
       </c>
     </row>
     <row r="17" spans="2:5" ht="60" x14ac:dyDescent="0.25">
       <c r="B17" s="24" t="s">
-        <v>512</v>
+        <v>511</v>
       </c>
       <c r="C17" s="22" t="s">
         <v>119</v>
       </c>
       <c r="D17" s="17" t="s">
+        <v>525</v>
+      </c>
+      <c r="E17" s="17" t="s">
         <v>526</v>
-      </c>
-      <c r="E17" s="17" t="s">
-        <v>527</v>
       </c>
     </row>
     <row r="18" spans="2:5" ht="30" x14ac:dyDescent="0.25">
       <c r="B18" s="24" t="s">
-        <v>513</v>
+        <v>512</v>
       </c>
       <c r="C18" s="22" t="s">
         <v>119</v>
       </c>
       <c r="D18" s="17" t="s">
+        <v>527</v>
+      </c>
+      <c r="E18" s="17" t="s">
         <v>528</v>
-      </c>
-      <c r="E18" s="17" t="s">
-        <v>529</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Finished minimum cost to connect all points
</commit_message>
<xml_diff>
--- a/LeetCode.xlsx
+++ b/LeetCode.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\EricS\Documents\VSCode Projects\LeetcodeGrind\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D8173D4F-337C-4485-B14D-32D64396B6FA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F2F804E9-0825-4E1F-8FD3-0D803ED4634E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="3" xr2:uid="{02D29AA1-7085-42F6-B3D4-4C0365DA5453}"/>
   </bookViews>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="765" uniqueCount="536">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="767" uniqueCount="538">
   <si>
     <t>Roman to Integer:</t>
   </si>
@@ -1651,6 +1651,12 @@
   </si>
   <si>
     <t>DFS/backtracking works but too slow</t>
+  </si>
+  <si>
+    <t>Min cost necessary to connect every point in a graph given list of point coordinates using Manhattan distance</t>
+  </si>
+  <si>
+    <t>Prim's algorithm, keep track of visited nodes and keep adding the shortest path from the connected group until everything is covered, use indices instead of x, y to make it easier to track nodes, can be done with a single vector if you are smart about how updating is done</t>
   </si>
 </sst>
 </file>
@@ -2815,7 +2821,7 @@
   <dimension ref="A1:G968"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A88" zoomScale="81" zoomScaleNormal="122" workbookViewId="0">
-      <selection activeCell="F95" sqref="F95"/>
+      <selection activeCell="D96" sqref="D96"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4401,12 +4407,18 @@
         <v>535</v>
       </c>
     </row>
-    <row r="95" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:6" ht="45" x14ac:dyDescent="0.25">
       <c r="B95" s="4" t="s">
         <v>456</v>
       </c>
       <c r="C95" s="4" t="s">
         <v>119</v>
+      </c>
+      <c r="D95" s="5" t="s">
+        <v>536</v>
+      </c>
+      <c r="E95" s="5" t="s">
+        <v>537</v>
       </c>
     </row>
     <row r="96" spans="1:6" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Finished network delay problem
</commit_message>
<xml_diff>
--- a/LeetCode.xlsx
+++ b/LeetCode.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\EricS\Documents\VSCode Projects\LeetcodeGrind\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F2F804E9-0825-4E1F-8FD3-0D803ED4634E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{49AD8A40-B35A-472D-B267-C0EAB3318CF7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="3" xr2:uid="{02D29AA1-7085-42F6-B3D4-4C0365DA5453}"/>
   </bookViews>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="767" uniqueCount="538">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="769" uniqueCount="540">
   <si>
     <t>Roman to Integer:</t>
   </si>
@@ -1657,6 +1657,12 @@
   </si>
   <si>
     <t>Prim's algorithm, keep track of visited nodes and keep adding the shortest path from the connected group until everything is covered, use indices instead of x, y to make it easier to track nodes, can be done with a single vector if you are smart about how updating is done</t>
+  </si>
+  <si>
+    <t>Given a start node and a list of directed edges as well as weights telling you delay for that edge, find the maximum time for signal to get from start to all other nodes</t>
+  </si>
+  <si>
+    <t>Dijkstra's algorithm basically, just create graph representation using vector of vector of pairs (pairs tracking dest and weight), then you start at k and make priority queue, checking over and over, make sure when adding to priority queue you do current time + extra delay to account for past delays as well.</t>
   </si>
 </sst>
 </file>
@@ -2821,7 +2827,7 @@
   <dimension ref="A1:G968"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A88" zoomScale="81" zoomScaleNormal="122" workbookViewId="0">
-      <selection activeCell="D96" sqref="D96"/>
+      <selection activeCell="D97" sqref="D97"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4421,12 +4427,18 @@
         <v>537</v>
       </c>
     </row>
-    <row r="96" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:6" ht="45" x14ac:dyDescent="0.25">
       <c r="B96" s="4" t="s">
         <v>457</v>
       </c>
       <c r="C96" s="4" t="s">
         <v>119</v>
+      </c>
+      <c r="D96" s="5" t="s">
+        <v>538</v>
+      </c>
+      <c r="E96" s="5" t="s">
+        <v>539</v>
       </c>
     </row>
     <row r="97" spans="1:6" ht="75.75" customHeight="1" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Finished rising water problem
</commit_message>
<xml_diff>
--- a/LeetCode.xlsx
+++ b/LeetCode.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\EricS\Documents\VSCode Projects\LeetcodeGrind\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{49AD8A40-B35A-472D-B267-C0EAB3318CF7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{88D7E842-10F1-4678-BA27-663A02D49E81}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="3" xr2:uid="{02D29AA1-7085-42F6-B3D4-4C0365DA5453}"/>
   </bookViews>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="769" uniqueCount="540">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="773" uniqueCount="544">
   <si>
     <t>Roman to Integer:</t>
   </si>
@@ -1663,6 +1663,18 @@
   </si>
   <si>
     <t>Dijkstra's algorithm basically, just create graph representation using vector of vector of pairs (pairs tracking dest and weight), then you start at k and make priority queue, checking over and over, make sure when adding to priority queue you do current time + extra delay to account for past delays as well.</t>
+  </si>
+  <si>
+    <t>also can do binary search dfs solution</t>
+  </si>
+  <si>
+    <t>each tick, rain water adds a level of water, making water everywhere at t height. Determine minimum number of ticks you need to wait for you to go from (0, 0) to bottom right, able to go horizontally or vertically.</t>
+  </si>
+  <si>
+    <t>One method is to use priority queue to keep track of all possible neighbors and keep traversing cheapest until you get to the end. Also make sure to track visited and then just do floodfill as normal.</t>
+  </si>
+  <si>
+    <t>Given array of words sorted by new lexicographical ordering, return the letters in the words in the new alien lexicographical order</t>
   </si>
 </sst>
 </file>
@@ -2827,7 +2839,7 @@
   <dimension ref="A1:G968"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A88" zoomScale="81" zoomScaleNormal="122" workbookViewId="0">
-      <selection activeCell="D97" sqref="D97"/>
+      <selection activeCell="E98" sqref="E98"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4441,20 +4453,32 @@
         <v>539</v>
       </c>
     </row>
-    <row r="97" spans="1:6" ht="75.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:6" ht="60" x14ac:dyDescent="0.25">
       <c r="B97" s="4" t="s">
         <v>458</v>
       </c>
       <c r="C97" s="4" t="s">
         <v>142</v>
       </c>
-    </row>
-    <row r="98" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="D97" s="5" t="s">
+        <v>541</v>
+      </c>
+      <c r="E97" s="5" t="s">
+        <v>542</v>
+      </c>
+      <c r="F97" s="4" t="s">
+        <v>540</v>
+      </c>
+    </row>
+    <row r="98" spans="1:6" ht="45" x14ac:dyDescent="0.25">
       <c r="B98" s="4" t="s">
         <v>459</v>
       </c>
       <c r="C98" s="4" t="s">
         <v>142</v>
+      </c>
+      <c r="D98" s="5" t="s">
+        <v>543</v>
       </c>
     </row>
     <row r="99" spans="1:6" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Finished cheapest flight k stops
</commit_message>
<xml_diff>
--- a/LeetCode.xlsx
+++ b/LeetCode.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\EricS\Documents\VSCode Projects\LeetcodeGrind\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{88D7E842-10F1-4678-BA27-663A02D49E81}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CAD247AD-C94E-4C4B-A93C-277A7B6E109B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="3" xr2:uid="{02D29AA1-7085-42F6-B3D4-4C0365DA5453}"/>
   </bookViews>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="773" uniqueCount="544">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="775" uniqueCount="546">
   <si>
     <t>Roman to Integer:</t>
   </si>
@@ -1675,6 +1675,12 @@
   </si>
   <si>
     <t>Given array of words sorted by new lexicographical ordering, return the letters in the words in the new alien lexicographical order</t>
+  </si>
+  <si>
+    <t>cheapest path of flights assuming maximum of k stops</t>
+  </si>
+  <si>
+    <t>dijkstra's algorithm basically, just create graph representation using vector of vector of pairs or special tuple tracking price, node, and number of stops (taken or remaining). Then, you put stuff into priority queue by price and do smart pruning, skipping if u reach k stops or if value is larger than previous for that node with that number of stops used thus far (dp-like table to track min price for each node at certain step)</t>
   </si>
 </sst>
 </file>
@@ -4481,12 +4487,18 @@
         <v>543</v>
       </c>
     </row>
-    <row r="99" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:6" ht="60" x14ac:dyDescent="0.25">
       <c r="B99" s="4" t="s">
         <v>460</v>
       </c>
       <c r="C99" s="4" t="s">
         <v>119</v>
+      </c>
+      <c r="D99" s="5" t="s">
+        <v>544</v>
+      </c>
+      <c r="E99" s="5" t="s">
+        <v>545</v>
       </c>
     </row>
     <row r="100" spans="1:6" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Finally finished alien dictionary and adv graphs
</commit_message>
<xml_diff>
--- a/LeetCode.xlsx
+++ b/LeetCode.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\EricS\Documents\VSCode Projects\LeetcodeGrind\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CAD247AD-C94E-4C4B-A93C-277A7B6E109B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E0259356-2043-4E86-BFA5-83F99A18A795}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="3" xr2:uid="{02D29AA1-7085-42F6-B3D4-4C0365DA5453}"/>
   </bookViews>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="775" uniqueCount="546">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="776" uniqueCount="547">
   <si>
     <t>Roman to Integer:</t>
   </si>
@@ -1681,6 +1681,9 @@
   </si>
   <si>
     <t>dijkstra's algorithm basically, just create graph representation using vector of vector of pairs or special tuple tracking price, node, and number of stops (taken or remaining). Then, you put stuff into priority queue by price and do smart pruning, skipping if u reach k stops or if value is larger than previous for that node with that number of stops used thus far (dp-like table to track min price for each node at certain step)</t>
+  </si>
+  <si>
+    <t>loop through consecutive words and find where they are distinct, adding the key letter pair as an edge to keep track of which letters should come after which. Then you do topological ordering of the graph, making sure to return "" if there is a loop and that every character is covered in case there are multiple cases (not fully connected graph)</t>
   </si>
 </sst>
 </file>
@@ -2844,7 +2847,7 @@
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:G968"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A88" zoomScale="81" zoomScaleNormal="122" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A87" zoomScale="81" zoomScaleNormal="122" workbookViewId="0">
       <selection activeCell="E98" sqref="E98"/>
     </sheetView>
   </sheetViews>
@@ -4485,6 +4488,9 @@
       </c>
       <c r="D98" s="5" t="s">
         <v>543</v>
+      </c>
+      <c r="E98" s="5" t="s">
+        <v>546</v>
       </c>
     </row>
     <row r="99" spans="1:6" ht="60" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Finished jump game 2
</commit_message>
<xml_diff>
--- a/LeetCode.xlsx
+++ b/LeetCode.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\EricS\Documents\VSCode Projects\LeetcodeGrind\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0D680807-6118-464A-8C0F-89C19C27F8A4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A9B95985-8238-4318-B78F-8172599F7B45}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="3" xr2:uid="{02D29AA1-7085-42F6-B3D4-4C0365DA5453}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="3" xr2:uid="{02D29AA1-7085-42F6-B3D4-4C0365DA5453}"/>
   </bookViews>
   <sheets>
     <sheet name="Easy" sheetId="1" r:id="rId1"/>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="781" uniqueCount="552">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1354" uniqueCount="553">
   <si>
     <t>Roman to Integer:</t>
   </si>
@@ -1700,6 +1700,9 @@
   </si>
   <si>
     <t>Same thing but return minimum number of jumps necessary given it's always possible</t>
+  </si>
+  <si>
+    <t>Basically, you track the furthest you can go in each jump and iterate until the end. First jump, l = r = 0, second jump, l = r + 1, r = furthest of jumps between l and r. Then you loop and continue</t>
   </si>
 </sst>
 </file>
@@ -2864,7 +2867,7 @@
   <dimension ref="A1:G968"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A121" zoomScale="81" zoomScaleNormal="122" workbookViewId="0">
-      <selection activeCell="E127" sqref="E127"/>
+      <selection activeCell="E128" sqref="E128"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4976,7 +4979,9 @@
       <c r="D127" s="3" t="s">
         <v>551</v>
       </c>
-      <c r="E127" s="3"/>
+      <c r="E127" s="3" t="s">
+        <v>552</v>
+      </c>
       <c r="F127" s="3"/>
     </row>
     <row r="128" spans="1:6" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Finished gas station problem
</commit_message>
<xml_diff>
--- a/LeetCode.xlsx
+++ b/LeetCode.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\EricS\Documents\VSCode Projects\LeetcodeGrind\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A9B95985-8238-4318-B78F-8172599F7B45}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{91F17508-4B1D-4E6B-9749-099AEC164BF2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="3" xr2:uid="{02D29AA1-7085-42F6-B3D4-4C0365DA5453}"/>
   </bookViews>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1354" uniqueCount="553">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="785" uniqueCount="556">
   <si>
     <t>Roman to Integer:</t>
   </si>
@@ -1703,6 +1703,15 @@
   </si>
   <si>
     <t>Basically, you track the furthest you can go in each jump and iterate until the end. First jump, l = r = 0, second jump, l = r + 1, r = furthest of jumps between l and r. Then you loop and continue</t>
+  </si>
+  <si>
+    <t>Given 2 arrays, one of max amount of gas you can get at each station and the other the cost to get out of the station to the next one, return unique starting index that allows you to cycle through the stations, -1 if impossible</t>
+  </si>
+  <si>
+    <t>You can loop through 2 * n, tracking current index and current amount of gas remaining, if i != start and i % n == start then we finish and return. If curr is ever below current cost, then we set start to i + 1 and curr to gas[tank % n], otherwise we increment by gas[i+1 % n] and decrement by cost[i % n]. Increment i. Return -1 at the end since we didn't return earlier.</t>
+  </si>
+  <si>
+    <t>We can also abuse the fact we know there's a unique solution, checking that solution is possible and then we only need to cycle once</t>
   </si>
 </sst>
 </file>
@@ -2867,7 +2876,7 @@
   <dimension ref="A1:G968"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A121" zoomScale="81" zoomScaleNormal="122" workbookViewId="0">
-      <selection activeCell="E128" sqref="E128"/>
+      <selection activeCell="D129" sqref="D129"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4984,16 +4993,22 @@
       </c>
       <c r="F127" s="3"/>
     </row>
-    <row r="128" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="128" spans="1:6" ht="60" x14ac:dyDescent="0.25">
       <c r="B128" s="4" t="s">
         <v>465</v>
       </c>
       <c r="C128" s="4" t="s">
         <v>119</v>
       </c>
-      <c r="D128" s="3"/>
-      <c r="E128" s="3"/>
-      <c r="F128" s="3"/>
+      <c r="D128" s="3" t="s">
+        <v>553</v>
+      </c>
+      <c r="E128" s="3" t="s">
+        <v>554</v>
+      </c>
+      <c r="F128" s="3" t="s">
+        <v>555</v>
+      </c>
     </row>
     <row r="129" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B129" s="4" t="s">

</xml_diff>

<commit_message>
Finished hand of straights
</commit_message>
<xml_diff>
--- a/LeetCode.xlsx
+++ b/LeetCode.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\EricS\Documents\VSCode Projects\LeetcodeGrind\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{91F17508-4B1D-4E6B-9749-099AEC164BF2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6FDB161C-B1F9-4735-A2C4-158976A0567F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="3" xr2:uid="{02D29AA1-7085-42F6-B3D4-4C0365DA5453}"/>
   </bookViews>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="785" uniqueCount="556">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="787" uniqueCount="558">
   <si>
     <t>Roman to Integer:</t>
   </si>
@@ -1712,6 +1712,12 @@
   </si>
   <si>
     <t>We can also abuse the fact we know there's a unique solution, checking that solution is possible and then we only need to cycle once</t>
+  </si>
+  <si>
+    <t>Given list of cards and group size, determine if the cards can be made into groups of straights of size group size</t>
+  </si>
+  <si>
+    <t>Basically sort the cards and keep cycling to make sure the rest of the straight always exists, best way to do it in cpp is to use queue and track the index in the straight it is, pushing the next index as necessary and tracking how many were finished. Easier way is to use a map and keep taking smallest key (auto sorted) and having nested loops decrementing counts and deleting keys as necessary.</t>
   </si>
 </sst>
 </file>
@@ -2875,8 +2881,8 @@
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:G968"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A121" zoomScale="81" zoomScaleNormal="122" workbookViewId="0">
-      <selection activeCell="D129" sqref="D129"/>
+    <sheetView tabSelected="1" topLeftCell="A123" zoomScale="81" zoomScaleNormal="122" workbookViewId="0">
+      <selection activeCell="E130" sqref="E130"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5010,15 +5016,19 @@
         <v>555</v>
       </c>
     </row>
-    <row r="129" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="129" spans="1:6" ht="60" x14ac:dyDescent="0.25">
       <c r="B129" s="4" t="s">
         <v>466</v>
       </c>
       <c r="C129" s="4" t="s">
         <v>119</v>
       </c>
-      <c r="D129" s="3"/>
-      <c r="E129" s="3"/>
+      <c r="D129" s="3" t="s">
+        <v>556</v>
+      </c>
+      <c r="E129" s="3" t="s">
+        <v>557</v>
+      </c>
       <c r="F129" s="3"/>
     </row>
     <row r="130" spans="1:6" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Finished valid parens string and all greedy
</commit_message>
<xml_diff>
--- a/LeetCode.xlsx
+++ b/LeetCode.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\EricS\Documents\VSCode Projects\LeetcodeGrind\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D48738FC-D1B4-49A8-9754-F8873AB15368}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{55ADFA7E-2B54-4676-B7D6-38319D74815E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="3" xr2:uid="{02D29AA1-7085-42F6-B3D4-4C0365DA5453}"/>
   </bookViews>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="791" uniqueCount="562">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="793" uniqueCount="564">
   <si>
     <t>Roman to Integer:</t>
   </si>
@@ -1730,6 +1730,12 @@
   </si>
   <si>
     <t>Track where the last occurrence of each letter is using array, loop through each index in string, keep track of maxLast which is the largest last index of the current substring thus far, if maxLast becomes less than current index i, push size to ret and reset size to 0. Update maxLast with current character and increment size. Remember to push one more time at end and return</t>
+  </si>
+  <si>
+    <t>Check if parenthesis string is valid with '(', ')', and '*' wildcard that can be left, right, or empty string</t>
+  </si>
+  <si>
+    <t>Loop through each character and track lmin, lmax for minimum number of left brackets unmatched and max number of unmatched left brackets. Increment both when '(', decrement both when ')', increment lmax decrement lmin when wildcard. If lmax is ever negative, return False since that means not possible to match all ')'. Force lmin to always be non-negative, return if lmin is equal to 0 at end, since that would mean no unmatched parens</t>
   </si>
 </sst>
 </file>
@@ -2894,7 +2900,7 @@
   <dimension ref="A1:G968"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A124" zoomScale="81" zoomScaleNormal="122" workbookViewId="0">
-      <selection activeCell="D132" sqref="D132"/>
+      <selection activeCell="E133" sqref="E133"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5073,15 +5079,19 @@
       </c>
       <c r="F131" s="3"/>
     </row>
-    <row r="132" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="132" spans="1:6" ht="60" x14ac:dyDescent="0.25">
       <c r="B132" s="4" t="s">
         <v>469</v>
       </c>
       <c r="C132" s="4" t="s">
         <v>119</v>
       </c>
-      <c r="D132" s="3"/>
-      <c r="E132" s="3"/>
+      <c r="D132" s="3" t="s">
+        <v>562</v>
+      </c>
+      <c r="E132" s="3" t="s">
+        <v>563</v>
+      </c>
       <c r="F132" s="3"/>
     </row>
     <row r="133" spans="1:6" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Finished non overlapping intervals
</commit_message>
<xml_diff>
--- a/LeetCode.xlsx
+++ b/LeetCode.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\EricS\Documents\VSCode Projects\LeetcodeGrind\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F04DD66F-D35D-4159-8D83-272AFEA0AD97}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E1866909-2507-4FFD-A00E-72897EA710E8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="3" xr2:uid="{02D29AA1-7085-42F6-B3D4-4C0365DA5453}"/>
   </bookViews>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="799" uniqueCount="570">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="802" uniqueCount="573">
   <si>
     <t>Roman to Integer:</t>
   </si>
@@ -1754,6 +1754,15 @@
   </si>
   <si>
     <t>Sort by start and loop through checking each and the one before it, determining if there is overlap</t>
+  </si>
+  <si>
+    <t>Count number of intervals need to remove to make non-overlapping</t>
+  </si>
+  <si>
+    <t>Sort by start and loop through, increasing ret every time there's overlap but instead of tracking furthest right, we take the minimum right bound since it's always more optimal to remove the interval that extends further.</t>
+  </si>
+  <si>
+    <t>Could also count non-overlapping and subtract from total n</t>
   </si>
 </sst>
 </file>
@@ -2917,7 +2926,7 @@
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:G968"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A127" zoomScale="81" zoomScaleNormal="122" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="B130" zoomScale="81" zoomScaleNormal="122" workbookViewId="0">
       <selection activeCell="D137" sqref="D137"/>
     </sheetView>
   </sheetViews>
@@ -5145,16 +5154,22 @@
       </c>
       <c r="F134" s="3"/>
     </row>
-    <row r="135" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="135" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="B135" s="4" t="s">
         <v>473</v>
       </c>
       <c r="C135" s="4" t="s">
         <v>119</v>
       </c>
-      <c r="D135" s="3"/>
-      <c r="E135" s="3"/>
-      <c r="F135" s="3"/>
+      <c r="D135" s="3" t="s">
+        <v>570</v>
+      </c>
+      <c r="E135" s="3" t="s">
+        <v>571</v>
+      </c>
+      <c r="F135" s="3" t="s">
+        <v>572</v>
+      </c>
     </row>
     <row r="136" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="B136" s="4" t="s">

</xml_diff>

<commit_message>
Finished meeting rooms 2
</commit_message>
<xml_diff>
--- a/LeetCode.xlsx
+++ b/LeetCode.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\EricS\Documents\VSCode Projects\LeetcodeGrind\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E1866909-2507-4FFD-A00E-72897EA710E8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2A394582-75A4-4E12-9D93-EF77742322EA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="3" xr2:uid="{02D29AA1-7085-42F6-B3D4-4C0365DA5453}"/>
   </bookViews>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="802" uniqueCount="573">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="804" uniqueCount="575">
   <si>
     <t>Roman to Integer:</t>
   </si>
@@ -1763,6 +1763,12 @@
   </si>
   <si>
     <t>Could also count non-overlapping and subtract from total n</t>
+  </si>
+  <si>
+    <t>Determine number of rooms needed to hold all meetings without any overlaps</t>
+  </si>
+  <si>
+    <t>Combine start and end and sort, tracking the current number of ongoing meetings and updating ret as needed going through them chronologically</t>
   </si>
 </sst>
 </file>
@@ -2926,8 +2932,8 @@
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:G968"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B130" zoomScale="81" zoomScaleNormal="122" workbookViewId="0">
-      <selection activeCell="D137" sqref="D137"/>
+    <sheetView tabSelected="1" topLeftCell="A130" zoomScale="81" zoomScaleNormal="122" workbookViewId="0">
+      <selection activeCell="D138" sqref="D138"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5186,15 +5192,19 @@
       </c>
       <c r="F136" s="3"/>
     </row>
-    <row r="137" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="137" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="B137" s="4" t="s">
         <v>475</v>
       </c>
       <c r="C137" s="4" t="s">
         <v>119</v>
       </c>
-      <c r="D137" s="3"/>
-      <c r="E137" s="3"/>
+      <c r="D137" s="3" t="s">
+        <v>573</v>
+      </c>
+      <c r="E137" s="3" t="s">
+        <v>574</v>
+      </c>
       <c r="F137" s="3"/>
     </row>
     <row r="138" spans="1:6" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Finished intervals, started moving stuff to MathGeom
</commit_message>
<xml_diff>
--- a/LeetCode.xlsx
+++ b/LeetCode.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\EricS\Documents\VSCode Projects\LeetcodeGrind\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2A394582-75A4-4E12-9D93-EF77742322EA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0805DA11-A46B-43DC-8CD1-A8F70DCB9649}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="3" xr2:uid="{02D29AA1-7085-42F6-B3D4-4C0365DA5453}"/>
   </bookViews>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="804" uniqueCount="575">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="806" uniqueCount="577">
   <si>
     <t>Roman to Integer:</t>
   </si>
@@ -1769,6 +1769,12 @@
   </si>
   <si>
     <t>Combine start and end and sort, tracking the current number of ongoing meetings and updating ret as needed going through them chronologically</t>
+  </si>
+  <si>
+    <t>Given bunch of intervals and list of queries, return list of sizes for the smallest size of an interval each query value is in, -1 for no intervals</t>
+  </si>
+  <si>
+    <t>Sort query and intervals by left bound, keeping track of query original index. Then, loop through query, adding each interval that is valid for that query into a min heap by (size, end) tuple. After adding all valid intervals for that query and incrementing j interval pointer with it, keep checking/popping min heap until end is valid for current query, taking the value and putting it into ret.</t>
   </si>
 </sst>
 </file>
@@ -2933,7 +2939,7 @@
   <dimension ref="A1:G968"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A130" zoomScale="81" zoomScaleNormal="122" workbookViewId="0">
-      <selection activeCell="D138" sqref="D138"/>
+      <selection activeCell="E139" sqref="E139"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5207,15 +5213,19 @@
       </c>
       <c r="F137" s="3"/>
     </row>
-    <row r="138" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="138" spans="1:6" ht="60" x14ac:dyDescent="0.25">
       <c r="B138" s="4" t="s">
         <v>476</v>
       </c>
       <c r="C138" s="4" t="s">
         <v>142</v>
       </c>
-      <c r="D138" s="3"/>
-      <c r="E138" s="3"/>
+      <c r="D138" s="3" t="s">
+        <v>575</v>
+      </c>
+      <c r="E138" s="3" t="s">
+        <v>576</v>
+      </c>
       <c r="F138" s="3"/>
     </row>
     <row r="139" spans="1:6" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Finished happy num, plus one, pow x n
</commit_message>
<xml_diff>
--- a/LeetCode.xlsx
+++ b/LeetCode.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\EricS\Documents\VSCode Projects\LeetcodeGrind\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0805DA11-A46B-43DC-8CD1-A8F70DCB9649}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A8E5C280-0C09-42C4-BBFA-B0EEC1C63A2D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="3" xr2:uid="{02D29AA1-7085-42F6-B3D4-4C0365DA5453}"/>
   </bookViews>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="806" uniqueCount="577">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="849" uniqueCount="599">
   <si>
     <t>Roman to Integer:</t>
   </si>
@@ -1775,13 +1775,79 @@
   </si>
   <si>
     <t>Sort query and intervals by left bound, keeping track of query original index. Then, loop through query, adding each interval that is valid for that query into a min heap by (size, end) tuple. After adding all valid intervals for that query and incrementing j interval pointer with it, keep checking/popping min heap until end is valid for current query, taking the value and putting it into ret.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Rotate Image   </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Spiral Matrix   </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Set Matrix Zeroes   </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Happy Number   </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Plus One   </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Pow(x, n)   </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Multiply Strings   </t>
+  </si>
+  <si>
+    <t>Detect Squares</t>
+  </si>
+  <si>
+    <t>Math/Geometry</t>
+  </si>
+  <si>
+    <t>Bit Manipulation</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Single Number   </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Number of 1 Bits   </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Counting Bits   </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Reverse Bits   </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Missing Number   </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Sum of Two Integers   </t>
+  </si>
+  <si>
+    <t>Reverse Integer</t>
+  </si>
+  <si>
+    <t>Separate function for math function and using Floyd fast and slow algorithm to look for loops, true if fast is equal to 1 at end</t>
+  </si>
+  <si>
+    <t>Add 1 to multi-digit number represented using array</t>
+  </si>
+  <si>
+    <t>Loop from back, if not 9, add 1 and return. Otherwise set to 0 and loop continues on, insert 1 at the start at the end</t>
+  </si>
+  <si>
+    <t>Manually calculate raising x to power of n</t>
+  </si>
+  <si>
+    <t>Recursively call pow(x,  n / 2) * pow(x, n / 2) * pow(x, n % 2), do base cases for 0, 1, and -1 powers.</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="12" x14ac:knownFonts="1">
+  <fonts count="13" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1873,6 +1939,13 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -1895,7 +1968,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="30">
+  <cellXfs count="32">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -1977,6 +2050,12 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -2386,8 +2465,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9DDE336F-4AFE-4B2A-A1AE-548ED7725D47}">
   <dimension ref="A1:E38"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D7" sqref="D7"/>
+    <sheetView topLeftCell="A18" workbookViewId="0">
+      <selection activeCell="D27" activeCellId="1" sqref="B27 D27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2938,8 +3017,8 @@
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:G968"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A130" zoomScale="81" zoomScaleNormal="122" workbookViewId="0">
-      <selection activeCell="E139" sqref="E139"/>
+    <sheetView tabSelected="1" topLeftCell="A135" zoomScale="81" zoomScaleNormal="122" workbookViewId="0">
+      <selection activeCell="E145" sqref="E145"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5228,112 +5307,230 @@
       </c>
       <c r="F138" s="3"/>
     </row>
-    <row r="139" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="D139" s="3"/>
-      <c r="E139" s="3"/>
-      <c r="F139" s="3"/>
-    </row>
-    <row r="140" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="D140" s="3"/>
-      <c r="E140" s="3"/>
-      <c r="F140" s="3"/>
+    <row r="139" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A139" s="16" t="s">
+        <v>585</v>
+      </c>
+      <c r="B139" s="4" t="s">
+        <v>577</v>
+      </c>
+      <c r="C139" s="4" t="s">
+        <v>119</v>
+      </c>
+      <c r="D139" s="17" t="s">
+        <v>501</v>
+      </c>
+      <c r="E139" s="17" t="s">
+        <v>502</v>
+      </c>
+      <c r="F139" s="17" t="s">
+        <v>500</v>
+      </c>
+    </row>
+    <row r="140" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="B140" s="4" t="s">
+        <v>578</v>
+      </c>
+      <c r="C140" s="4" t="s">
+        <v>119</v>
+      </c>
+      <c r="D140" s="17" t="s">
+        <v>496</v>
+      </c>
+      <c r="E140" s="17" t="s">
+        <v>497</v>
+      </c>
+      <c r="F140" s="17"/>
     </row>
     <row r="141" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B141" s="4" t="s">
+        <v>579</v>
+      </c>
+      <c r="C141" s="4" t="s">
+        <v>119</v>
+      </c>
       <c r="D141" s="3"/>
       <c r="E141" s="3"/>
       <c r="F141" s="3"/>
     </row>
-    <row r="142" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="D142" s="3"/>
-      <c r="E142" s="3"/>
-      <c r="F142" s="3"/>
+    <row r="142" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="B142" s="4" t="s">
+        <v>580</v>
+      </c>
+      <c r="C142" s="4" t="s">
+        <v>112</v>
+      </c>
+      <c r="D142" s="30" t="s">
+        <v>91</v>
+      </c>
+      <c r="E142" s="31" t="s">
+        <v>594</v>
+      </c>
+      <c r="F142" s="30"/>
     </row>
     <row r="143" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="D143" s="3"/>
-      <c r="E143" s="3"/>
+      <c r="B143" s="4" t="s">
+        <v>581</v>
+      </c>
+      <c r="C143" s="4" t="s">
+        <v>112</v>
+      </c>
+      <c r="D143" s="5" t="s">
+        <v>595</v>
+      </c>
+      <c r="E143" s="3" t="s">
+        <v>596</v>
+      </c>
       <c r="F143" s="3"/>
     </row>
     <row r="144" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="D144" s="3"/>
-      <c r="E144" s="3"/>
+      <c r="B144" s="4" t="s">
+        <v>582</v>
+      </c>
+      <c r="C144" s="4" t="s">
+        <v>119</v>
+      </c>
+      <c r="D144" s="3" t="s">
+        <v>597</v>
+      </c>
+      <c r="E144" s="3" t="s">
+        <v>598</v>
+      </c>
       <c r="F144" s="3"/>
     </row>
-    <row r="145" spans="4:6" x14ac:dyDescent="0.25">
+    <row r="145" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B145" s="4" t="s">
+        <v>583</v>
+      </c>
+      <c r="C145" s="4" t="s">
+        <v>119</v>
+      </c>
       <c r="D145" s="3"/>
       <c r="E145" s="3"/>
       <c r="F145" s="3"/>
     </row>
-    <row r="146" spans="4:6" x14ac:dyDescent="0.25">
+    <row r="146" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B146" s="4" t="s">
+        <v>584</v>
+      </c>
+      <c r="C146" s="4" t="s">
+        <v>119</v>
+      </c>
       <c r="D146" s="3"/>
       <c r="E146" s="3"/>
       <c r="F146" s="3"/>
     </row>
-    <row r="147" spans="4:6" x14ac:dyDescent="0.25">
+    <row r="147" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A147" s="16" t="s">
+        <v>586</v>
+      </c>
+      <c r="B147" s="4" t="s">
+        <v>587</v>
+      </c>
+      <c r="C147" s="4" t="s">
+        <v>112</v>
+      </c>
       <c r="D147" s="3"/>
       <c r="E147" s="3"/>
       <c r="F147" s="3"/>
     </row>
-    <row r="148" spans="4:6" x14ac:dyDescent="0.25">
+    <row r="148" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B148" s="4" t="s">
+        <v>588</v>
+      </c>
+      <c r="C148" s="4" t="s">
+        <v>112</v>
+      </c>
       <c r="D148" s="3"/>
       <c r="E148" s="3"/>
       <c r="F148" s="3"/>
     </row>
-    <row r="149" spans="4:6" x14ac:dyDescent="0.25">
+    <row r="149" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B149" s="4" t="s">
+        <v>589</v>
+      </c>
+      <c r="C149" s="4" t="s">
+        <v>112</v>
+      </c>
       <c r="D149" s="3"/>
       <c r="E149" s="3"/>
       <c r="F149" s="3"/>
     </row>
-    <row r="150" spans="4:6" x14ac:dyDescent="0.25">
+    <row r="150" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B150" s="4" t="s">
+        <v>590</v>
+      </c>
+      <c r="C150" s="4" t="s">
+        <v>112</v>
+      </c>
       <c r="D150" s="3"/>
       <c r="E150" s="3"/>
       <c r="F150" s="3"/>
     </row>
-    <row r="151" spans="4:6" x14ac:dyDescent="0.25">
+    <row r="151" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B151" s="4" t="s">
+        <v>591</v>
+      </c>
+      <c r="C151" s="4" t="s">
+        <v>112</v>
+      </c>
       <c r="D151" s="3"/>
       <c r="E151" s="3"/>
       <c r="F151" s="3"/>
     </row>
-    <row r="152" spans="4:6" x14ac:dyDescent="0.25">
+    <row r="152" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B152" s="4" t="s">
+        <v>592</v>
+      </c>
+      <c r="C152" s="4" t="s">
+        <v>119</v>
+      </c>
       <c r="D152" s="3"/>
       <c r="E152" s="3"/>
       <c r="F152" s="3"/>
     </row>
-    <row r="153" spans="4:6" x14ac:dyDescent="0.25">
+    <row r="153" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B153" s="4" t="s">
+        <v>593</v>
+      </c>
+      <c r="C153" s="4" t="s">
+        <v>119</v>
+      </c>
       <c r="D153" s="3"/>
       <c r="E153" s="3"/>
       <c r="F153" s="3"/>
     </row>
-    <row r="154" spans="4:6" x14ac:dyDescent="0.25">
+    <row r="154" spans="1:6" x14ac:dyDescent="0.25">
       <c r="D154" s="3"/>
       <c r="E154" s="3"/>
       <c r="F154" s="3"/>
     </row>
-    <row r="155" spans="4:6" x14ac:dyDescent="0.25">
+    <row r="155" spans="1:6" x14ac:dyDescent="0.25">
       <c r="D155" s="3"/>
       <c r="E155" s="3"/>
       <c r="F155" s="3"/>
     </row>
-    <row r="156" spans="4:6" x14ac:dyDescent="0.25">
+    <row r="156" spans="1:6" x14ac:dyDescent="0.25">
       <c r="D156" s="3"/>
       <c r="E156" s="3"/>
       <c r="F156" s="3"/>
     </row>
-    <row r="157" spans="4:6" x14ac:dyDescent="0.25">
+    <row r="157" spans="1:6" x14ac:dyDescent="0.25">
       <c r="D157" s="3"/>
       <c r="E157" s="3"/>
       <c r="F157" s="3"/>
     </row>
-    <row r="158" spans="4:6" x14ac:dyDescent="0.25">
+    <row r="158" spans="1:6" x14ac:dyDescent="0.25">
       <c r="D158" s="3"/>
       <c r="E158" s="3"/>
       <c r="F158" s="3"/>
     </row>
-    <row r="159" spans="4:6" x14ac:dyDescent="0.25">
+    <row r="159" spans="1:6" x14ac:dyDescent="0.25">
       <c r="D159" s="3"/>
       <c r="E159" s="3"/>
       <c r="F159" s="3"/>
     </row>
-    <row r="160" spans="4:6" x14ac:dyDescent="0.25">
+    <row r="160" spans="1:6" x14ac:dyDescent="0.25">
       <c r="D160" s="3"/>
       <c r="E160" s="3"/>
       <c r="F160" s="3"/>
@@ -9406,8 +9603,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6933FBFC-44BD-4904-99DA-B0AF53F41F06}">
   <dimension ref="A1:G18"/>
   <sheetViews>
-    <sheetView topLeftCell="A15" workbookViewId="0">
-      <selection activeCell="E18" sqref="E18"/>
+    <sheetView zoomScale="83" workbookViewId="0">
+      <selection activeCell="D3" sqref="D3:F3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Finished detect squares and math/geom
</commit_message>
<xml_diff>
--- a/LeetCode.xlsx
+++ b/LeetCode.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\EricS\Documents\VSCode Projects\LeetcodeGrind\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E5F1514E-3307-48EA-ADFA-0B4A8CC158ED}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E03C0DCB-EFD9-46C5-80C7-D49662C4B621}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="3" xr2:uid="{02D29AA1-7085-42F6-B3D4-4C0365DA5453}"/>
   </bookViews>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="853" uniqueCount="603">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="855" uniqueCount="605">
   <si>
     <t>Roman to Integer:</t>
   </si>
@@ -1853,6 +1853,12 @@
   </si>
   <si>
     <t>Basically just do digit by digit multiplication using subtraction to get each digit value, combining it using vector, and then converting it back into a string by adding '0'</t>
+  </si>
+  <si>
+    <t>Create class that can add points, and query with a point where you return number of squares you can create using that point, allows for repeated points</t>
+  </si>
+  <si>
+    <t>Nested hashmap first by row, then by column, then you get count of point at (row, col). Add just increments track[row][col]++, query loops through all points in the row (skipping if same column), and checks above and below the distance from query to current point in row, if there is square, it multiples the multiplicities of each of the points in the square and adds to ret</t>
   </si>
 </sst>
 </file>
@@ -3030,7 +3036,7 @@
   <dimension ref="A1:G968"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A135" zoomScale="81" zoomScaleNormal="122" workbookViewId="0">
-      <selection activeCell="D146" sqref="D146"/>
+      <selection activeCell="E147" sqref="E147"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5429,15 +5435,19 @@
       </c>
       <c r="F145" s="3"/>
     </row>
-    <row r="146" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="146" spans="1:6" ht="60" x14ac:dyDescent="0.25">
       <c r="B146" s="4" t="s">
         <v>584</v>
       </c>
       <c r="C146" s="4" t="s">
         <v>119</v>
       </c>
-      <c r="D146" s="3"/>
-      <c r="E146" s="3"/>
+      <c r="D146" s="3" t="s">
+        <v>603</v>
+      </c>
+      <c r="E146" s="3" t="s">
+        <v>604</v>
+      </c>
       <c r="F146" s="3"/>
     </row>
     <row r="147" spans="1:6" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Finished all easy bit manipulation qs
</commit_message>
<xml_diff>
--- a/LeetCode.xlsx
+++ b/LeetCode.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\EricS\Documents\VSCode Projects\LeetcodeGrind\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E03C0DCB-EFD9-46C5-80C7-D49662C4B621}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DFB728A7-5B37-4A51-BE3B-6AA0615CAB94}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="3" xr2:uid="{02D29AA1-7085-42F6-B3D4-4C0365DA5453}"/>
   </bookViews>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="855" uniqueCount="605">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="867" uniqueCount="616">
   <si>
     <t>Roman to Integer:</t>
   </si>
@@ -1859,6 +1859,39 @@
   </si>
   <si>
     <t>Nested hashmap first by row, then by column, then you get count of point at (row, col). Add just increments track[row][col]++, query loops through all points in the row (skipping if same column), and checks above and below the distance from query to current point in row, if there is square, it multiples the multiplicities of each of the points in the square and adds to ret</t>
+  </si>
+  <si>
+    <t>Given array of numbers where each number appears twice except 1, return that 1</t>
+  </si>
+  <si>
+    <t>Xor through everything, aggregation starts with 0, return</t>
+  </si>
+  <si>
+    <t>Count 1 bits in int</t>
+  </si>
+  <si>
+    <t>Ret += n &amp; 1, n shift right 1, loop while n is not 0</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Return vector of  number of 1 bits for all numbers 0 - n </t>
+  </si>
+  <si>
+    <t>If curr &amp; 1, then we have ret[curr - 1] + 1 since before there had to be 0 there. Otherwise, we get ret[curr &gt;&gt; 1] since the last slot is zero so it's equal to previous number of all bits except lsb</t>
+  </si>
+  <si>
+    <t>Easiest way is to create ret = 0, keep shifting n right and using &amp; 1 to extract lsb, shift result left each time u add a new one</t>
+  </si>
+  <si>
+    <t>Can also do swaps, looping 0 - 16 and comparing bits and swapping</t>
+  </si>
+  <si>
+    <t>Given vector, find missing number from 0 - n</t>
+  </si>
+  <si>
+    <t>Can also do n(n-1)/2 and subtract each element in vector to find missing</t>
+  </si>
+  <si>
+    <t>xor through every number from 0 to n and xor through every element in the vector to end up with the missing number, basically manually creating the single number problem</t>
   </si>
 </sst>
 </file>
@@ -3035,8 +3068,8 @@
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:G968"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A135" zoomScale="81" zoomScaleNormal="122" workbookViewId="0">
-      <selection activeCell="E147" sqref="E147"/>
+    <sheetView tabSelected="1" topLeftCell="A139" zoomScale="81" zoomScaleNormal="122" workbookViewId="0">
+      <selection activeCell="D152" sqref="D152"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5450,7 +5483,7 @@
       </c>
       <c r="F146" s="3"/>
     </row>
-    <row r="147" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="147" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A147" s="16" t="s">
         <v>586</v>
       </c>
@@ -5460,8 +5493,12 @@
       <c r="C147" s="4" t="s">
         <v>112</v>
       </c>
-      <c r="D147" s="3"/>
-      <c r="E147" s="3"/>
+      <c r="D147" s="3" t="s">
+        <v>605</v>
+      </c>
+      <c r="E147" s="3" t="s">
+        <v>606</v>
+      </c>
       <c r="F147" s="3"/>
     </row>
     <row r="148" spans="1:6" x14ac:dyDescent="0.25">
@@ -5471,42 +5508,62 @@
       <c r="C148" s="4" t="s">
         <v>112</v>
       </c>
-      <c r="D148" s="3"/>
-      <c r="E148" s="3"/>
+      <c r="D148" s="3" t="s">
+        <v>607</v>
+      </c>
+      <c r="E148" s="3" t="s">
+        <v>608</v>
+      </c>
       <c r="F148" s="3"/>
     </row>
-    <row r="149" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="149" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="B149" s="4" t="s">
         <v>589</v>
       </c>
       <c r="C149" s="4" t="s">
         <v>112</v>
       </c>
-      <c r="D149" s="3"/>
-      <c r="E149" s="3"/>
+      <c r="D149" s="3" t="s">
+        <v>609</v>
+      </c>
+      <c r="E149" s="3" t="s">
+        <v>610</v>
+      </c>
       <c r="F149" s="3"/>
     </row>
-    <row r="150" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="150" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="B150" s="4" t="s">
         <v>590</v>
       </c>
       <c r="C150" s="4" t="s">
         <v>112</v>
       </c>
-      <c r="D150" s="3"/>
-      <c r="E150" s="3"/>
-      <c r="F150" s="3"/>
-    </row>
-    <row r="151" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="D150" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="E150" s="3" t="s">
+        <v>611</v>
+      </c>
+      <c r="F150" s="3" t="s">
+        <v>612</v>
+      </c>
+    </row>
+    <row r="151" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="B151" s="4" t="s">
         <v>591</v>
       </c>
       <c r="C151" s="4" t="s">
         <v>112</v>
       </c>
-      <c r="D151" s="3"/>
-      <c r="E151" s="3"/>
-      <c r="F151" s="3"/>
+      <c r="D151" s="3" t="s">
+        <v>613</v>
+      </c>
+      <c r="E151" s="3" t="s">
+        <v>615</v>
+      </c>
+      <c r="F151" s="3" t="s">
+        <v>614</v>
+      </c>
     </row>
     <row r="152" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B152" s="4" t="s">

</xml_diff>

<commit_message>
Done with neetcode !!!
</commit_message>
<xml_diff>
--- a/LeetCode.xlsx
+++ b/LeetCode.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\EricS\Documents\VSCode Projects\LeetcodeGrind\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DFB728A7-5B37-4A51-BE3B-6AA0615CAB94}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8FF9AC5A-0619-4BD5-8AEB-E04020BFCFD0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="3" xr2:uid="{02D29AA1-7085-42F6-B3D4-4C0365DA5453}"/>
   </bookViews>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="867" uniqueCount="616">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="871" uniqueCount="618">
   <si>
     <t>Roman to Integer:</t>
   </si>
@@ -1892,6 +1892,12 @@
   </si>
   <si>
     <t>xor through every number from 0 to n and xor through every element in the vector to end up with the missing number, basically manually creating the single number problem</t>
+  </si>
+  <si>
+    <t>First you have a ^= b to get sum for everything except carries, then you have carry = a &amp; b which has all the possible carry bits, which you then have to shift by 1. Set b = carry &lt;&lt; 1. Loop while b is non-zero, continuing to calculate carry and a ^= b and b = carry &lt;&lt; 1.</t>
+  </si>
+  <si>
+    <t>Same thing as reverse bits except with /= 10 and + % 10 instead. Have to do a check every loop for if ret is larger than INT_MAX / 10 or less than INT_MIN / 10 in which case we return 0 (check done before the adding)</t>
   </si>
 </sst>
 </file>
@@ -3069,7 +3075,7 @@
   <dimension ref="A1:G968"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A139" zoomScale="81" zoomScaleNormal="122" workbookViewId="0">
-      <selection activeCell="D152" sqref="D152"/>
+      <selection activeCell="E154" sqref="E154"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5565,26 +5571,34 @@
         <v>614</v>
       </c>
     </row>
-    <row r="152" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="152" spans="1:6" ht="45" x14ac:dyDescent="0.25">
       <c r="B152" s="4" t="s">
         <v>592</v>
       </c>
       <c r="C152" s="4" t="s">
         <v>119</v>
       </c>
-      <c r="D152" s="3"/>
-      <c r="E152" s="3"/>
+      <c r="D152" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="E152" s="3" t="s">
+        <v>616</v>
+      </c>
       <c r="F152" s="3"/>
     </row>
-    <row r="153" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="153" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="B153" s="4" t="s">
         <v>593</v>
       </c>
       <c r="C153" s="4" t="s">
         <v>119</v>
       </c>
-      <c r="D153" s="3"/>
-      <c r="E153" s="3"/>
+      <c r="D153" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="E153" s="3" t="s">
+        <v>617</v>
+      </c>
       <c r="F153" s="3"/>
     </row>
     <row r="154" spans="1:6" x14ac:dyDescent="0.25">

</xml_diff>